<commit_message>
Horas Extra Sem 26
</commit_message>
<xml_diff>
--- a/datasets/horas_extras_2024.xlsx
+++ b/datasets/horas_extras_2024.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41E01BA1-453E-4A69-9522-5D786D3D9D22}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3A704EF-41BC-41C4-B628-6FA3EC10749B}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5830" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6085" uniqueCount="418">
   <si>
     <t>José Guadalupe de Jesús Venegas Acosta</t>
   </si>
@@ -1288,6 +1288,9 @@
   <si>
     <t>costo</t>
   </si>
+  <si>
+    <t xml:space="preserve"> $                                   -  </t>
+  </si>
 </sst>
 </file>
 
@@ -1360,8 +1363,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G2360" totalsRowShown="0">
-  <autoFilter ref="A1:G2360" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G2452" totalsRowShown="0">
+  <autoFilter ref="A1:G2452" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{933A802B-1DFA-4F50-A708-F8B071DB7BC5}" name="no"/>
     <tableColumn id="2" xr3:uid="{6D6E4B13-9BB4-4B8D-9AB2-9B4BC34C4362}" name="id"/>
@@ -1692,15 +1695,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C5034C-9333-43F5-A544-30F944CBFAC1}">
-  <dimension ref="A1:G2360"/>
+  <dimension ref="A1:G2452"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2340" workbookViewId="0">
-      <selection activeCell="F2327" sqref="F2327"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2413" workbookViewId="0">
+      <selection activeCell="H2449" sqref="H2449"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="6" max="7" width="10.6640625" style="1"/>
+    <col min="6" max="6" width="10.6640625" style="1"/>
+    <col min="7" max="7" width="16.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.45">
@@ -55465,6 +55469,2122 @@
       </c>
       <c r="G2360" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2361">
+        <v>1</v>
+      </c>
+      <c r="B2361">
+        <v>101</v>
+      </c>
+      <c r="C2361" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2361">
+        <v>26</v>
+      </c>
+      <c r="E2361" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2361" s="1">
+        <v>12</v>
+      </c>
+      <c r="G2361" s="1">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2362">
+        <v>2</v>
+      </c>
+      <c r="B2362">
+        <v>103</v>
+      </c>
+      <c r="C2362" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2362">
+        <v>26</v>
+      </c>
+      <c r="E2362" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2362" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2362" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2363">
+        <v>3</v>
+      </c>
+      <c r="B2363">
+        <v>104</v>
+      </c>
+      <c r="C2363" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2363">
+        <v>26</v>
+      </c>
+      <c r="E2363" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2363" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2363" s="1">
+        <v>647.29999999999995</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2364">
+        <v>4</v>
+      </c>
+      <c r="B2364">
+        <v>106</v>
+      </c>
+      <c r="C2364" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2364">
+        <v>26</v>
+      </c>
+      <c r="E2364" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2364" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2364" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2365">
+        <v>5</v>
+      </c>
+      <c r="B2365">
+        <v>107</v>
+      </c>
+      <c r="C2365" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2365">
+        <v>26</v>
+      </c>
+      <c r="E2365" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2365" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2365" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2366">
+        <v>6</v>
+      </c>
+      <c r="B2366">
+        <v>108</v>
+      </c>
+      <c r="C2366" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2366">
+        <v>26</v>
+      </c>
+      <c r="E2366" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2366" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2366" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2367">
+        <v>7</v>
+      </c>
+      <c r="B2367">
+        <v>109</v>
+      </c>
+      <c r="C2367" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2367">
+        <v>26</v>
+      </c>
+      <c r="E2367" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2367" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2367" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2368">
+        <v>8</v>
+      </c>
+      <c r="B2368">
+        <v>110</v>
+      </c>
+      <c r="C2368" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2368">
+        <v>26</v>
+      </c>
+      <c r="E2368" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2368" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2368" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2369">
+        <v>9</v>
+      </c>
+      <c r="B2369">
+        <v>111</v>
+      </c>
+      <c r="C2369" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2369">
+        <v>26</v>
+      </c>
+      <c r="E2369" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2369" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2369" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2370">
+        <v>10</v>
+      </c>
+      <c r="B2370">
+        <v>113</v>
+      </c>
+      <c r="C2370" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2370">
+        <v>26</v>
+      </c>
+      <c r="E2370" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2370" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2370" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2371">
+        <v>11</v>
+      </c>
+      <c r="B2371">
+        <v>114</v>
+      </c>
+      <c r="C2371" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2371">
+        <v>26</v>
+      </c>
+      <c r="E2371" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2371" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2371" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2372">
+        <v>12</v>
+      </c>
+      <c r="B2372">
+        <v>117</v>
+      </c>
+      <c r="C2372" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2372">
+        <v>26</v>
+      </c>
+      <c r="E2372" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2372" s="1">
+        <v>9</v>
+      </c>
+      <c r="G2372" s="1">
+        <v>763.38</v>
+      </c>
+    </row>
+    <row r="2373" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2373">
+        <v>13</v>
+      </c>
+      <c r="B2373">
+        <v>119</v>
+      </c>
+      <c r="C2373" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2373">
+        <v>26</v>
+      </c>
+      <c r="E2373" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2373" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2373" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2374">
+        <v>14</v>
+      </c>
+      <c r="B2374">
+        <v>125</v>
+      </c>
+      <c r="C2374" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2374">
+        <v>26</v>
+      </c>
+      <c r="E2374" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2374" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2374" s="1">
+        <v>75.89</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2375">
+        <v>15</v>
+      </c>
+      <c r="B2375">
+        <v>126</v>
+      </c>
+      <c r="C2375" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2375">
+        <v>26</v>
+      </c>
+      <c r="E2375" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2375" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2375" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2376">
+        <v>16</v>
+      </c>
+      <c r="B2376">
+        <v>129</v>
+      </c>
+      <c r="C2376" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2376">
+        <v>26</v>
+      </c>
+      <c r="E2376" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2376" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2376" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2377">
+        <v>17</v>
+      </c>
+      <c r="B2377">
+        <v>131</v>
+      </c>
+      <c r="C2377" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2377">
+        <v>26</v>
+      </c>
+      <c r="E2377" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2377" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2377" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2378">
+        <v>18</v>
+      </c>
+      <c r="B2378">
+        <v>133</v>
+      </c>
+      <c r="C2378" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2378">
+        <v>26</v>
+      </c>
+      <c r="E2378" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2378" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2378" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2379">
+        <v>19</v>
+      </c>
+      <c r="B2379">
+        <v>134</v>
+      </c>
+      <c r="C2379" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2379">
+        <v>26</v>
+      </c>
+      <c r="E2379" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2379" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2379" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2380">
+        <v>20</v>
+      </c>
+      <c r="B2380">
+        <v>136</v>
+      </c>
+      <c r="C2380" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2380">
+        <v>26</v>
+      </c>
+      <c r="E2380" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2380" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2380" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2381">
+        <v>21</v>
+      </c>
+      <c r="B2381">
+        <v>141</v>
+      </c>
+      <c r="C2381" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2381">
+        <v>26</v>
+      </c>
+      <c r="E2381" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2381" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2381" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2382">
+        <v>22</v>
+      </c>
+      <c r="B2382">
+        <v>145</v>
+      </c>
+      <c r="C2382" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2382">
+        <v>26</v>
+      </c>
+      <c r="E2382" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2382" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2382" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2383">
+        <v>23</v>
+      </c>
+      <c r="B2383">
+        <v>147</v>
+      </c>
+      <c r="C2383" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2383">
+        <v>26</v>
+      </c>
+      <c r="E2383" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2383" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2383" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2384">
+        <v>24</v>
+      </c>
+      <c r="B2384">
+        <v>149</v>
+      </c>
+      <c r="C2384" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2384">
+        <v>26</v>
+      </c>
+      <c r="E2384" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2384" s="1">
+        <v>6</v>
+      </c>
+      <c r="G2384" s="1">
+        <v>857.16</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2385">
+        <v>25</v>
+      </c>
+      <c r="B2385">
+        <v>150</v>
+      </c>
+      <c r="C2385" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2385">
+        <v>26</v>
+      </c>
+      <c r="E2385" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2385" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2385" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2386">
+        <v>26</v>
+      </c>
+      <c r="B2386">
+        <v>151</v>
+      </c>
+      <c r="C2386" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2386">
+        <v>26</v>
+      </c>
+      <c r="E2386" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2386" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2386" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2387">
+        <v>27</v>
+      </c>
+      <c r="B2387">
+        <v>154</v>
+      </c>
+      <c r="C2387" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2387">
+        <v>26</v>
+      </c>
+      <c r="E2387" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2387" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2387" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2388">
+        <v>28</v>
+      </c>
+      <c r="B2388">
+        <v>160</v>
+      </c>
+      <c r="C2388" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2388">
+        <v>26</v>
+      </c>
+      <c r="E2388" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2388" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2388" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2389">
+        <v>29</v>
+      </c>
+      <c r="B2389">
+        <v>162</v>
+      </c>
+      <c r="C2389" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2389">
+        <v>26</v>
+      </c>
+      <c r="E2389" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2389" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2389" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2390">
+        <v>30</v>
+      </c>
+      <c r="B2390">
+        <v>164</v>
+      </c>
+      <c r="C2390" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2390">
+        <v>26</v>
+      </c>
+      <c r="E2390" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2390" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2390" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2391">
+        <v>31</v>
+      </c>
+      <c r="B2391">
+        <v>165</v>
+      </c>
+      <c r="C2391" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2391">
+        <v>26</v>
+      </c>
+      <c r="E2391" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2391" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2391" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2392">
+        <v>32</v>
+      </c>
+      <c r="B2392">
+        <v>167</v>
+      </c>
+      <c r="C2392" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2392">
+        <v>26</v>
+      </c>
+      <c r="E2392" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2392" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2392" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2393" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2393">
+        <v>33</v>
+      </c>
+      <c r="B2393">
+        <v>175</v>
+      </c>
+      <c r="C2393" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2393">
+        <v>26</v>
+      </c>
+      <c r="E2393" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2393" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2393" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2394">
+        <v>34</v>
+      </c>
+      <c r="B2394">
+        <v>181</v>
+      </c>
+      <c r="C2394" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2394">
+        <v>26</v>
+      </c>
+      <c r="E2394" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2394" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2394" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2395">
+        <v>35</v>
+      </c>
+      <c r="B2395">
+        <v>182</v>
+      </c>
+      <c r="C2395" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2395">
+        <v>26</v>
+      </c>
+      <c r="E2395" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2395" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2395" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2396">
+        <v>36</v>
+      </c>
+      <c r="B2396">
+        <v>184</v>
+      </c>
+      <c r="C2396" t="s">
+        <v>368</v>
+      </c>
+      <c r="D2396">
+        <v>26</v>
+      </c>
+      <c r="E2396" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2396" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2396" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2397">
+        <v>37</v>
+      </c>
+      <c r="B2397">
+        <v>186</v>
+      </c>
+      <c r="C2397" t="s">
+        <v>369</v>
+      </c>
+      <c r="D2397">
+        <v>26</v>
+      </c>
+      <c r="E2397" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2397" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2397" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2398">
+        <v>38</v>
+      </c>
+      <c r="B2398">
+        <v>190</v>
+      </c>
+      <c r="C2398" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2398">
+        <v>26</v>
+      </c>
+      <c r="E2398" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2398" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2398" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2399">
+        <v>39</v>
+      </c>
+      <c r="B2399">
+        <v>194</v>
+      </c>
+      <c r="C2399" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2399">
+        <v>26</v>
+      </c>
+      <c r="E2399" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2399" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2399" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2400">
+        <v>40</v>
+      </c>
+      <c r="B2400">
+        <v>199</v>
+      </c>
+      <c r="C2400" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2400">
+        <v>26</v>
+      </c>
+      <c r="E2400" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2400" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2400" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2401">
+        <v>41</v>
+      </c>
+      <c r="B2401">
+        <v>200</v>
+      </c>
+      <c r="C2401" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2401">
+        <v>26</v>
+      </c>
+      <c r="E2401" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2401" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2401" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2402">
+        <v>42</v>
+      </c>
+      <c r="B2402">
+        <v>203</v>
+      </c>
+      <c r="C2402" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2402">
+        <v>26</v>
+      </c>
+      <c r="E2402" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2402" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2402" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2403">
+        <v>43</v>
+      </c>
+      <c r="B2403">
+        <v>205</v>
+      </c>
+      <c r="C2403" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2403">
+        <v>26</v>
+      </c>
+      <c r="E2403" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2403" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G2403" s="1">
+        <v>61.16</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2404">
+        <v>44</v>
+      </c>
+      <c r="B2404">
+        <v>208</v>
+      </c>
+      <c r="C2404" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2404">
+        <v>26</v>
+      </c>
+      <c r="E2404" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2404" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2404" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2405">
+        <v>45</v>
+      </c>
+      <c r="B2405">
+        <v>209</v>
+      </c>
+      <c r="C2405" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2405">
+        <v>26</v>
+      </c>
+      <c r="E2405" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2405" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G2405" s="1">
+        <v>103.13</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2406">
+        <v>46</v>
+      </c>
+      <c r="B2406">
+        <v>212</v>
+      </c>
+      <c r="C2406" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2406">
+        <v>26</v>
+      </c>
+      <c r="E2406" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2406" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2406" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2407">
+        <v>47</v>
+      </c>
+      <c r="B2407">
+        <v>214</v>
+      </c>
+      <c r="C2407" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2407">
+        <v>26</v>
+      </c>
+      <c r="E2407" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2407" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2407" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2408">
+        <v>48</v>
+      </c>
+      <c r="B2408">
+        <v>215</v>
+      </c>
+      <c r="C2408" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2408">
+        <v>26</v>
+      </c>
+      <c r="E2408" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2408" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G2408" s="1">
+        <v>378.13</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2409">
+        <v>49</v>
+      </c>
+      <c r="B2409">
+        <v>217</v>
+      </c>
+      <c r="C2409" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2409">
+        <v>26</v>
+      </c>
+      <c r="E2409" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2409" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2409" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2410">
+        <v>50</v>
+      </c>
+      <c r="B2410">
+        <v>219</v>
+      </c>
+      <c r="C2410" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2410">
+        <v>26</v>
+      </c>
+      <c r="E2410" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2410" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2410" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2411">
+        <v>51</v>
+      </c>
+      <c r="B2411">
+        <v>222</v>
+      </c>
+      <c r="C2411" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2411">
+        <v>26</v>
+      </c>
+      <c r="E2411" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2411" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2411" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2412">
+        <v>52</v>
+      </c>
+      <c r="B2412">
+        <v>223</v>
+      </c>
+      <c r="C2412" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2412">
+        <v>26</v>
+      </c>
+      <c r="E2412" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2412" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2412" s="1">
+        <v>343.75</v>
+      </c>
+    </row>
+    <row r="2413" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2413">
+        <v>53</v>
+      </c>
+      <c r="B2413">
+        <v>224</v>
+      </c>
+      <c r="C2413" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2413">
+        <v>26</v>
+      </c>
+      <c r="E2413" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2413" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2413" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2414">
+        <v>54</v>
+      </c>
+      <c r="B2414">
+        <v>228</v>
+      </c>
+      <c r="C2414" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2414">
+        <v>26</v>
+      </c>
+      <c r="E2414" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2414" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2414" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2415">
+        <v>55</v>
+      </c>
+      <c r="B2415">
+        <v>232</v>
+      </c>
+      <c r="C2415" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2415">
+        <v>26</v>
+      </c>
+      <c r="E2415" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2415" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2415" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2416">
+        <v>56</v>
+      </c>
+      <c r="B2416">
+        <v>234</v>
+      </c>
+      <c r="C2416" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2416">
+        <v>26</v>
+      </c>
+      <c r="E2416" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2416" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2416" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2417">
+        <v>57</v>
+      </c>
+      <c r="B2417">
+        <v>235</v>
+      </c>
+      <c r="C2417" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2417">
+        <v>26</v>
+      </c>
+      <c r="E2417" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2417" s="1">
+        <v>7</v>
+      </c>
+      <c r="G2417" s="1">
+        <v>531.23</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2418">
+        <v>58</v>
+      </c>
+      <c r="B2418">
+        <v>237</v>
+      </c>
+      <c r="C2418" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2418">
+        <v>26</v>
+      </c>
+      <c r="E2418" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2418" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2418" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2419">
+        <v>59</v>
+      </c>
+      <c r="B2419">
+        <v>241</v>
+      </c>
+      <c r="C2419" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2419">
+        <v>26</v>
+      </c>
+      <c r="E2419" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2419" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2419" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2420">
+        <v>60</v>
+      </c>
+      <c r="B2420">
+        <v>242</v>
+      </c>
+      <c r="C2420" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2420">
+        <v>26</v>
+      </c>
+      <c r="E2420" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2420" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2420" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2421">
+        <v>61</v>
+      </c>
+      <c r="B2421">
+        <v>243</v>
+      </c>
+      <c r="C2421" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2421">
+        <v>26</v>
+      </c>
+      <c r="E2421" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2421" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2421" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2422">
+        <v>62</v>
+      </c>
+      <c r="B2422">
+        <v>251</v>
+      </c>
+      <c r="C2422" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2422">
+        <v>26</v>
+      </c>
+      <c r="E2422" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2422" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2422" s="1">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2423">
+        <v>63</v>
+      </c>
+      <c r="B2423">
+        <v>255</v>
+      </c>
+      <c r="C2423" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2423">
+        <v>26</v>
+      </c>
+      <c r="E2423" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2423" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2423" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2424">
+        <v>64</v>
+      </c>
+      <c r="B2424">
+        <v>258</v>
+      </c>
+      <c r="C2424" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2424">
+        <v>26</v>
+      </c>
+      <c r="E2424" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2424" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2424" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2425">
+        <v>65</v>
+      </c>
+      <c r="B2425">
+        <v>259</v>
+      </c>
+      <c r="C2425" t="s">
+        <v>348</v>
+      </c>
+      <c r="D2425">
+        <v>26</v>
+      </c>
+      <c r="E2425" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2425" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2425" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2426">
+        <v>66</v>
+      </c>
+      <c r="B2426">
+        <v>260</v>
+      </c>
+      <c r="C2426" t="s">
+        <v>351</v>
+      </c>
+      <c r="D2426">
+        <v>26</v>
+      </c>
+      <c r="E2426" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2426" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2426" s="1">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2427">
+        <v>67</v>
+      </c>
+      <c r="B2427">
+        <v>261</v>
+      </c>
+      <c r="C2427" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2427">
+        <v>26</v>
+      </c>
+      <c r="E2427" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2427" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2427" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2428">
+        <v>68</v>
+      </c>
+      <c r="B2428">
+        <v>263</v>
+      </c>
+      <c r="C2428" t="s">
+        <v>359</v>
+      </c>
+      <c r="D2428">
+        <v>26</v>
+      </c>
+      <c r="E2428" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2428" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2428" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2429">
+        <v>69</v>
+      </c>
+      <c r="B2429">
+        <v>264</v>
+      </c>
+      <c r="C2429" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2429">
+        <v>26</v>
+      </c>
+      <c r="E2429" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2429" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2429" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2430">
+        <v>70</v>
+      </c>
+      <c r="B2430">
+        <v>265</v>
+      </c>
+      <c r="C2430" t="s">
+        <v>409</v>
+      </c>
+      <c r="D2430">
+        <v>26</v>
+      </c>
+      <c r="E2430" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2430" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G2430" s="1">
+        <v>89.28</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2431">
+        <v>71</v>
+      </c>
+      <c r="B2431">
+        <v>269</v>
+      </c>
+      <c r="C2431" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2431">
+        <v>26</v>
+      </c>
+      <c r="E2431" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2431" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2431" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2432">
+        <v>72</v>
+      </c>
+      <c r="B2432">
+        <v>301</v>
+      </c>
+      <c r="C2432" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2432">
+        <v>26</v>
+      </c>
+      <c r="E2432" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2432" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2432" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2433" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2433">
+        <v>73</v>
+      </c>
+      <c r="B2433">
+        <v>302</v>
+      </c>
+      <c r="C2433" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2433">
+        <v>26</v>
+      </c>
+      <c r="E2433" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2433" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2433" s="1">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2434">
+        <v>74</v>
+      </c>
+      <c r="B2434">
+        <v>272</v>
+      </c>
+      <c r="C2434" t="s">
+        <v>395</v>
+      </c>
+      <c r="D2434">
+        <v>26</v>
+      </c>
+      <c r="E2434" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2434" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2434" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2435">
+        <v>75</v>
+      </c>
+      <c r="B2435">
+        <v>273</v>
+      </c>
+      <c r="C2435" t="s">
+        <v>382</v>
+      </c>
+      <c r="D2435">
+        <v>26</v>
+      </c>
+      <c r="E2435" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2435" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2435" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2436">
+        <v>76</v>
+      </c>
+      <c r="B2436">
+        <v>274</v>
+      </c>
+      <c r="C2436" t="s">
+        <v>383</v>
+      </c>
+      <c r="D2436">
+        <v>26</v>
+      </c>
+      <c r="E2436" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2436" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2436" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2437">
+        <v>77</v>
+      </c>
+      <c r="B2437">
+        <v>275</v>
+      </c>
+      <c r="C2437" t="s">
+        <v>385</v>
+      </c>
+      <c r="D2437">
+        <v>26</v>
+      </c>
+      <c r="E2437" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2437" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2437" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2438">
+        <v>78</v>
+      </c>
+      <c r="B2438">
+        <v>277</v>
+      </c>
+      <c r="C2438" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2438">
+        <v>26</v>
+      </c>
+      <c r="E2438" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2438" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G2438" s="1">
+        <v>262.5</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2439">
+        <v>79</v>
+      </c>
+      <c r="B2439">
+        <v>278</v>
+      </c>
+      <c r="C2439" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2439">
+        <v>26</v>
+      </c>
+      <c r="E2439" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2439" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2439" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2440">
+        <v>80</v>
+      </c>
+      <c r="B2440">
+        <v>279</v>
+      </c>
+      <c r="C2440" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2440">
+        <v>26</v>
+      </c>
+      <c r="E2440" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2440" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2440" s="1">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2441">
+        <v>81</v>
+      </c>
+      <c r="B2441">
+        <v>280</v>
+      </c>
+      <c r="C2441" t="s">
+        <v>390</v>
+      </c>
+      <c r="D2441">
+        <v>26</v>
+      </c>
+      <c r="E2441" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2441" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2441" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2442">
+        <v>82</v>
+      </c>
+      <c r="B2442">
+        <v>281</v>
+      </c>
+      <c r="C2442" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2442">
+        <v>26</v>
+      </c>
+      <c r="E2442" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2442" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2442" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2443">
+        <v>83</v>
+      </c>
+      <c r="B2443">
+        <v>282</v>
+      </c>
+      <c r="C2443" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2443">
+        <v>26</v>
+      </c>
+      <c r="E2443" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2443" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2443" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2444">
+        <v>84</v>
+      </c>
+      <c r="B2444">
+        <v>283</v>
+      </c>
+      <c r="C2444" t="s">
+        <v>398</v>
+      </c>
+      <c r="D2444">
+        <v>26</v>
+      </c>
+      <c r="E2444" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2444" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2444" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2445">
+        <v>85</v>
+      </c>
+      <c r="B2445">
+        <v>284</v>
+      </c>
+      <c r="C2445" t="s">
+        <v>399</v>
+      </c>
+      <c r="D2445">
+        <v>26</v>
+      </c>
+      <c r="E2445" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2445" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G2445" s="1">
+        <v>378.13</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2446">
+        <v>86</v>
+      </c>
+      <c r="B2446">
+        <v>286</v>
+      </c>
+      <c r="C2446" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2446">
+        <v>26</v>
+      </c>
+      <c r="E2446" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2446" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G2446" s="1">
+        <v>171.88</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2447">
+        <v>87</v>
+      </c>
+      <c r="B2447">
+        <v>287</v>
+      </c>
+      <c r="C2447" t="s">
+        <v>402</v>
+      </c>
+      <c r="D2447">
+        <v>26</v>
+      </c>
+      <c r="E2447" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2447" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2447" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2448">
+        <v>88</v>
+      </c>
+      <c r="B2448">
+        <v>288</v>
+      </c>
+      <c r="C2448" t="s">
+        <v>404</v>
+      </c>
+      <c r="D2448">
+        <v>26</v>
+      </c>
+      <c r="E2448" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2448" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2448" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2449">
+        <v>89</v>
+      </c>
+      <c r="B2449">
+        <v>289</v>
+      </c>
+      <c r="C2449" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2449">
+        <v>26</v>
+      </c>
+      <c r="E2449" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2449" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2449" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2450">
+        <v>90</v>
+      </c>
+      <c r="B2450">
+        <v>290</v>
+      </c>
+      <c r="C2450" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2450">
+        <v>26</v>
+      </c>
+      <c r="E2450" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2450" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2450" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2451">
+        <v>91</v>
+      </c>
+      <c r="B2451">
+        <v>291</v>
+      </c>
+      <c r="C2451" t="s">
+        <v>407</v>
+      </c>
+      <c r="D2451">
+        <v>26</v>
+      </c>
+      <c r="E2451" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2451" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G2451" s="1">
+        <v>378.13</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2452">
+        <v>92</v>
+      </c>
+      <c r="B2452">
+        <v>292</v>
+      </c>
+      <c r="C2452" t="s">
+        <v>408</v>
+      </c>
+      <c r="D2452">
+        <v>26</v>
+      </c>
+      <c r="E2452" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2452" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2452" s="1" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hrs Extras Sem 29
</commit_message>
<xml_diff>
--- a/datasets/horas_extras_2024.xlsx
+++ b/datasets/horas_extras_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CC9E80FD-F272-4578-984E-F016CE327F00}"/>
+  <xr:revisionPtr revIDLastSave="109" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AAB3A21-1F72-4FBD-A88F-B71E7A6CE480}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6372" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6546" uniqueCount="417">
   <si>
     <t>José Guadalupe de Jesús Venegas Acosta</t>
   </si>
@@ -1362,8 +1362,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G2631" totalsRowShown="0">
-  <autoFilter ref="A1:G2631" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G2718" totalsRowShown="0">
+  <autoFilter ref="A1:G2718" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{933A802B-1DFA-4F50-A708-F8B071DB7BC5}" name="no"/>
     <tableColumn id="2" xr3:uid="{6D6E4B13-9BB4-4B8D-9AB2-9B4BC34C4362}" name="id"/>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C5034C-9333-43F5-A544-30F944CBFAC1}">
   <dimension ref="A1:G2949"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G2631"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2598" workbookViewId="0">
+      <selection activeCell="E2632" sqref="E2632"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61539,270 +61539,2010 @@
       </c>
     </row>
     <row r="2632" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2632" s="2"/>
+      <c r="A2632">
+        <v>1</v>
+      </c>
+      <c r="B2632">
+        <v>101</v>
+      </c>
+      <c r="C2632" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2632">
+        <v>29</v>
+      </c>
+      <c r="E2632" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2632" s="1">
+        <v>12</v>
+      </c>
+      <c r="G2632" s="3">
+        <v>1875</v>
+      </c>
     </row>
     <row r="2633" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2633" s="2"/>
+      <c r="A2633">
+        <v>2</v>
+      </c>
+      <c r="B2633">
+        <v>103</v>
+      </c>
+      <c r="C2633" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2633">
+        <v>29</v>
+      </c>
+      <c r="E2633" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2633" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2633" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="2634" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2634" s="2"/>
+      <c r="A2634">
+        <v>3</v>
+      </c>
+      <c r="B2634">
+        <v>104</v>
+      </c>
+      <c r="C2634" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2634">
+        <v>29</v>
+      </c>
+      <c r="E2634" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2634" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G2634" s="3">
+        <v>1100.4100000000001</v>
+      </c>
     </row>
     <row r="2635" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2635" s="2"/>
+      <c r="A2635">
+        <v>4</v>
+      </c>
+      <c r="B2635">
+        <v>106</v>
+      </c>
+      <c r="C2635" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2635">
+        <v>29</v>
+      </c>
+      <c r="E2635" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2635" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2635" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="2636" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2636" s="2"/>
+      <c r="A2636">
+        <v>5</v>
+      </c>
+      <c r="B2636">
+        <v>107</v>
+      </c>
+      <c r="C2636" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2636">
+        <v>29</v>
+      </c>
+      <c r="E2636" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2636" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2636" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="2637" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2637" s="2"/>
+      <c r="A2637">
+        <v>6</v>
+      </c>
+      <c r="B2637">
+        <v>108</v>
+      </c>
+      <c r="C2637" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2637">
+        <v>29</v>
+      </c>
+      <c r="E2637" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2637" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2637" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="2638" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2638" s="2"/>
+      <c r="A2638">
+        <v>7</v>
+      </c>
+      <c r="B2638">
+        <v>109</v>
+      </c>
+      <c r="C2638" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2638">
+        <v>29</v>
+      </c>
+      <c r="E2638" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2638" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2638" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="2639" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2639" s="2"/>
+      <c r="A2639">
+        <v>8</v>
+      </c>
+      <c r="B2639">
+        <v>110</v>
+      </c>
+      <c r="C2639" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2639">
+        <v>29</v>
+      </c>
+      <c r="E2639" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2639" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2639" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="2640" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2640" s="2"/>
-    </row>
-    <row r="2641" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2641" s="2"/>
-    </row>
-    <row r="2642" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2642" s="2"/>
-    </row>
-    <row r="2643" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2643" s="2"/>
-    </row>
-    <row r="2644" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2644" s="2"/>
-    </row>
-    <row r="2645" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2645" s="2"/>
-    </row>
-    <row r="2646" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2646" s="2"/>
-    </row>
-    <row r="2647" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2647" s="2"/>
-    </row>
-    <row r="2648" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2648" s="2"/>
-    </row>
-    <row r="2649" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2649" s="2"/>
-    </row>
-    <row r="2650" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2650" s="2"/>
-    </row>
-    <row r="2651" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2651" s="2"/>
-    </row>
-    <row r="2652" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2652" s="2"/>
-    </row>
-    <row r="2653" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2653" s="2"/>
-    </row>
-    <row r="2654" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2654" s="2"/>
-    </row>
-    <row r="2655" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2655" s="2"/>
-    </row>
-    <row r="2656" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2656" s="2"/>
-    </row>
-    <row r="2657" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2657" s="2"/>
-    </row>
-    <row r="2658" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2658" s="2"/>
-    </row>
-    <row r="2659" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2659" s="2"/>
-    </row>
-    <row r="2660" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2660" s="2"/>
-    </row>
-    <row r="2661" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2661" s="2"/>
-    </row>
-    <row r="2662" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2662" s="2"/>
-    </row>
-    <row r="2663" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2663" s="2"/>
-    </row>
-    <row r="2664" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2664" s="2"/>
-    </row>
-    <row r="2665" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2665" s="2"/>
-    </row>
-    <row r="2666" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2666" s="2"/>
-    </row>
-    <row r="2667" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2667" s="2"/>
-    </row>
-    <row r="2668" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2668" s="2"/>
-    </row>
-    <row r="2669" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2669" s="2"/>
-    </row>
-    <row r="2670" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2670" s="2"/>
-    </row>
-    <row r="2671" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2671" s="2"/>
-    </row>
-    <row r="2672" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2672" s="2"/>
-    </row>
-    <row r="2673" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2673" s="2"/>
-    </row>
-    <row r="2674" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2674" s="2"/>
-    </row>
-    <row r="2675" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2675" s="2"/>
-    </row>
-    <row r="2676" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2676" s="2"/>
-    </row>
-    <row r="2677" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2677" s="2"/>
-    </row>
-    <row r="2678" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2678" s="2"/>
-    </row>
-    <row r="2679" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2679" s="2"/>
-    </row>
-    <row r="2680" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2680" s="2"/>
-    </row>
-    <row r="2681" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2681" s="2"/>
-    </row>
-    <row r="2682" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2682" s="2"/>
-    </row>
-    <row r="2683" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2683" s="2"/>
-    </row>
-    <row r="2684" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2684" s="2"/>
-    </row>
-    <row r="2685" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2685" s="2"/>
-    </row>
-    <row r="2686" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2686" s="2"/>
-    </row>
-    <row r="2687" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2687" s="2"/>
-    </row>
-    <row r="2688" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2688" s="2"/>
-    </row>
-    <row r="2689" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2689" s="2"/>
-    </row>
-    <row r="2690" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2690" s="2"/>
-    </row>
-    <row r="2691" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2691" s="2"/>
-    </row>
-    <row r="2692" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2692" s="2"/>
-    </row>
-    <row r="2693" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2693" s="2"/>
-    </row>
-    <row r="2694" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2694" s="2"/>
-    </row>
-    <row r="2695" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2695" s="2"/>
-    </row>
-    <row r="2696" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2696" s="2"/>
-    </row>
-    <row r="2697" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2697" s="2"/>
-    </row>
-    <row r="2698" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2698" s="2"/>
-    </row>
-    <row r="2699" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2699" s="2"/>
-    </row>
-    <row r="2700" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2700" s="2"/>
-    </row>
-    <row r="2701" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2701" s="2"/>
-    </row>
-    <row r="2702" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2702" s="2"/>
-    </row>
-    <row r="2703" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2703" s="2"/>
-    </row>
-    <row r="2704" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2704" s="2"/>
-    </row>
-    <row r="2705" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2705" s="2"/>
-    </row>
-    <row r="2706" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2706" s="2"/>
-    </row>
-    <row r="2707" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2707" s="2"/>
-    </row>
-    <row r="2708" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2708" s="2"/>
-    </row>
-    <row r="2709" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2709" s="2"/>
-    </row>
-    <row r="2710" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2710" s="2"/>
-    </row>
-    <row r="2711" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2711" s="2"/>
-    </row>
-    <row r="2712" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2712" s="2"/>
-    </row>
-    <row r="2713" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2713" s="2"/>
-    </row>
-    <row r="2714" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2714" s="2"/>
-    </row>
-    <row r="2715" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2715" s="2"/>
-    </row>
-    <row r="2716" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2716" s="2"/>
-    </row>
-    <row r="2717" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2717" s="2"/>
-    </row>
-    <row r="2718" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2718" s="2"/>
-    </row>
-    <row r="2719" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="A2640">
+        <v>9</v>
+      </c>
+      <c r="B2640">
+        <v>111</v>
+      </c>
+      <c r="C2640" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2640">
+        <v>29</v>
+      </c>
+      <c r="E2640" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2640" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2640" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2641">
+        <v>10</v>
+      </c>
+      <c r="B2641">
+        <v>113</v>
+      </c>
+      <c r="C2641" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2641">
+        <v>29</v>
+      </c>
+      <c r="E2641" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2641" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2641" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2642">
+        <v>11</v>
+      </c>
+      <c r="B2642">
+        <v>114</v>
+      </c>
+      <c r="C2642" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2642">
+        <v>29</v>
+      </c>
+      <c r="E2642" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2642" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2642" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2643">
+        <v>12</v>
+      </c>
+      <c r="B2643">
+        <v>117</v>
+      </c>
+      <c r="C2643" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2643">
+        <v>29</v>
+      </c>
+      <c r="E2643" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2643" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G2643" s="3">
+        <v>720.96999999999991</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2644">
+        <v>13</v>
+      </c>
+      <c r="B2644">
+        <v>119</v>
+      </c>
+      <c r="C2644" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2644">
+        <v>29</v>
+      </c>
+      <c r="E2644" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2644" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2644" s="3">
+        <v>491.04999999999995</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2645">
+        <v>14</v>
+      </c>
+      <c r="B2645">
+        <v>125</v>
+      </c>
+      <c r="C2645" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2645">
+        <v>29</v>
+      </c>
+      <c r="E2645" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2645" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2645" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2646">
+        <v>15</v>
+      </c>
+      <c r="B2646">
+        <v>126</v>
+      </c>
+      <c r="C2646" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2646">
+        <v>29</v>
+      </c>
+      <c r="E2646" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2646" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2646" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2647">
+        <v>16</v>
+      </c>
+      <c r="B2647">
+        <v>129</v>
+      </c>
+      <c r="C2647" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2647">
+        <v>29</v>
+      </c>
+      <c r="E2647" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2647" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2647" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2648">
+        <v>17</v>
+      </c>
+      <c r="B2648">
+        <v>131</v>
+      </c>
+      <c r="C2648" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2648">
+        <v>29</v>
+      </c>
+      <c r="E2648" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2648" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2648" s="3">
+        <v>158.91999999999999</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2649">
+        <v>18</v>
+      </c>
+      <c r="B2649">
+        <v>133</v>
+      </c>
+      <c r="C2649" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2649">
+        <v>29</v>
+      </c>
+      <c r="E2649" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2649" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2649" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2650">
+        <v>19</v>
+      </c>
+      <c r="B2650">
+        <v>134</v>
+      </c>
+      <c r="C2650" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2650">
+        <v>29</v>
+      </c>
+      <c r="E2650" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2650" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2650" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2651">
+        <v>20</v>
+      </c>
+      <c r="B2651">
+        <v>136</v>
+      </c>
+      <c r="C2651" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2651">
+        <v>29</v>
+      </c>
+      <c r="E2651" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2651" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2651" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2652">
+        <v>21</v>
+      </c>
+      <c r="B2652">
+        <v>141</v>
+      </c>
+      <c r="C2652" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2652">
+        <v>29</v>
+      </c>
+      <c r="E2652" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2652" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2652" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2653">
+        <v>22</v>
+      </c>
+      <c r="B2653">
+        <v>145</v>
+      </c>
+      <c r="C2653" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2653">
+        <v>29</v>
+      </c>
+      <c r="E2653" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2653" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2653" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2654">
+        <v>23</v>
+      </c>
+      <c r="B2654">
+        <v>147</v>
+      </c>
+      <c r="C2654" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2654">
+        <v>29</v>
+      </c>
+      <c r="E2654" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2654" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2654" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2655">
+        <v>24</v>
+      </c>
+      <c r="B2655">
+        <v>149</v>
+      </c>
+      <c r="C2655" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2655">
+        <v>29</v>
+      </c>
+      <c r="E2655" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2655" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2655" s="3">
+        <v>142.86000000000001</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2656">
+        <v>25</v>
+      </c>
+      <c r="B2656">
+        <v>150</v>
+      </c>
+      <c r="C2656" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2656">
+        <v>29</v>
+      </c>
+      <c r="E2656" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2656" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2656" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2657">
+        <v>26</v>
+      </c>
+      <c r="B2657">
+        <v>151</v>
+      </c>
+      <c r="C2657" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2657">
+        <v>29</v>
+      </c>
+      <c r="E2657" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2657" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G2657" s="3">
+        <v>584.375</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2658">
+        <v>27</v>
+      </c>
+      <c r="B2658">
+        <v>154</v>
+      </c>
+      <c r="C2658" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2658">
+        <v>29</v>
+      </c>
+      <c r="E2658" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2658" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2658" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2659" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2659">
+        <v>28</v>
+      </c>
+      <c r="B2659">
+        <v>160</v>
+      </c>
+      <c r="C2659" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2659">
+        <v>29</v>
+      </c>
+      <c r="E2659" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2659" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2659" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2660">
+        <v>29</v>
+      </c>
+      <c r="B2660">
+        <v>162</v>
+      </c>
+      <c r="C2660" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2660">
+        <v>29</v>
+      </c>
+      <c r="E2660" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2660" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2660" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2661">
+        <v>30</v>
+      </c>
+      <c r="B2661">
+        <v>164</v>
+      </c>
+      <c r="C2661" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2661">
+        <v>29</v>
+      </c>
+      <c r="E2661" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2661" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2661" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2662">
+        <v>31</v>
+      </c>
+      <c r="B2662">
+        <v>165</v>
+      </c>
+      <c r="C2662" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2662">
+        <v>29</v>
+      </c>
+      <c r="E2662" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2662" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2662" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2663">
+        <v>32</v>
+      </c>
+      <c r="B2663">
+        <v>167</v>
+      </c>
+      <c r="C2663" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2663">
+        <v>29</v>
+      </c>
+      <c r="E2663" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2663" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2663" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2664">
+        <v>33</v>
+      </c>
+      <c r="B2664">
+        <v>175</v>
+      </c>
+      <c r="C2664" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2664">
+        <v>29</v>
+      </c>
+      <c r="E2664" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2664" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2664" s="3">
+        <v>74.11</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2665">
+        <v>34</v>
+      </c>
+      <c r="B2665">
+        <v>181</v>
+      </c>
+      <c r="C2665" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2665">
+        <v>29</v>
+      </c>
+      <c r="E2665" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2665" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2665" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2666">
+        <v>35</v>
+      </c>
+      <c r="B2666">
+        <v>182</v>
+      </c>
+      <c r="C2666" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2666">
+        <v>29</v>
+      </c>
+      <c r="E2666" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2666" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2666" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2667">
+        <v>36</v>
+      </c>
+      <c r="B2667">
+        <v>184</v>
+      </c>
+      <c r="C2667" t="s">
+        <v>368</v>
+      </c>
+      <c r="D2667">
+        <v>29</v>
+      </c>
+      <c r="E2667" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2667" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2667" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2668">
+        <v>37</v>
+      </c>
+      <c r="B2668">
+        <v>186</v>
+      </c>
+      <c r="C2668" t="s">
+        <v>369</v>
+      </c>
+      <c r="D2668">
+        <v>29</v>
+      </c>
+      <c r="E2668" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2668" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2668" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2669">
+        <v>38</v>
+      </c>
+      <c r="B2669">
+        <v>190</v>
+      </c>
+      <c r="C2669" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2669">
+        <v>29</v>
+      </c>
+      <c r="E2669" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2669" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2669" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2670">
+        <v>39</v>
+      </c>
+      <c r="B2670">
+        <v>194</v>
+      </c>
+      <c r="C2670" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2670">
+        <v>29</v>
+      </c>
+      <c r="E2670" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2670" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2670" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2671">
+        <v>40</v>
+      </c>
+      <c r="B2671">
+        <v>199</v>
+      </c>
+      <c r="C2671" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2671">
+        <v>29</v>
+      </c>
+      <c r="E2671" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2671" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2671" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2672">
+        <v>41</v>
+      </c>
+      <c r="B2672">
+        <v>200</v>
+      </c>
+      <c r="C2672" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2672">
+        <v>29</v>
+      </c>
+      <c r="E2672" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2672" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2672" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2673">
+        <v>42</v>
+      </c>
+      <c r="B2673">
+        <v>203</v>
+      </c>
+      <c r="C2673" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2673">
+        <v>29</v>
+      </c>
+      <c r="E2673" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2673" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2673" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2674">
+        <v>43</v>
+      </c>
+      <c r="B2674">
+        <v>205</v>
+      </c>
+      <c r="C2674" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2674">
+        <v>29</v>
+      </c>
+      <c r="E2674" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2674" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G2674" s="3">
+        <v>428.12</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2675">
+        <v>44</v>
+      </c>
+      <c r="B2675">
+        <v>209</v>
+      </c>
+      <c r="C2675" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2675">
+        <v>29</v>
+      </c>
+      <c r="E2675" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2675" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2675" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2676">
+        <v>45</v>
+      </c>
+      <c r="B2676">
+        <v>212</v>
+      </c>
+      <c r="C2676" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2676">
+        <v>29</v>
+      </c>
+      <c r="E2676" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2676" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2676" s="3">
+        <v>73.209999999999994</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2677">
+        <v>46</v>
+      </c>
+      <c r="B2677">
+        <v>214</v>
+      </c>
+      <c r="C2677" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2677">
+        <v>29</v>
+      </c>
+      <c r="E2677" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2677" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2677" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2678">
+        <v>47</v>
+      </c>
+      <c r="B2678">
+        <v>215</v>
+      </c>
+      <c r="C2678" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2678">
+        <v>29</v>
+      </c>
+      <c r="E2678" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2678" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2678" s="3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2679">
+        <v>48</v>
+      </c>
+      <c r="B2679">
+        <v>217</v>
+      </c>
+      <c r="C2679" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2679">
+        <v>29</v>
+      </c>
+      <c r="E2679" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2679" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2679" s="3">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2680">
+        <v>49</v>
+      </c>
+      <c r="B2680">
+        <v>219</v>
+      </c>
+      <c r="C2680" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2680">
+        <v>29</v>
+      </c>
+      <c r="E2680" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2680" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2680" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2681" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2681">
+        <v>50</v>
+      </c>
+      <c r="B2681">
+        <v>222</v>
+      </c>
+      <c r="C2681" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2681">
+        <v>29</v>
+      </c>
+      <c r="E2681" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2681" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2681" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2682">
+        <v>51</v>
+      </c>
+      <c r="B2682">
+        <v>223</v>
+      </c>
+      <c r="C2682" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2682">
+        <v>29</v>
+      </c>
+      <c r="E2682" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2682" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G2682" s="3">
+        <v>349.56000000000006</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2683">
+        <v>52</v>
+      </c>
+      <c r="B2683">
+        <v>224</v>
+      </c>
+      <c r="C2683" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2683">
+        <v>29</v>
+      </c>
+      <c r="E2683" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2683" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2683" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2684">
+        <v>53</v>
+      </c>
+      <c r="B2684">
+        <v>228</v>
+      </c>
+      <c r="C2684" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2684">
+        <v>29</v>
+      </c>
+      <c r="E2684" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2684" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2684" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2685">
+        <v>54</v>
+      </c>
+      <c r="B2685">
+        <v>234</v>
+      </c>
+      <c r="C2685" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2685">
+        <v>29</v>
+      </c>
+      <c r="E2685" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2685" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2685" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2686">
+        <v>55</v>
+      </c>
+      <c r="B2686">
+        <v>235</v>
+      </c>
+      <c r="C2686" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2686">
+        <v>29</v>
+      </c>
+      <c r="E2686" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2686" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G2686" s="3">
+        <v>189.72499999999999</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2687">
+        <v>56</v>
+      </c>
+      <c r="B2687">
+        <v>237</v>
+      </c>
+      <c r="C2687" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2687">
+        <v>29</v>
+      </c>
+      <c r="E2687" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2687" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2687" s="3">
+        <v>155.36000000000001</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2688">
+        <v>57</v>
+      </c>
+      <c r="B2688">
+        <v>241</v>
+      </c>
+      <c r="C2688" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2688">
+        <v>29</v>
+      </c>
+      <c r="E2688" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2688" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2688" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2689">
+        <v>58</v>
+      </c>
+      <c r="B2689">
+        <v>242</v>
+      </c>
+      <c r="C2689" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2689">
+        <v>29</v>
+      </c>
+      <c r="E2689" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2689" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2689" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2690">
+        <v>59</v>
+      </c>
+      <c r="B2690">
+        <v>243</v>
+      </c>
+      <c r="C2690" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2690">
+        <v>29</v>
+      </c>
+      <c r="E2690" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2690" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2690" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2691">
+        <v>60</v>
+      </c>
+      <c r="B2691">
+        <v>251</v>
+      </c>
+      <c r="C2691" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2691">
+        <v>29</v>
+      </c>
+      <c r="E2691" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2691" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G2691" s="3">
+        <v>378.125</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2692">
+        <v>61</v>
+      </c>
+      <c r="B2692">
+        <v>255</v>
+      </c>
+      <c r="C2692" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2692">
+        <v>29</v>
+      </c>
+      <c r="E2692" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2692" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2692" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2693">
+        <v>62</v>
+      </c>
+      <c r="B2693">
+        <v>258</v>
+      </c>
+      <c r="C2693" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2693">
+        <v>29</v>
+      </c>
+      <c r="E2693" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2693" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2693" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2694">
+        <v>63</v>
+      </c>
+      <c r="B2694">
+        <v>259</v>
+      </c>
+      <c r="C2694" t="s">
+        <v>348</v>
+      </c>
+      <c r="D2694">
+        <v>29</v>
+      </c>
+      <c r="E2694" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2694" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2694" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2695">
+        <v>64</v>
+      </c>
+      <c r="B2695">
+        <v>260</v>
+      </c>
+      <c r="C2695" t="s">
+        <v>351</v>
+      </c>
+      <c r="D2695">
+        <v>29</v>
+      </c>
+      <c r="E2695" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2695" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G2695" s="3">
+        <v>240.625</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2696">
+        <v>65</v>
+      </c>
+      <c r="B2696">
+        <v>261</v>
+      </c>
+      <c r="C2696" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2696">
+        <v>29</v>
+      </c>
+      <c r="E2696" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2696" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2696" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2697">
+        <v>66</v>
+      </c>
+      <c r="B2697">
+        <v>263</v>
+      </c>
+      <c r="C2697" t="s">
+        <v>359</v>
+      </c>
+      <c r="D2697">
+        <v>29</v>
+      </c>
+      <c r="E2697" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2697" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2697" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2698">
+        <v>67</v>
+      </c>
+      <c r="B2698">
+        <v>264</v>
+      </c>
+      <c r="C2698" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2698">
+        <v>29</v>
+      </c>
+      <c r="E2698" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2698" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2698" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2699">
+        <v>68</v>
+      </c>
+      <c r="B2699">
+        <v>265</v>
+      </c>
+      <c r="C2699" t="s">
+        <v>409</v>
+      </c>
+      <c r="D2699">
+        <v>29</v>
+      </c>
+      <c r="E2699" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2699" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G2699" s="3">
+        <v>294.63499999999999</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2700">
+        <v>69</v>
+      </c>
+      <c r="B2700">
+        <v>269</v>
+      </c>
+      <c r="C2700" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2700">
+        <v>29</v>
+      </c>
+      <c r="E2700" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2700" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2700" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2701">
+        <v>70</v>
+      </c>
+      <c r="B2701">
+        <v>301</v>
+      </c>
+      <c r="C2701" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2701">
+        <v>29</v>
+      </c>
+      <c r="E2701" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2701" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2701" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2702">
+        <v>71</v>
+      </c>
+      <c r="B2702">
+        <v>302</v>
+      </c>
+      <c r="C2702" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2702">
+        <v>29</v>
+      </c>
+      <c r="E2702" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2702" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2702" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2703" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2703">
+        <v>72</v>
+      </c>
+      <c r="B2703">
+        <v>273</v>
+      </c>
+      <c r="C2703" t="s">
+        <v>382</v>
+      </c>
+      <c r="D2703">
+        <v>29</v>
+      </c>
+      <c r="E2703" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2703" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2703" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2704">
+        <v>73</v>
+      </c>
+      <c r="B2704">
+        <v>274</v>
+      </c>
+      <c r="C2704" t="s">
+        <v>383</v>
+      </c>
+      <c r="D2704">
+        <v>29</v>
+      </c>
+      <c r="E2704" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2704" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2704" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2705">
+        <v>74</v>
+      </c>
+      <c r="B2705">
+        <v>275</v>
+      </c>
+      <c r="C2705" t="s">
+        <v>385</v>
+      </c>
+      <c r="D2705">
+        <v>29</v>
+      </c>
+      <c r="E2705" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2705" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G2705" s="3">
+        <v>34.375</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2706">
+        <v>75</v>
+      </c>
+      <c r="B2706">
+        <v>277</v>
+      </c>
+      <c r="C2706" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2706">
+        <v>29</v>
+      </c>
+      <c r="E2706" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2706" s="1">
+        <v>6</v>
+      </c>
+      <c r="G2706" s="3">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2707">
+        <v>76</v>
+      </c>
+      <c r="B2707">
+        <v>278</v>
+      </c>
+      <c r="C2707" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2707">
+        <v>29</v>
+      </c>
+      <c r="E2707" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2707" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2707" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2708">
+        <v>77</v>
+      </c>
+      <c r="B2708">
+        <v>279</v>
+      </c>
+      <c r="C2708" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2708">
+        <v>29</v>
+      </c>
+      <c r="E2708" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2708" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2708" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2709">
+        <v>78</v>
+      </c>
+      <c r="B2709">
+        <v>281</v>
+      </c>
+      <c r="C2709" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2709">
+        <v>29</v>
+      </c>
+      <c r="E2709" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2709" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2709" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2710">
+        <v>79</v>
+      </c>
+      <c r="B2710">
+        <v>282</v>
+      </c>
+      <c r="C2710" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2710">
+        <v>29</v>
+      </c>
+      <c r="E2710" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2710" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2710" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2711">
+        <v>80</v>
+      </c>
+      <c r="B2711">
+        <v>283</v>
+      </c>
+      <c r="C2711" t="s">
+        <v>398</v>
+      </c>
+      <c r="D2711">
+        <v>29</v>
+      </c>
+      <c r="E2711" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2711" s="1">
+        <v>7</v>
+      </c>
+      <c r="G2711" s="3">
+        <v>481.25</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2712">
+        <v>81</v>
+      </c>
+      <c r="B2712">
+        <v>284</v>
+      </c>
+      <c r="C2712" t="s">
+        <v>399</v>
+      </c>
+      <c r="D2712">
+        <v>29</v>
+      </c>
+      <c r="E2712" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2712" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2712" s="3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2713">
+        <v>82</v>
+      </c>
+      <c r="B2713">
+        <v>286</v>
+      </c>
+      <c r="C2713" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2713">
+        <v>29</v>
+      </c>
+      <c r="E2713" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2713" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G2713" s="3">
+        <v>171.875</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2714">
+        <v>83</v>
+      </c>
+      <c r="B2714">
+        <v>287</v>
+      </c>
+      <c r="C2714" t="s">
+        <v>402</v>
+      </c>
+      <c r="D2714">
+        <v>29</v>
+      </c>
+      <c r="E2714" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2714" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2714" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2715">
+        <v>84</v>
+      </c>
+      <c r="B2715">
+        <v>288</v>
+      </c>
+      <c r="C2715" t="s">
+        <v>404</v>
+      </c>
+      <c r="D2715">
+        <v>29</v>
+      </c>
+      <c r="E2715" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2715" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2715" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2716">
+        <v>85</v>
+      </c>
+      <c r="B2716">
+        <v>289</v>
+      </c>
+      <c r="C2716" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2716">
+        <v>29</v>
+      </c>
+      <c r="E2716" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2716" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2716" s="3">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2717">
+        <v>86</v>
+      </c>
+      <c r="B2717">
+        <v>291</v>
+      </c>
+      <c r="C2717" t="s">
+        <v>407</v>
+      </c>
+      <c r="D2717">
+        <v>29</v>
+      </c>
+      <c r="E2717" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2717" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2717" s="3">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2718">
+        <v>87</v>
+      </c>
+      <c r="B2718">
+        <v>292</v>
+      </c>
+      <c r="C2718" t="s">
+        <v>408</v>
+      </c>
+      <c r="D2718">
+        <v>29</v>
+      </c>
+      <c r="E2718" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2718" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2718" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2719" s="2"/>
     </row>
-    <row r="2720" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2720" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2720" s="2"/>
     </row>
     <row r="2721" spans="7:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Prod Hrs Sem 30
</commit_message>
<xml_diff>
--- a/datasets/horas_extras_2024.xlsx
+++ b/datasets/horas_extras_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AAB3A21-1F72-4FBD-A88F-B71E7A6CE480}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F22E8BE3-1B4A-4B38-A1E9-902205B6B223}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6546" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6714" uniqueCount="417">
   <si>
     <t>José Guadalupe de Jesús Venegas Acosta</t>
   </si>
@@ -1362,8 +1362,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G2718" totalsRowShown="0">
-  <autoFilter ref="A1:G2718" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G2802" totalsRowShown="0">
+  <autoFilter ref="A1:G2802" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{933A802B-1DFA-4F50-A708-F8B071DB7BC5}" name="no"/>
     <tableColumn id="2" xr3:uid="{6D6E4B13-9BB4-4B8D-9AB2-9B4BC34C4362}" name="id"/>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C5034C-9333-43F5-A544-30F944CBFAC1}">
   <dimension ref="A1:G2949"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2598" workbookViewId="0">
-      <selection activeCell="E2632" sqref="E2632"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2780" workbookViewId="0">
+      <selection activeCell="G2798" sqref="G2798"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63540,297 +63540,1977 @@
       </c>
     </row>
     <row r="2719" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2719" s="2"/>
+      <c r="A2719">
+        <v>1</v>
+      </c>
+      <c r="B2719">
+        <v>101</v>
+      </c>
+      <c r="C2719" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2719">
+        <v>30</v>
+      </c>
+      <c r="E2719" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2719" s="1">
+        <v>12</v>
+      </c>
+      <c r="G2719" s="3">
+        <v>1875</v>
+      </c>
     </row>
     <row r="2720" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G2720" s="2"/>
-    </row>
-    <row r="2721" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2721" s="2"/>
-    </row>
-    <row r="2722" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2722" s="2"/>
-    </row>
-    <row r="2723" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2723" s="2"/>
-    </row>
-    <row r="2724" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2724" s="2"/>
-    </row>
-    <row r="2725" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2725" s="2"/>
-    </row>
-    <row r="2726" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2726" s="2"/>
-    </row>
-    <row r="2727" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2727" s="2"/>
-    </row>
-    <row r="2728" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2728" s="2"/>
-    </row>
-    <row r="2729" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2729" s="2"/>
-    </row>
-    <row r="2730" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2730" s="2"/>
-    </row>
-    <row r="2731" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2731" s="2"/>
-    </row>
-    <row r="2732" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2732" s="2"/>
-    </row>
-    <row r="2733" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2733" s="2"/>
-    </row>
-    <row r="2734" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2734" s="2"/>
-    </row>
-    <row r="2735" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2735" s="2"/>
-    </row>
-    <row r="2736" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2736" s="2"/>
-    </row>
-    <row r="2737" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2737" s="2"/>
-    </row>
-    <row r="2738" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2738" s="2"/>
-    </row>
-    <row r="2739" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2739" s="2"/>
-    </row>
-    <row r="2740" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2740" s="2"/>
-    </row>
-    <row r="2741" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2741" s="2"/>
-    </row>
-    <row r="2742" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2742" s="2"/>
-    </row>
-    <row r="2743" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2743" s="2"/>
-    </row>
-    <row r="2744" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2744" s="2"/>
-    </row>
-    <row r="2745" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2745" s="2"/>
-    </row>
-    <row r="2746" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2746" s="2"/>
-    </row>
-    <row r="2747" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2747" s="2"/>
-    </row>
-    <row r="2748" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2748" s="2"/>
-    </row>
-    <row r="2749" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2749" s="2"/>
-    </row>
-    <row r="2750" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2750" s="2"/>
-    </row>
-    <row r="2751" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2751" s="2"/>
-    </row>
-    <row r="2752" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2752" s="2"/>
-    </row>
-    <row r="2753" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2753" s="2"/>
-    </row>
-    <row r="2754" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2754" s="2"/>
-    </row>
-    <row r="2755" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2755" s="2"/>
-    </row>
-    <row r="2756" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2756" s="2"/>
-    </row>
-    <row r="2757" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2757" s="2"/>
-    </row>
-    <row r="2758" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2758" s="2"/>
-    </row>
-    <row r="2759" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2759" s="2"/>
-    </row>
-    <row r="2760" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2760" s="2"/>
-    </row>
-    <row r="2761" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2761" s="2"/>
-    </row>
-    <row r="2762" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2762" s="2"/>
-    </row>
-    <row r="2763" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2763" s="2"/>
-    </row>
-    <row r="2764" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2764" s="2"/>
-    </row>
-    <row r="2765" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2765" s="2"/>
-    </row>
-    <row r="2766" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2766" s="2"/>
-    </row>
-    <row r="2767" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2767" s="2"/>
-    </row>
-    <row r="2768" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2768" s="2"/>
-    </row>
-    <row r="2769" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2769" s="2"/>
-    </row>
-    <row r="2770" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2770" s="2"/>
-    </row>
-    <row r="2771" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2771" s="2"/>
-    </row>
-    <row r="2772" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2772" s="2"/>
-    </row>
-    <row r="2773" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2773" s="2"/>
-    </row>
-    <row r="2774" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2774" s="2"/>
-    </row>
-    <row r="2775" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2775" s="2"/>
-    </row>
-    <row r="2776" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2776" s="2"/>
-    </row>
-    <row r="2777" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2777" s="2"/>
-    </row>
-    <row r="2778" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2778" s="2"/>
-    </row>
-    <row r="2779" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2779" s="2"/>
-    </row>
-    <row r="2780" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2780" s="2"/>
-    </row>
-    <row r="2781" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2781" s="2"/>
-    </row>
-    <row r="2782" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2782" s="2"/>
-    </row>
-    <row r="2783" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2783" s="2"/>
-    </row>
-    <row r="2784" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2784" s="2"/>
-    </row>
-    <row r="2785" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2785" s="2"/>
-    </row>
-    <row r="2786" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2786" s="2"/>
-    </row>
-    <row r="2787" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2787" s="2"/>
-    </row>
-    <row r="2788" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2788" s="2"/>
-    </row>
-    <row r="2789" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2789" s="2"/>
-    </row>
-    <row r="2790" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2790" s="2"/>
-    </row>
-    <row r="2791" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2791" s="2"/>
-    </row>
-    <row r="2792" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2792" s="2"/>
-    </row>
-    <row r="2793" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2793" s="2"/>
-    </row>
-    <row r="2794" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2794" s="2"/>
-    </row>
-    <row r="2795" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2795" s="2"/>
-    </row>
-    <row r="2796" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2796" s="2"/>
-    </row>
-    <row r="2797" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2797" s="2"/>
-    </row>
-    <row r="2798" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2798" s="2"/>
-    </row>
-    <row r="2799" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2799" s="2"/>
-    </row>
-    <row r="2800" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2800" s="2"/>
-    </row>
-    <row r="2801" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2801" s="2"/>
-    </row>
-    <row r="2802" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G2802" s="2"/>
-    </row>
-    <row r="2803" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="A2720">
+        <v>2</v>
+      </c>
+      <c r="B2720">
+        <v>103</v>
+      </c>
+      <c r="C2720" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2720">
+        <v>30</v>
+      </c>
+      <c r="E2720" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2720" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2720" s="3">
+        <v>430.36</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2721">
+        <v>3</v>
+      </c>
+      <c r="B2721">
+        <v>104</v>
+      </c>
+      <c r="C2721" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2721">
+        <v>30</v>
+      </c>
+      <c r="E2721" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2721" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G2721" s="3">
+        <v>453.11</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2722">
+        <v>4</v>
+      </c>
+      <c r="B2722">
+        <v>106</v>
+      </c>
+      <c r="C2722" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2722">
+        <v>30</v>
+      </c>
+      <c r="E2722" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2722" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2722" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2723">
+        <v>5</v>
+      </c>
+      <c r="B2723">
+        <v>107</v>
+      </c>
+      <c r="C2723" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2723">
+        <v>30</v>
+      </c>
+      <c r="E2723" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2723" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2723" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2724">
+        <v>6</v>
+      </c>
+      <c r="B2724">
+        <v>108</v>
+      </c>
+      <c r="C2724" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2724">
+        <v>30</v>
+      </c>
+      <c r="E2724" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2724" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2724" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2725" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2725">
+        <v>7</v>
+      </c>
+      <c r="B2725">
+        <v>109</v>
+      </c>
+      <c r="C2725" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2725">
+        <v>30</v>
+      </c>
+      <c r="E2725" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2725" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2725" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2726">
+        <v>8</v>
+      </c>
+      <c r="B2726">
+        <v>110</v>
+      </c>
+      <c r="C2726" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2726">
+        <v>30</v>
+      </c>
+      <c r="E2726" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2726" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2726" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2727">
+        <v>9</v>
+      </c>
+      <c r="B2727">
+        <v>111</v>
+      </c>
+      <c r="C2727" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2727">
+        <v>30</v>
+      </c>
+      <c r="E2727" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2727" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2727" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2728">
+        <v>10</v>
+      </c>
+      <c r="B2728">
+        <v>113</v>
+      </c>
+      <c r="C2728" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2728">
+        <v>30</v>
+      </c>
+      <c r="E2728" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2728" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2728" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2729">
+        <v>11</v>
+      </c>
+      <c r="B2729">
+        <v>114</v>
+      </c>
+      <c r="C2729" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2729">
+        <v>30</v>
+      </c>
+      <c r="E2729" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2729" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2729" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2730">
+        <v>12</v>
+      </c>
+      <c r="B2730">
+        <v>117</v>
+      </c>
+      <c r="C2730" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2730">
+        <v>30</v>
+      </c>
+      <c r="E2730" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2730" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2730" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2731">
+        <v>13</v>
+      </c>
+      <c r="B2731">
+        <v>119</v>
+      </c>
+      <c r="C2731" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2731">
+        <v>30</v>
+      </c>
+      <c r="E2731" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2731" s="1">
+        <v>6</v>
+      </c>
+      <c r="G2731" s="3">
+        <v>589.26</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2732">
+        <v>14</v>
+      </c>
+      <c r="B2732">
+        <v>125</v>
+      </c>
+      <c r="C2732" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2732">
+        <v>30</v>
+      </c>
+      <c r="E2732" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2732" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2732" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2733">
+        <v>15</v>
+      </c>
+      <c r="B2733">
+        <v>126</v>
+      </c>
+      <c r="C2733" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2733">
+        <v>30</v>
+      </c>
+      <c r="E2733" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2733" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2733" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2734">
+        <v>16</v>
+      </c>
+      <c r="B2734">
+        <v>129</v>
+      </c>
+      <c r="C2734" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2734">
+        <v>30</v>
+      </c>
+      <c r="E2734" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2734" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2734" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2735">
+        <v>17</v>
+      </c>
+      <c r="B2735">
+        <v>131</v>
+      </c>
+      <c r="C2735" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2735">
+        <v>30</v>
+      </c>
+      <c r="E2735" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2735" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2735" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2736">
+        <v>18</v>
+      </c>
+      <c r="B2736">
+        <v>133</v>
+      </c>
+      <c r="C2736" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2736">
+        <v>30</v>
+      </c>
+      <c r="E2736" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2736" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2736" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2737">
+        <v>19</v>
+      </c>
+      <c r="B2737">
+        <v>134</v>
+      </c>
+      <c r="C2737" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2737">
+        <v>30</v>
+      </c>
+      <c r="E2737" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2737" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2737" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2738">
+        <v>20</v>
+      </c>
+      <c r="B2738">
+        <v>136</v>
+      </c>
+      <c r="C2738" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2738">
+        <v>30</v>
+      </c>
+      <c r="E2738" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2738" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2738" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2739">
+        <v>21</v>
+      </c>
+      <c r="B2739">
+        <v>141</v>
+      </c>
+      <c r="C2739" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2739">
+        <v>30</v>
+      </c>
+      <c r="E2739" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2739" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2739" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2740">
+        <v>22</v>
+      </c>
+      <c r="B2740">
+        <v>145</v>
+      </c>
+      <c r="C2740" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2740">
+        <v>30</v>
+      </c>
+      <c r="E2740" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2740" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2740" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2741">
+        <v>23</v>
+      </c>
+      <c r="B2741">
+        <v>147</v>
+      </c>
+      <c r="C2741" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2741">
+        <v>30</v>
+      </c>
+      <c r="E2741" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2741" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2741" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2742">
+        <v>24</v>
+      </c>
+      <c r="B2742">
+        <v>149</v>
+      </c>
+      <c r="C2742" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2742">
+        <v>30</v>
+      </c>
+      <c r="E2742" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2742" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2742" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2743">
+        <v>25</v>
+      </c>
+      <c r="B2743">
+        <v>150</v>
+      </c>
+      <c r="C2743" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2743">
+        <v>30</v>
+      </c>
+      <c r="E2743" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2743" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2743" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2744">
+        <v>26</v>
+      </c>
+      <c r="B2744">
+        <v>151</v>
+      </c>
+      <c r="C2744" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2744">
+        <v>30</v>
+      </c>
+      <c r="E2744" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2744" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2744" s="3">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2745">
+        <v>27</v>
+      </c>
+      <c r="B2745">
+        <v>154</v>
+      </c>
+      <c r="C2745" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2745">
+        <v>30</v>
+      </c>
+      <c r="E2745" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2745" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2745" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2746">
+        <v>28</v>
+      </c>
+      <c r="B2746">
+        <v>160</v>
+      </c>
+      <c r="C2746" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2746">
+        <v>30</v>
+      </c>
+      <c r="E2746" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2746" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2746" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2747" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2747">
+        <v>29</v>
+      </c>
+      <c r="B2747">
+        <v>162</v>
+      </c>
+      <c r="C2747" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2747">
+        <v>30</v>
+      </c>
+      <c r="E2747" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2747" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2747" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2748">
+        <v>30</v>
+      </c>
+      <c r="B2748">
+        <v>164</v>
+      </c>
+      <c r="C2748" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2748">
+        <v>30</v>
+      </c>
+      <c r="E2748" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2748" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2748" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2749">
+        <v>31</v>
+      </c>
+      <c r="B2749">
+        <v>165</v>
+      </c>
+      <c r="C2749" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2749">
+        <v>30</v>
+      </c>
+      <c r="E2749" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2749" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2749" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2750">
+        <v>32</v>
+      </c>
+      <c r="B2750">
+        <v>167</v>
+      </c>
+      <c r="C2750" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2750">
+        <v>30</v>
+      </c>
+      <c r="E2750" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2750" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2750" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2751">
+        <v>33</v>
+      </c>
+      <c r="B2751">
+        <v>175</v>
+      </c>
+      <c r="C2751" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2751">
+        <v>30</v>
+      </c>
+      <c r="E2751" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2751" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2751" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2752">
+        <v>34</v>
+      </c>
+      <c r="B2752">
+        <v>181</v>
+      </c>
+      <c r="C2752" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2752">
+        <v>30</v>
+      </c>
+      <c r="E2752" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2752" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2752" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2753">
+        <v>35</v>
+      </c>
+      <c r="B2753">
+        <v>182</v>
+      </c>
+      <c r="C2753" t="s">
+        <v>203</v>
+      </c>
+      <c r="D2753">
+        <v>30</v>
+      </c>
+      <c r="E2753" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2753" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2753" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2754">
+        <v>36</v>
+      </c>
+      <c r="B2754">
+        <v>184</v>
+      </c>
+      <c r="C2754" t="s">
+        <v>368</v>
+      </c>
+      <c r="D2754">
+        <v>30</v>
+      </c>
+      <c r="E2754" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2754" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2754" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2755">
+        <v>37</v>
+      </c>
+      <c r="B2755">
+        <v>186</v>
+      </c>
+      <c r="C2755" t="s">
+        <v>369</v>
+      </c>
+      <c r="D2755">
+        <v>30</v>
+      </c>
+      <c r="E2755" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2755" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2755" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2756">
+        <v>38</v>
+      </c>
+      <c r="B2756">
+        <v>190</v>
+      </c>
+      <c r="C2756" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2756">
+        <v>30</v>
+      </c>
+      <c r="E2756" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2756" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2756" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2757">
+        <v>39</v>
+      </c>
+      <c r="B2757">
+        <v>194</v>
+      </c>
+      <c r="C2757" t="s">
+        <v>370</v>
+      </c>
+      <c r="D2757">
+        <v>30</v>
+      </c>
+      <c r="E2757" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2757" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2757" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2758">
+        <v>40</v>
+      </c>
+      <c r="B2758">
+        <v>199</v>
+      </c>
+      <c r="C2758" t="s">
+        <v>371</v>
+      </c>
+      <c r="D2758">
+        <v>30</v>
+      </c>
+      <c r="E2758" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2758" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2758" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2759">
+        <v>41</v>
+      </c>
+      <c r="B2759">
+        <v>200</v>
+      </c>
+      <c r="C2759" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2759">
+        <v>30</v>
+      </c>
+      <c r="E2759" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2759" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2759" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2760">
+        <v>42</v>
+      </c>
+      <c r="B2760">
+        <v>203</v>
+      </c>
+      <c r="C2760" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2760">
+        <v>30</v>
+      </c>
+      <c r="E2760" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2760" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2760" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2761">
+        <v>43</v>
+      </c>
+      <c r="B2761">
+        <v>205</v>
+      </c>
+      <c r="C2761" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2761">
+        <v>30</v>
+      </c>
+      <c r="E2761" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2761" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2761" s="3">
+        <v>122.32</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2762">
+        <v>44</v>
+      </c>
+      <c r="B2762">
+        <v>209</v>
+      </c>
+      <c r="C2762" t="s">
+        <v>238</v>
+      </c>
+      <c r="D2762">
+        <v>30</v>
+      </c>
+      <c r="E2762" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2762" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2762" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2763">
+        <v>45</v>
+      </c>
+      <c r="B2763">
+        <v>212</v>
+      </c>
+      <c r="C2763" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2763">
+        <v>30</v>
+      </c>
+      <c r="E2763" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2763" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2763" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2764">
+        <v>46</v>
+      </c>
+      <c r="B2764">
+        <v>214</v>
+      </c>
+      <c r="C2764" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2764">
+        <v>30</v>
+      </c>
+      <c r="E2764" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2764" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2764" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2765">
+        <v>47</v>
+      </c>
+      <c r="B2765">
+        <v>215</v>
+      </c>
+      <c r="C2765" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2765">
+        <v>30</v>
+      </c>
+      <c r="E2765" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2765" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2765" s="3">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2766">
+        <v>48</v>
+      </c>
+      <c r="B2766">
+        <v>217</v>
+      </c>
+      <c r="C2766" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2766">
+        <v>30</v>
+      </c>
+      <c r="E2766" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2766" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2766" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2767">
+        <v>49</v>
+      </c>
+      <c r="B2767">
+        <v>219</v>
+      </c>
+      <c r="C2767" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2767">
+        <v>30</v>
+      </c>
+      <c r="E2767" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2767" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2767" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2768">
+        <v>50</v>
+      </c>
+      <c r="B2768">
+        <v>222</v>
+      </c>
+      <c r="C2768" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2768">
+        <v>30</v>
+      </c>
+      <c r="E2768" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2768" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2768" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2769">
+        <v>51</v>
+      </c>
+      <c r="B2769">
+        <v>223</v>
+      </c>
+      <c r="C2769" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2769">
+        <v>30</v>
+      </c>
+      <c r="E2769" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2769" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2769" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2770">
+        <v>52</v>
+      </c>
+      <c r="B2770">
+        <v>224</v>
+      </c>
+      <c r="C2770" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2770">
+        <v>30</v>
+      </c>
+      <c r="E2770" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2770" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2770" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2771">
+        <v>53</v>
+      </c>
+      <c r="B2771">
+        <v>228</v>
+      </c>
+      <c r="C2771" t="s">
+        <v>267</v>
+      </c>
+      <c r="D2771">
+        <v>30</v>
+      </c>
+      <c r="E2771" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2771" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2771" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2772">
+        <v>54</v>
+      </c>
+      <c r="B2772">
+        <v>234</v>
+      </c>
+      <c r="C2772" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2772">
+        <v>30</v>
+      </c>
+      <c r="E2772" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2772" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2772" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2773">
+        <v>55</v>
+      </c>
+      <c r="B2773">
+        <v>235</v>
+      </c>
+      <c r="C2773" t="s">
+        <v>280</v>
+      </c>
+      <c r="D2773">
+        <v>30</v>
+      </c>
+      <c r="E2773" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2773" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2773" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2774">
+        <v>56</v>
+      </c>
+      <c r="B2774">
+        <v>237</v>
+      </c>
+      <c r="C2774" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2774">
+        <v>30</v>
+      </c>
+      <c r="E2774" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2774" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2774" s="3">
+        <v>77.680000000000007</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2775">
+        <v>57</v>
+      </c>
+      <c r="B2775">
+        <v>241</v>
+      </c>
+      <c r="C2775" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2775">
+        <v>30</v>
+      </c>
+      <c r="E2775" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2775" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2775" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2776">
+        <v>58</v>
+      </c>
+      <c r="B2776">
+        <v>243</v>
+      </c>
+      <c r="C2776" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2776">
+        <v>30</v>
+      </c>
+      <c r="E2776" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2776" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2776" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2777">
+        <v>59</v>
+      </c>
+      <c r="B2777">
+        <v>251</v>
+      </c>
+      <c r="C2777" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2777">
+        <v>30</v>
+      </c>
+      <c r="E2777" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2777" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2777" s="3">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2778">
+        <v>60</v>
+      </c>
+      <c r="B2778">
+        <v>255</v>
+      </c>
+      <c r="C2778" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2778">
+        <v>30</v>
+      </c>
+      <c r="E2778" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2778" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2778" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2779">
+        <v>61</v>
+      </c>
+      <c r="B2779">
+        <v>258</v>
+      </c>
+      <c r="C2779" t="s">
+        <v>345</v>
+      </c>
+      <c r="D2779">
+        <v>30</v>
+      </c>
+      <c r="E2779" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2779" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2779" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2780">
+        <v>62</v>
+      </c>
+      <c r="B2780">
+        <v>260</v>
+      </c>
+      <c r="C2780" t="s">
+        <v>351</v>
+      </c>
+      <c r="D2780">
+        <v>30</v>
+      </c>
+      <c r="E2780" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2780" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2780" s="3">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2781">
+        <v>63</v>
+      </c>
+      <c r="B2781">
+        <v>261</v>
+      </c>
+      <c r="C2781" t="s">
+        <v>354</v>
+      </c>
+      <c r="D2781">
+        <v>30</v>
+      </c>
+      <c r="E2781" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2781" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2781" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2782" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2782">
+        <v>64</v>
+      </c>
+      <c r="B2782">
+        <v>263</v>
+      </c>
+      <c r="C2782" t="s">
+        <v>359</v>
+      </c>
+      <c r="D2782">
+        <v>30</v>
+      </c>
+      <c r="E2782" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2782" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2782" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2783">
+        <v>65</v>
+      </c>
+      <c r="B2783">
+        <v>264</v>
+      </c>
+      <c r="C2783" t="s">
+        <v>360</v>
+      </c>
+      <c r="D2783">
+        <v>30</v>
+      </c>
+      <c r="E2783" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2783" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2783" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2784" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2784">
+        <v>66</v>
+      </c>
+      <c r="B2784">
+        <v>265</v>
+      </c>
+      <c r="C2784" t="s">
+        <v>409</v>
+      </c>
+      <c r="D2784">
+        <v>30</v>
+      </c>
+      <c r="E2784" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2784" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2784" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2785">
+        <v>67</v>
+      </c>
+      <c r="B2785">
+        <v>269</v>
+      </c>
+      <c r="C2785" t="s">
+        <v>374</v>
+      </c>
+      <c r="D2785">
+        <v>30</v>
+      </c>
+      <c r="E2785" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2785" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2785" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2786" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2786">
+        <v>68</v>
+      </c>
+      <c r="B2786">
+        <v>301</v>
+      </c>
+      <c r="C2786" t="s">
+        <v>362</v>
+      </c>
+      <c r="D2786">
+        <v>30</v>
+      </c>
+      <c r="E2786" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2786" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2786" s="3">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2787">
+        <v>69</v>
+      </c>
+      <c r="B2787">
+        <v>302</v>
+      </c>
+      <c r="C2787" t="s">
+        <v>363</v>
+      </c>
+      <c r="D2787">
+        <v>30</v>
+      </c>
+      <c r="E2787" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2787" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G2787" s="3">
+        <v>171.875</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2788">
+        <v>70</v>
+      </c>
+      <c r="B2788">
+        <v>273</v>
+      </c>
+      <c r="C2788" t="s">
+        <v>382</v>
+      </c>
+      <c r="D2788">
+        <v>30</v>
+      </c>
+      <c r="E2788" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2788" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2788" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2789">
+        <v>71</v>
+      </c>
+      <c r="B2789">
+        <v>274</v>
+      </c>
+      <c r="C2789" t="s">
+        <v>383</v>
+      </c>
+      <c r="D2789">
+        <v>30</v>
+      </c>
+      <c r="E2789" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2789" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2789" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2790">
+        <v>72</v>
+      </c>
+      <c r="B2790">
+        <v>275</v>
+      </c>
+      <c r="C2790" t="s">
+        <v>385</v>
+      </c>
+      <c r="D2790">
+        <v>30</v>
+      </c>
+      <c r="E2790" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2790" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2790" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2791" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2791">
+        <v>73</v>
+      </c>
+      <c r="B2791">
+        <v>277</v>
+      </c>
+      <c r="C2791" t="s">
+        <v>387</v>
+      </c>
+      <c r="D2791">
+        <v>30</v>
+      </c>
+      <c r="E2791" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2791" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2791" s="3">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2792">
+        <v>74</v>
+      </c>
+      <c r="B2792">
+        <v>278</v>
+      </c>
+      <c r="C2792" t="s">
+        <v>388</v>
+      </c>
+      <c r="D2792">
+        <v>30</v>
+      </c>
+      <c r="E2792" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2792" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2792" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2793">
+        <v>75</v>
+      </c>
+      <c r="B2793">
+        <v>279</v>
+      </c>
+      <c r="C2793" t="s">
+        <v>389</v>
+      </c>
+      <c r="D2793">
+        <v>30</v>
+      </c>
+      <c r="E2793" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2793" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2793" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2794">
+        <v>76</v>
+      </c>
+      <c r="B2794">
+        <v>281</v>
+      </c>
+      <c r="C2794" t="s">
+        <v>400</v>
+      </c>
+      <c r="D2794">
+        <v>30</v>
+      </c>
+      <c r="E2794" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2794" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2794" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2795" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2795">
+        <v>77</v>
+      </c>
+      <c r="B2795">
+        <v>282</v>
+      </c>
+      <c r="C2795" t="s">
+        <v>397</v>
+      </c>
+      <c r="D2795">
+        <v>30</v>
+      </c>
+      <c r="E2795" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2795" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2795" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2796" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2796">
+        <v>78</v>
+      </c>
+      <c r="B2796">
+        <v>283</v>
+      </c>
+      <c r="C2796" t="s">
+        <v>398</v>
+      </c>
+      <c r="D2796">
+        <v>30</v>
+      </c>
+      <c r="E2796" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2796" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2796" s="3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2797" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2797">
+        <v>79</v>
+      </c>
+      <c r="B2797">
+        <v>284</v>
+      </c>
+      <c r="C2797" t="s">
+        <v>399</v>
+      </c>
+      <c r="D2797">
+        <v>30</v>
+      </c>
+      <c r="E2797" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2797" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G2797" s="3">
+        <v>309.375</v>
+      </c>
+    </row>
+    <row r="2798" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2798">
+        <v>80</v>
+      </c>
+      <c r="B2798">
+        <v>286</v>
+      </c>
+      <c r="C2798" t="s">
+        <v>401</v>
+      </c>
+      <c r="D2798">
+        <v>30</v>
+      </c>
+      <c r="E2798" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2798" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G2798" s="3">
+        <v>171.875</v>
+      </c>
+    </row>
+    <row r="2799" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2799">
+        <v>81</v>
+      </c>
+      <c r="B2799">
+        <v>287</v>
+      </c>
+      <c r="C2799" t="s">
+        <v>402</v>
+      </c>
+      <c r="D2799">
+        <v>30</v>
+      </c>
+      <c r="E2799" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2799" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2799" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2800" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2800">
+        <v>82</v>
+      </c>
+      <c r="B2800">
+        <v>288</v>
+      </c>
+      <c r="C2800" t="s">
+        <v>404</v>
+      </c>
+      <c r="D2800">
+        <v>30</v>
+      </c>
+      <c r="E2800" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2800" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2800" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2801" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2801">
+        <v>83</v>
+      </c>
+      <c r="B2801">
+        <v>289</v>
+      </c>
+      <c r="C2801" t="s">
+        <v>405</v>
+      </c>
+      <c r="D2801">
+        <v>30</v>
+      </c>
+      <c r="E2801" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2801" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G2801" s="3">
+        <v>34.375</v>
+      </c>
+    </row>
+    <row r="2802" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2802">
+        <v>84</v>
+      </c>
+      <c r="B2802">
+        <v>291</v>
+      </c>
+      <c r="C2802" t="s">
+        <v>407</v>
+      </c>
+      <c r="D2802">
+        <v>30</v>
+      </c>
+      <c r="E2802" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2802" s="1">
+        <v>4</v>
+      </c>
+      <c r="G2802" s="3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2803" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2803" s="2"/>
     </row>
-    <row r="2804" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2804" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2804" s="2"/>
     </row>
-    <row r="2805" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2805" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2805" s="2"/>
     </row>
-    <row r="2806" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2806" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2806" s="2"/>
     </row>
-    <row r="2807" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2807" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2807" s="2"/>
     </row>
-    <row r="2808" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2808" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2808" s="2"/>
     </row>
-    <row r="2809" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2809" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2809" s="2"/>
     </row>
-    <row r="2810" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2810" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2810" s="2"/>
     </row>
-    <row r="2811" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2811" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2811" s="2"/>
     </row>
-    <row r="2812" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2812" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2812" s="2"/>
     </row>
-    <row r="2813" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2813" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2813" s="2"/>
     </row>
-    <row r="2814" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2814" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2814" s="2"/>
     </row>
-    <row r="2815" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2815" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2815" s="2"/>
     </row>
-    <row r="2816" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="2816" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G2816" s="2"/>
     </row>
     <row r="2817" spans="7:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Prod Hrs Sem 33
</commit_message>
<xml_diff>
--- a/datasets/horas_extras_2024.xlsx
+++ b/datasets/horas_extras_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1638A5A9-4C81-4875-9200-B1EE5D4168BF}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1FE785B-8CAC-4C68-BA9B-810146057CBC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7042" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7204" uniqueCount="425">
   <si>
     <t>José Guadalupe de Jesús Venegas Acosta</t>
   </si>
@@ -1385,8 +1385,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G2966" totalsRowShown="0">
-  <autoFilter ref="A1:G2966" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G3047" totalsRowShown="0">
+  <autoFilter ref="A1:G3047" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{933A802B-1DFA-4F50-A708-F8B071DB7BC5}" name="no"/>
     <tableColumn id="2" xr3:uid="{6D6E4B13-9BB4-4B8D-9AB2-9B4BC34C4362}" name="id"/>
@@ -1717,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C5034C-9333-43F5-A544-30F944CBFAC1}">
-  <dimension ref="A1:G2966"/>
+  <dimension ref="A1:G3047"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2949" workbookViewId="0">
-      <selection activeCell="E2957" sqref="E2957"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3017" workbookViewId="0">
+      <selection activeCell="A2967" sqref="A2967:G3047"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69266,6 +69266,1869 @@
         <v>206.25</v>
       </c>
     </row>
+    <row r="2967" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2967">
+        <v>1</v>
+      </c>
+      <c r="B2967">
+        <v>101</v>
+      </c>
+      <c r="C2967" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2967">
+        <v>33</v>
+      </c>
+      <c r="E2967" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2967" s="1">
+        <v>12</v>
+      </c>
+      <c r="G2967" s="2">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="2968" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2968">
+        <v>2</v>
+      </c>
+      <c r="B2968">
+        <v>103</v>
+      </c>
+      <c r="C2968" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2968">
+        <v>33</v>
+      </c>
+      <c r="E2968" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2968" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2968" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2969" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2969">
+        <v>3</v>
+      </c>
+      <c r="B2969">
+        <v>104</v>
+      </c>
+      <c r="C2969" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2969">
+        <v>33</v>
+      </c>
+      <c r="E2969" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2969" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2969" s="2">
+        <v>129.46</v>
+      </c>
+    </row>
+    <row r="2970" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2970">
+        <v>4</v>
+      </c>
+      <c r="B2970">
+        <v>106</v>
+      </c>
+      <c r="C2970" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2970">
+        <v>33</v>
+      </c>
+      <c r="E2970" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2970" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2970" s="2">
+        <v>107.14</v>
+      </c>
+    </row>
+    <row r="2971" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2971">
+        <v>5</v>
+      </c>
+      <c r="B2971">
+        <v>107</v>
+      </c>
+      <c r="C2971" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2971">
+        <v>33</v>
+      </c>
+      <c r="E2971" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2971" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G2971" s="2">
+        <v>53.57</v>
+      </c>
+    </row>
+    <row r="2972" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2972">
+        <v>6</v>
+      </c>
+      <c r="B2972">
+        <v>108</v>
+      </c>
+      <c r="C2972" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2972">
+        <v>33</v>
+      </c>
+      <c r="E2972" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2972" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2972" s="2">
+        <v>107.14</v>
+      </c>
+    </row>
+    <row r="2973" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2973">
+        <v>7</v>
+      </c>
+      <c r="B2973">
+        <v>109</v>
+      </c>
+      <c r="C2973" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2973">
+        <v>33</v>
+      </c>
+      <c r="E2973" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2973" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2973" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2974" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2974">
+        <v>8</v>
+      </c>
+      <c r="B2974">
+        <v>110</v>
+      </c>
+      <c r="C2974" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2974">
+        <v>33</v>
+      </c>
+      <c r="E2974" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2974" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2974" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2975" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2975">
+        <v>9</v>
+      </c>
+      <c r="B2975">
+        <v>111</v>
+      </c>
+      <c r="C2975" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2975">
+        <v>33</v>
+      </c>
+      <c r="E2975" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2975" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2975" s="2">
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="2976" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2976">
+        <v>10</v>
+      </c>
+      <c r="B2976">
+        <v>113</v>
+      </c>
+      <c r="C2976" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2976">
+        <v>33</v>
+      </c>
+      <c r="E2976" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2976" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G2976" s="2">
+        <v>56.695</v>
+      </c>
+    </row>
+    <row r="2977" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2977">
+        <v>11</v>
+      </c>
+      <c r="B2977">
+        <v>114</v>
+      </c>
+      <c r="C2977" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2977">
+        <v>33</v>
+      </c>
+      <c r="E2977" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2977" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2977" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2978" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2978">
+        <v>12</v>
+      </c>
+      <c r="B2978">
+        <v>117</v>
+      </c>
+      <c r="C2978" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2978">
+        <v>33</v>
+      </c>
+      <c r="E2978" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2978" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2978" s="2">
+        <v>84.82</v>
+      </c>
+    </row>
+    <row r="2979" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2979">
+        <v>13</v>
+      </c>
+      <c r="B2979">
+        <v>119</v>
+      </c>
+      <c r="C2979" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2979">
+        <v>33</v>
+      </c>
+      <c r="E2979" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2979" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2979" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2980" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2980">
+        <v>14</v>
+      </c>
+      <c r="B2980">
+        <v>125</v>
+      </c>
+      <c r="C2980" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2980">
+        <v>33</v>
+      </c>
+      <c r="E2980" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2980" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2980" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2981" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2981">
+        <v>15</v>
+      </c>
+      <c r="B2981">
+        <v>126</v>
+      </c>
+      <c r="C2981" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2981">
+        <v>33</v>
+      </c>
+      <c r="E2981" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2981" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2981" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2982" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2982">
+        <v>16</v>
+      </c>
+      <c r="B2982">
+        <v>129</v>
+      </c>
+      <c r="C2982" t="s">
+        <v>132</v>
+      </c>
+      <c r="D2982">
+        <v>33</v>
+      </c>
+      <c r="E2982" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2982" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2982" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2983" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2983">
+        <v>17</v>
+      </c>
+      <c r="B2983">
+        <v>131</v>
+      </c>
+      <c r="C2983" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2983">
+        <v>33</v>
+      </c>
+      <c r="E2983" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2983" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2983" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2984" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2984">
+        <v>18</v>
+      </c>
+      <c r="B2984">
+        <v>133</v>
+      </c>
+      <c r="C2984" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2984">
+        <v>33</v>
+      </c>
+      <c r="E2984" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2984" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2984" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2985" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2985">
+        <v>19</v>
+      </c>
+      <c r="B2985">
+        <v>134</v>
+      </c>
+      <c r="C2985" t="s">
+        <v>140</v>
+      </c>
+      <c r="D2985">
+        <v>33</v>
+      </c>
+      <c r="E2985" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2985" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2985" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2986" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2986">
+        <v>20</v>
+      </c>
+      <c r="B2986">
+        <v>136</v>
+      </c>
+      <c r="C2986" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2986">
+        <v>33</v>
+      </c>
+      <c r="E2986" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2986" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2986" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2987" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2987">
+        <v>21</v>
+      </c>
+      <c r="B2987">
+        <v>141</v>
+      </c>
+      <c r="C2987" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2987">
+        <v>33</v>
+      </c>
+      <c r="E2987" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2987" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2987" s="2">
+        <v>82.14</v>
+      </c>
+    </row>
+    <row r="2988" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2988">
+        <v>22</v>
+      </c>
+      <c r="B2988">
+        <v>145</v>
+      </c>
+      <c r="C2988" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2988">
+        <v>33</v>
+      </c>
+      <c r="E2988" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2988" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2988" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2989" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2989">
+        <v>23</v>
+      </c>
+      <c r="B2989">
+        <v>147</v>
+      </c>
+      <c r="C2989" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2989">
+        <v>33</v>
+      </c>
+      <c r="E2989" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2989" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2989" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2990" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2990">
+        <v>24</v>
+      </c>
+      <c r="B2990">
+        <v>149</v>
+      </c>
+      <c r="C2990" t="s">
+        <v>158</v>
+      </c>
+      <c r="D2990">
+        <v>33</v>
+      </c>
+      <c r="E2990" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2990" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2990" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2991" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2991">
+        <v>25</v>
+      </c>
+      <c r="B2991">
+        <v>150</v>
+      </c>
+      <c r="C2991" t="s">
+        <v>161</v>
+      </c>
+      <c r="D2991">
+        <v>33</v>
+      </c>
+      <c r="E2991" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2991" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2991" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2992" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2992">
+        <v>26</v>
+      </c>
+      <c r="B2992">
+        <v>151</v>
+      </c>
+      <c r="C2992" t="s">
+        <v>164</v>
+      </c>
+      <c r="D2992">
+        <v>33</v>
+      </c>
+      <c r="E2992" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2992" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G2992" s="2">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="2993" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2993">
+        <v>27</v>
+      </c>
+      <c r="B2993">
+        <v>154</v>
+      </c>
+      <c r="C2993" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2993">
+        <v>33</v>
+      </c>
+      <c r="E2993" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2993" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2993" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2994" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2994">
+        <v>28</v>
+      </c>
+      <c r="B2994">
+        <v>160</v>
+      </c>
+      <c r="C2994" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2994">
+        <v>33</v>
+      </c>
+      <c r="E2994" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2994" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2994" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2995" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2995">
+        <v>29</v>
+      </c>
+      <c r="B2995">
+        <v>162</v>
+      </c>
+      <c r="C2995" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2995">
+        <v>33</v>
+      </c>
+      <c r="E2995" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2995" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2995" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2996" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2996">
+        <v>30</v>
+      </c>
+      <c r="B2996">
+        <v>164</v>
+      </c>
+      <c r="C2996" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2996">
+        <v>33</v>
+      </c>
+      <c r="E2996" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2996" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2996" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2997" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2997">
+        <v>31</v>
+      </c>
+      <c r="B2997">
+        <v>165</v>
+      </c>
+      <c r="C2997" t="s">
+        <v>365</v>
+      </c>
+      <c r="D2997">
+        <v>33</v>
+      </c>
+      <c r="E2997" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2997" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2997" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2998" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2998">
+        <v>32</v>
+      </c>
+      <c r="B2998">
+        <v>167</v>
+      </c>
+      <c r="C2998" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2998">
+        <v>33</v>
+      </c>
+      <c r="E2998" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2998" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2998" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2999" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2999">
+        <v>33</v>
+      </c>
+      <c r="B2999">
+        <v>175</v>
+      </c>
+      <c r="C2999" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2999">
+        <v>33</v>
+      </c>
+      <c r="E2999" t="s">
+        <v>403</v>
+      </c>
+      <c r="F2999" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2999" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3000" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3000">
+        <v>34</v>
+      </c>
+      <c r="B3000">
+        <v>181</v>
+      </c>
+      <c r="C3000" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3000">
+        <v>33</v>
+      </c>
+      <c r="E3000" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3000" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3000" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3001" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3001">
+        <v>35</v>
+      </c>
+      <c r="B3001">
+        <v>182</v>
+      </c>
+      <c r="C3001" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3001">
+        <v>33</v>
+      </c>
+      <c r="E3001" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3001" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3001" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3002" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3002">
+        <v>36</v>
+      </c>
+      <c r="B3002">
+        <v>184</v>
+      </c>
+      <c r="C3002" t="s">
+        <v>368</v>
+      </c>
+      <c r="D3002">
+        <v>33</v>
+      </c>
+      <c r="E3002" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3002" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3002" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3003" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3003">
+        <v>37</v>
+      </c>
+      <c r="B3003">
+        <v>186</v>
+      </c>
+      <c r="C3003" t="s">
+        <v>369</v>
+      </c>
+      <c r="D3003">
+        <v>33</v>
+      </c>
+      <c r="E3003" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3003" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3003" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3004" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3004">
+        <v>38</v>
+      </c>
+      <c r="B3004">
+        <v>194</v>
+      </c>
+      <c r="C3004" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3004">
+        <v>33</v>
+      </c>
+      <c r="E3004" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3004" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3004" s="2">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="3005" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3005">
+        <v>39</v>
+      </c>
+      <c r="B3005">
+        <v>199</v>
+      </c>
+      <c r="C3005" t="s">
+        <v>371</v>
+      </c>
+      <c r="D3005">
+        <v>33</v>
+      </c>
+      <c r="E3005" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3005" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3005" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3006" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3006">
+        <v>40</v>
+      </c>
+      <c r="B3006">
+        <v>200</v>
+      </c>
+      <c r="C3006" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3006">
+        <v>33</v>
+      </c>
+      <c r="E3006" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3006" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3006" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3007" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3007">
+        <v>41</v>
+      </c>
+      <c r="B3007">
+        <v>203</v>
+      </c>
+      <c r="C3007" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3007">
+        <v>33</v>
+      </c>
+      <c r="E3007" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3007" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3007" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3008" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3008">
+        <v>42</v>
+      </c>
+      <c r="B3008">
+        <v>205</v>
+      </c>
+      <c r="C3008" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3008">
+        <v>33</v>
+      </c>
+      <c r="E3008" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3008" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3008" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3009" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3009">
+        <v>43</v>
+      </c>
+      <c r="B3009">
+        <v>209</v>
+      </c>
+      <c r="C3009" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3009">
+        <v>33</v>
+      </c>
+      <c r="E3009" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3009" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3009" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3010" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3010">
+        <v>44</v>
+      </c>
+      <c r="B3010">
+        <v>212</v>
+      </c>
+      <c r="C3010" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3010">
+        <v>33</v>
+      </c>
+      <c r="E3010" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3010" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3010" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3011" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3011">
+        <v>45</v>
+      </c>
+      <c r="B3011">
+        <v>214</v>
+      </c>
+      <c r="C3011" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3011">
+        <v>33</v>
+      </c>
+      <c r="E3011" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3011" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3011" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3012" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3012">
+        <v>46</v>
+      </c>
+      <c r="B3012">
+        <v>217</v>
+      </c>
+      <c r="C3012" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3012">
+        <v>33</v>
+      </c>
+      <c r="E3012" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3012" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3012" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3013" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3013">
+        <v>47</v>
+      </c>
+      <c r="B3013">
+        <v>219</v>
+      </c>
+      <c r="C3013" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3013">
+        <v>33</v>
+      </c>
+      <c r="E3013" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3013" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3013" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3014" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3014">
+        <v>48</v>
+      </c>
+      <c r="B3014">
+        <v>222</v>
+      </c>
+      <c r="C3014" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3014">
+        <v>33</v>
+      </c>
+      <c r="E3014" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3014" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3014" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3015" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3015">
+        <v>49</v>
+      </c>
+      <c r="B3015">
+        <v>223</v>
+      </c>
+      <c r="C3015" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3015">
+        <v>33</v>
+      </c>
+      <c r="E3015" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3015" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G3015" s="2">
+        <v>271.88</v>
+      </c>
+    </row>
+    <row r="3016" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3016">
+        <v>50</v>
+      </c>
+      <c r="B3016">
+        <v>228</v>
+      </c>
+      <c r="C3016" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3016">
+        <v>33</v>
+      </c>
+      <c r="E3016" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3016" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3016" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3017" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3017">
+        <v>51</v>
+      </c>
+      <c r="B3017">
+        <v>234</v>
+      </c>
+      <c r="C3017" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3017">
+        <v>33</v>
+      </c>
+      <c r="E3017" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3017" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3017" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3018" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3018">
+        <v>52</v>
+      </c>
+      <c r="B3018">
+        <v>235</v>
+      </c>
+      <c r="C3018" t="s">
+        <v>280</v>
+      </c>
+      <c r="D3018">
+        <v>33</v>
+      </c>
+      <c r="E3018" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3018" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G3018" s="2">
+        <v>265.61500000000001</v>
+      </c>
+    </row>
+    <row r="3019" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3019">
+        <v>53</v>
+      </c>
+      <c r="B3019">
+        <v>237</v>
+      </c>
+      <c r="C3019" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3019">
+        <v>33</v>
+      </c>
+      <c r="E3019" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3019" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3019" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3020" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3020">
+        <v>54</v>
+      </c>
+      <c r="B3020">
+        <v>241</v>
+      </c>
+      <c r="C3020" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3020">
+        <v>33</v>
+      </c>
+      <c r="E3020" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3020" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3020" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3021" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3021">
+        <v>55</v>
+      </c>
+      <c r="B3021">
+        <v>243</v>
+      </c>
+      <c r="C3021" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3021">
+        <v>33</v>
+      </c>
+      <c r="E3021" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3021" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3021" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3022" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3022">
+        <v>56</v>
+      </c>
+      <c r="B3022">
+        <v>251</v>
+      </c>
+      <c r="C3022" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3022">
+        <v>33</v>
+      </c>
+      <c r="E3022" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3022" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3022" s="2">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="3023" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3023">
+        <v>57</v>
+      </c>
+      <c r="B3023">
+        <v>255</v>
+      </c>
+      <c r="C3023" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3023">
+        <v>33</v>
+      </c>
+      <c r="E3023" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3023" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3023" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3024" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3024">
+        <v>58</v>
+      </c>
+      <c r="B3024">
+        <v>258</v>
+      </c>
+      <c r="C3024" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3024">
+        <v>33</v>
+      </c>
+      <c r="E3024" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3024" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3024" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3025" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3025">
+        <v>59</v>
+      </c>
+      <c r="B3025">
+        <v>260</v>
+      </c>
+      <c r="C3025" t="s">
+        <v>351</v>
+      </c>
+      <c r="D3025">
+        <v>33</v>
+      </c>
+      <c r="E3025" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3025" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3025" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3026" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3026">
+        <v>60</v>
+      </c>
+      <c r="B3026">
+        <v>261</v>
+      </c>
+      <c r="C3026" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3026">
+        <v>33</v>
+      </c>
+      <c r="E3026" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3026" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3026" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3027" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3027">
+        <v>61</v>
+      </c>
+      <c r="B3027">
+        <v>263</v>
+      </c>
+      <c r="C3027" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3027">
+        <v>33</v>
+      </c>
+      <c r="E3027" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3027" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3027" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3028" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3028">
+        <v>62</v>
+      </c>
+      <c r="B3028">
+        <v>264</v>
+      </c>
+      <c r="C3028" t="s">
+        <v>360</v>
+      </c>
+      <c r="D3028">
+        <v>33</v>
+      </c>
+      <c r="E3028" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3028" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3028" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3029" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3029">
+        <v>63</v>
+      </c>
+      <c r="B3029">
+        <v>265</v>
+      </c>
+      <c r="C3029" t="s">
+        <v>409</v>
+      </c>
+      <c r="D3029">
+        <v>33</v>
+      </c>
+      <c r="E3029" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3029" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3029" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3030" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3030">
+        <v>64</v>
+      </c>
+      <c r="B3030">
+        <v>269</v>
+      </c>
+      <c r="C3030" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3030">
+        <v>33</v>
+      </c>
+      <c r="E3030" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3030" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3030" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3031" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3031">
+        <v>65</v>
+      </c>
+      <c r="B3031">
+        <v>301</v>
+      </c>
+      <c r="C3031" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3031">
+        <v>33</v>
+      </c>
+      <c r="E3031" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3031" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3031" s="2">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3032" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3032">
+        <v>66</v>
+      </c>
+      <c r="B3032">
+        <v>302</v>
+      </c>
+      <c r="C3032" t="s">
+        <v>363</v>
+      </c>
+      <c r="D3032">
+        <v>33</v>
+      </c>
+      <c r="E3032" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3032" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3032" s="2">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="3033" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3033">
+        <v>67</v>
+      </c>
+      <c r="B3033">
+        <v>273</v>
+      </c>
+      <c r="C3033" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3033">
+        <v>33</v>
+      </c>
+      <c r="E3033" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3033" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3033" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3034" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3034">
+        <v>68</v>
+      </c>
+      <c r="B3034">
+        <v>274</v>
+      </c>
+      <c r="C3034" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3034">
+        <v>33</v>
+      </c>
+      <c r="E3034" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3034" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3034" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3035" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3035">
+        <v>69</v>
+      </c>
+      <c r="B3035">
+        <v>275</v>
+      </c>
+      <c r="C3035" t="s">
+        <v>417</v>
+      </c>
+      <c r="D3035">
+        <v>33</v>
+      </c>
+      <c r="E3035" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3035" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3035" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3036" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3036">
+        <v>70</v>
+      </c>
+      <c r="B3036">
+        <v>277</v>
+      </c>
+      <c r="C3036" t="s">
+        <v>387</v>
+      </c>
+      <c r="D3036">
+        <v>33</v>
+      </c>
+      <c r="E3036" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3036" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3036" s="2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3037" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3037">
+        <v>71</v>
+      </c>
+      <c r="B3037">
+        <v>278</v>
+      </c>
+      <c r="C3037" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3037">
+        <v>33</v>
+      </c>
+      <c r="E3037" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3037" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3037" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3038" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3038">
+        <v>72</v>
+      </c>
+      <c r="B3038">
+        <v>279</v>
+      </c>
+      <c r="C3038" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3038">
+        <v>33</v>
+      </c>
+      <c r="E3038" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3038" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3038" s="2">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="3039" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3039">
+        <v>73</v>
+      </c>
+      <c r="B3039">
+        <v>281</v>
+      </c>
+      <c r="C3039" t="s">
+        <v>419</v>
+      </c>
+      <c r="D3039">
+        <v>33</v>
+      </c>
+      <c r="E3039" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3039" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3039" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3040" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3040">
+        <v>74</v>
+      </c>
+      <c r="B3040">
+        <v>282</v>
+      </c>
+      <c r="C3040" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3040">
+        <v>33</v>
+      </c>
+      <c r="E3040" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3040" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3040" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3041" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3041">
+        <v>75</v>
+      </c>
+      <c r="B3041">
+        <v>283</v>
+      </c>
+      <c r="C3041" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3041">
+        <v>33</v>
+      </c>
+      <c r="E3041" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3041" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3041" s="2">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3042" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3042">
+        <v>76</v>
+      </c>
+      <c r="B3042">
+        <v>284</v>
+      </c>
+      <c r="C3042" t="s">
+        <v>399</v>
+      </c>
+      <c r="D3042">
+        <v>33</v>
+      </c>
+      <c r="E3042" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3042" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3042" s="2">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3043" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3043">
+        <v>77</v>
+      </c>
+      <c r="B3043">
+        <v>286</v>
+      </c>
+      <c r="C3043" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3043">
+        <v>33</v>
+      </c>
+      <c r="E3043" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3043" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3043" s="2">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3044" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3044">
+        <v>78</v>
+      </c>
+      <c r="B3044">
+        <v>287</v>
+      </c>
+      <c r="C3044" t="s">
+        <v>421</v>
+      </c>
+      <c r="D3044">
+        <v>33</v>
+      </c>
+      <c r="E3044" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3044" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3044" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3045" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3045">
+        <v>79</v>
+      </c>
+      <c r="B3045">
+        <v>288</v>
+      </c>
+      <c r="C3045" t="s">
+        <v>422</v>
+      </c>
+      <c r="D3045">
+        <v>33</v>
+      </c>
+      <c r="E3045" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3045" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3045" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3046" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3046">
+        <v>80</v>
+      </c>
+      <c r="B3046">
+        <v>289</v>
+      </c>
+      <c r="C3046" t="s">
+        <v>423</v>
+      </c>
+      <c r="D3046">
+        <v>33</v>
+      </c>
+      <c r="E3046" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3046" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3046" s="2">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="3047" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3047">
+        <v>81</v>
+      </c>
+      <c r="B3047">
+        <v>291</v>
+      </c>
+      <c r="C3047" t="s">
+        <v>424</v>
+      </c>
+      <c r="D3047">
+        <v>33</v>
+      </c>
+      <c r="E3047" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3047" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3047" s="2">
+        <v>103.125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Hrs y Ventas Ago
</commit_message>
<xml_diff>
--- a/datasets/horas_extras_2024.xlsx
+++ b/datasets/horas_extras_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="114" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5F82959-C5C9-4A58-939D-B62DDBD84CA4}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06BA8B27-3525-42B1-885A-179A6119EA41}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7366" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7528" uniqueCount="425">
   <si>
     <t>José Guadalupe de Jesús Venegas Acosta</t>
   </si>
@@ -1384,9 +1384,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G3128" totalsRowShown="0">
-  <autoFilter ref="A1:G3128" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G3209" totalsRowShown="0">
+  <autoFilter ref="A1:G3209" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{933A802B-1DFA-4F50-A708-F8B071DB7BC5}" name="no"/>
     <tableColumn id="2" xr3:uid="{6D6E4B13-9BB4-4B8D-9AB2-9B4BC34C4362}" name="id"/>
@@ -1717,10 +1721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C5034C-9333-43F5-A544-30F944CBFAC1}">
-  <dimension ref="A1:G3128"/>
+  <dimension ref="A1:G3209"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3013" workbookViewId="0">
-      <selection activeCell="G3024" sqref="G3024"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3108" workbookViewId="0">
+      <selection activeCell="E3115" sqref="E3115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -72992,6 +72996,1869 @@
         <v>137.5</v>
       </c>
     </row>
+    <row r="3129" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3129">
+        <v>1</v>
+      </c>
+      <c r="B3129">
+        <v>101</v>
+      </c>
+      <c r="C3129" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3129">
+        <v>35</v>
+      </c>
+      <c r="E3129" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3129" s="1">
+        <v>12</v>
+      </c>
+      <c r="G3129" s="2">
+        <v>1875</v>
+      </c>
+    </row>
+    <row r="3130" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3130">
+        <v>2</v>
+      </c>
+      <c r="B3130">
+        <v>103</v>
+      </c>
+      <c r="C3130" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3130">
+        <v>35</v>
+      </c>
+      <c r="E3130" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3130" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3130" s="2">
+        <v>322.77</v>
+      </c>
+    </row>
+    <row r="3131" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3131">
+        <v>3</v>
+      </c>
+      <c r="B3131">
+        <v>104</v>
+      </c>
+      <c r="C3131" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3131">
+        <v>35</v>
+      </c>
+      <c r="E3131" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3131" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G3131" s="2">
+        <v>712.03000000000009</v>
+      </c>
+    </row>
+    <row r="3132" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3132">
+        <v>4</v>
+      </c>
+      <c r="B3132">
+        <v>106</v>
+      </c>
+      <c r="C3132" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3132">
+        <v>35</v>
+      </c>
+      <c r="E3132" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3132" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G3132" s="2">
+        <v>267.85000000000002</v>
+      </c>
+    </row>
+    <row r="3133" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3133">
+        <v>5</v>
+      </c>
+      <c r="B3133">
+        <v>107</v>
+      </c>
+      <c r="C3133" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3133">
+        <v>35</v>
+      </c>
+      <c r="E3133" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3133" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3133" s="2">
+        <v>214.28</v>
+      </c>
+    </row>
+    <row r="3134" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3134">
+        <v>6</v>
+      </c>
+      <c r="B3134">
+        <v>108</v>
+      </c>
+      <c r="C3134" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3134">
+        <v>35</v>
+      </c>
+      <c r="E3134" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3134" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3134" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3135" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3135">
+        <v>7</v>
+      </c>
+      <c r="B3135">
+        <v>109</v>
+      </c>
+      <c r="C3135" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3135">
+        <v>35</v>
+      </c>
+      <c r="E3135" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3135" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3135" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3136" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3136">
+        <v>8</v>
+      </c>
+      <c r="B3136">
+        <v>110</v>
+      </c>
+      <c r="C3136" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3136">
+        <v>35</v>
+      </c>
+      <c r="E3136" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3136" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3136" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3137" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3137">
+        <v>9</v>
+      </c>
+      <c r="B3137">
+        <v>111</v>
+      </c>
+      <c r="C3137" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3137">
+        <v>35</v>
+      </c>
+      <c r="E3137" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3137" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G3137" s="2">
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="3138" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3138">
+        <v>10</v>
+      </c>
+      <c r="B3138">
+        <v>113</v>
+      </c>
+      <c r="C3138" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3138">
+        <v>35</v>
+      </c>
+      <c r="E3138" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3138" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3138" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3139" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3139">
+        <v>11</v>
+      </c>
+      <c r="B3139">
+        <v>114</v>
+      </c>
+      <c r="C3139" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3139">
+        <v>35</v>
+      </c>
+      <c r="E3139" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3139" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3139" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3140" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3140">
+        <v>12</v>
+      </c>
+      <c r="B3140">
+        <v>117</v>
+      </c>
+      <c r="C3140" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3140">
+        <v>35</v>
+      </c>
+      <c r="E3140" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3140" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G3140" s="2">
+        <v>381.68999999999994</v>
+      </c>
+    </row>
+    <row r="3141" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3141">
+        <v>13</v>
+      </c>
+      <c r="B3141">
+        <v>119</v>
+      </c>
+      <c r="C3141" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3141">
+        <v>35</v>
+      </c>
+      <c r="E3141" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3141" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3141" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3142" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3142">
+        <v>14</v>
+      </c>
+      <c r="B3142">
+        <v>125</v>
+      </c>
+      <c r="C3142" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3142">
+        <v>35</v>
+      </c>
+      <c r="E3142" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3142" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3142" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3143" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3143">
+        <v>15</v>
+      </c>
+      <c r="B3143">
+        <v>126</v>
+      </c>
+      <c r="C3143" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3143">
+        <v>35</v>
+      </c>
+      <c r="E3143" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3143" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3143" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3144" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3144">
+        <v>16</v>
+      </c>
+      <c r="B3144">
+        <v>129</v>
+      </c>
+      <c r="C3144" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3144">
+        <v>35</v>
+      </c>
+      <c r="E3144" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3144" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3144" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3145" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3145">
+        <v>17</v>
+      </c>
+      <c r="B3145">
+        <v>131</v>
+      </c>
+      <c r="C3145" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3145">
+        <v>35</v>
+      </c>
+      <c r="E3145" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3145" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3145" s="2">
+        <v>79.459999999999994</v>
+      </c>
+    </row>
+    <row r="3146" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3146">
+        <v>18</v>
+      </c>
+      <c r="B3146">
+        <v>133</v>
+      </c>
+      <c r="C3146" t="s">
+        <v>137</v>
+      </c>
+      <c r="D3146">
+        <v>35</v>
+      </c>
+      <c r="E3146" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3146" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3146" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3147" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3147">
+        <v>19</v>
+      </c>
+      <c r="B3147">
+        <v>134</v>
+      </c>
+      <c r="C3147" t="s">
+        <v>140</v>
+      </c>
+      <c r="D3147">
+        <v>35</v>
+      </c>
+      <c r="E3147" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3147" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3147" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3148" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3148">
+        <v>20</v>
+      </c>
+      <c r="B3148">
+        <v>136</v>
+      </c>
+      <c r="C3148" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3148">
+        <v>35</v>
+      </c>
+      <c r="E3148" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3148" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3148" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3149" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3149">
+        <v>21</v>
+      </c>
+      <c r="B3149">
+        <v>141</v>
+      </c>
+      <c r="C3149" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3149">
+        <v>35</v>
+      </c>
+      <c r="E3149" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3149" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3149" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3150" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3150">
+        <v>22</v>
+      </c>
+      <c r="B3150">
+        <v>145</v>
+      </c>
+      <c r="C3150" t="s">
+        <v>152</v>
+      </c>
+      <c r="D3150">
+        <v>35</v>
+      </c>
+      <c r="E3150" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3150" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3150" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3151" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3151">
+        <v>23</v>
+      </c>
+      <c r="B3151">
+        <v>147</v>
+      </c>
+      <c r="C3151" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3151">
+        <v>35</v>
+      </c>
+      <c r="E3151" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3151" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3151" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3152" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3152">
+        <v>24</v>
+      </c>
+      <c r="B3152">
+        <v>149</v>
+      </c>
+      <c r="C3152" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3152">
+        <v>35</v>
+      </c>
+      <c r="E3152" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3152" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3152" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3153" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3153">
+        <v>25</v>
+      </c>
+      <c r="B3153">
+        <v>150</v>
+      </c>
+      <c r="C3153" t="s">
+        <v>161</v>
+      </c>
+      <c r="D3153">
+        <v>35</v>
+      </c>
+      <c r="E3153" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3153" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3153" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3154" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3154">
+        <v>26</v>
+      </c>
+      <c r="B3154">
+        <v>151</v>
+      </c>
+      <c r="C3154" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3154">
+        <v>35</v>
+      </c>
+      <c r="E3154" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3154" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3154" s="2">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3155" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3155">
+        <v>27</v>
+      </c>
+      <c r="B3155">
+        <v>154</v>
+      </c>
+      <c r="C3155" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3155">
+        <v>35</v>
+      </c>
+      <c r="E3155" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3155" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3155" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3156" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3156">
+        <v>28</v>
+      </c>
+      <c r="B3156">
+        <v>160</v>
+      </c>
+      <c r="C3156" t="s">
+        <v>364</v>
+      </c>
+      <c r="D3156">
+        <v>35</v>
+      </c>
+      <c r="E3156" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3156" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3156" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3157" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3157">
+        <v>29</v>
+      </c>
+      <c r="B3157">
+        <v>162</v>
+      </c>
+      <c r="C3157" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3157">
+        <v>35</v>
+      </c>
+      <c r="E3157" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3157" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3157" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3158" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3158">
+        <v>30</v>
+      </c>
+      <c r="B3158">
+        <v>164</v>
+      </c>
+      <c r="C3158" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3158">
+        <v>35</v>
+      </c>
+      <c r="E3158" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3158" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3158" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3159" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3159">
+        <v>31</v>
+      </c>
+      <c r="B3159">
+        <v>165</v>
+      </c>
+      <c r="C3159" t="s">
+        <v>365</v>
+      </c>
+      <c r="D3159">
+        <v>35</v>
+      </c>
+      <c r="E3159" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3159" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3159" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3160" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3160">
+        <v>32</v>
+      </c>
+      <c r="B3160">
+        <v>167</v>
+      </c>
+      <c r="C3160" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3160">
+        <v>35</v>
+      </c>
+      <c r="E3160" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3160" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3160" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3161" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3161">
+        <v>33</v>
+      </c>
+      <c r="B3161">
+        <v>175</v>
+      </c>
+      <c r="C3161" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3161">
+        <v>35</v>
+      </c>
+      <c r="E3161" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3161" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3161" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3162" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3162">
+        <v>34</v>
+      </c>
+      <c r="B3162">
+        <v>181</v>
+      </c>
+      <c r="C3162" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3162">
+        <v>35</v>
+      </c>
+      <c r="E3162" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3162" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3162" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3163" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3163">
+        <v>35</v>
+      </c>
+      <c r="B3163">
+        <v>182</v>
+      </c>
+      <c r="C3163" t="s">
+        <v>203</v>
+      </c>
+      <c r="D3163">
+        <v>35</v>
+      </c>
+      <c r="E3163" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3163" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3163" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3164" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3164">
+        <v>36</v>
+      </c>
+      <c r="B3164">
+        <v>184</v>
+      </c>
+      <c r="C3164" t="s">
+        <v>368</v>
+      </c>
+      <c r="D3164">
+        <v>35</v>
+      </c>
+      <c r="E3164" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3164" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3164" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3165" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3165">
+        <v>37</v>
+      </c>
+      <c r="B3165">
+        <v>186</v>
+      </c>
+      <c r="C3165" t="s">
+        <v>369</v>
+      </c>
+      <c r="D3165">
+        <v>35</v>
+      </c>
+      <c r="E3165" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3165" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3165" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3166" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3166">
+        <v>38</v>
+      </c>
+      <c r="B3166">
+        <v>194</v>
+      </c>
+      <c r="C3166" t="s">
+        <v>370</v>
+      </c>
+      <c r="D3166">
+        <v>35</v>
+      </c>
+      <c r="E3166" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3166" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3166" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3167" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3167">
+        <v>39</v>
+      </c>
+      <c r="B3167">
+        <v>199</v>
+      </c>
+      <c r="C3167" t="s">
+        <v>371</v>
+      </c>
+      <c r="D3167">
+        <v>35</v>
+      </c>
+      <c r="E3167" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3167" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3167" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3168" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3168">
+        <v>40</v>
+      </c>
+      <c r="B3168">
+        <v>200</v>
+      </c>
+      <c r="C3168" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3168">
+        <v>35</v>
+      </c>
+      <c r="E3168" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3168" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3168" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3169" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3169">
+        <v>41</v>
+      </c>
+      <c r="B3169">
+        <v>203</v>
+      </c>
+      <c r="C3169" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3169">
+        <v>35</v>
+      </c>
+      <c r="E3169" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3169" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3169" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3170" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3170">
+        <v>42</v>
+      </c>
+      <c r="B3170">
+        <v>205</v>
+      </c>
+      <c r="C3170" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3170">
+        <v>35</v>
+      </c>
+      <c r="E3170" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3170" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3170" s="2">
+        <v>122.32</v>
+      </c>
+    </row>
+    <row r="3171" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3171">
+        <v>43</v>
+      </c>
+      <c r="B3171">
+        <v>209</v>
+      </c>
+      <c r="C3171" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3171">
+        <v>35</v>
+      </c>
+      <c r="E3171" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3171" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3171" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3172" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3172">
+        <v>44</v>
+      </c>
+      <c r="B3172">
+        <v>212</v>
+      </c>
+      <c r="C3172" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3172">
+        <v>35</v>
+      </c>
+      <c r="E3172" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3172" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3172" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3173" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3173">
+        <v>45</v>
+      </c>
+      <c r="B3173">
+        <v>214</v>
+      </c>
+      <c r="C3173" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3173">
+        <v>35</v>
+      </c>
+      <c r="E3173" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3173" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3173" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3174" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3174">
+        <v>46</v>
+      </c>
+      <c r="B3174">
+        <v>217</v>
+      </c>
+      <c r="C3174" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3174">
+        <v>35</v>
+      </c>
+      <c r="E3174" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3174" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3174" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3175" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3175">
+        <v>47</v>
+      </c>
+      <c r="B3175">
+        <v>219</v>
+      </c>
+      <c r="C3175" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3175">
+        <v>35</v>
+      </c>
+      <c r="E3175" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3175" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3175" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3176" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3176">
+        <v>48</v>
+      </c>
+      <c r="B3176">
+        <v>222</v>
+      </c>
+      <c r="C3176" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3176">
+        <v>35</v>
+      </c>
+      <c r="E3176" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3176" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3176" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3177" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3177">
+        <v>49</v>
+      </c>
+      <c r="B3177">
+        <v>223</v>
+      </c>
+      <c r="C3177" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3177">
+        <v>35</v>
+      </c>
+      <c r="E3177" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3177" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G3177" s="2">
+        <v>349.56000000000006</v>
+      </c>
+    </row>
+    <row r="3178" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3178">
+        <v>50</v>
+      </c>
+      <c r="B3178">
+        <v>228</v>
+      </c>
+      <c r="C3178" t="s">
+        <v>267</v>
+      </c>
+      <c r="D3178">
+        <v>35</v>
+      </c>
+      <c r="E3178" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3178" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3178" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3179" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3179">
+        <v>51</v>
+      </c>
+      <c r="B3179">
+        <v>234</v>
+      </c>
+      <c r="C3179" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3179">
+        <v>35</v>
+      </c>
+      <c r="E3179" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3179" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3179" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3180" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3180">
+        <v>52</v>
+      </c>
+      <c r="B3180">
+        <v>235</v>
+      </c>
+      <c r="C3180" t="s">
+        <v>280</v>
+      </c>
+      <c r="D3180">
+        <v>35</v>
+      </c>
+      <c r="E3180" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3180" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3180" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3181" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3181">
+        <v>53</v>
+      </c>
+      <c r="B3181">
+        <v>237</v>
+      </c>
+      <c r="C3181" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3181">
+        <v>35</v>
+      </c>
+      <c r="E3181" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3181" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3181" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3182" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3182">
+        <v>54</v>
+      </c>
+      <c r="B3182">
+        <v>241</v>
+      </c>
+      <c r="C3182" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3182">
+        <v>35</v>
+      </c>
+      <c r="E3182" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3182" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3182" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3183" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3183">
+        <v>55</v>
+      </c>
+      <c r="B3183">
+        <v>243</v>
+      </c>
+      <c r="C3183" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3183">
+        <v>35</v>
+      </c>
+      <c r="E3183" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3183" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3183" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3184" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3184">
+        <v>56</v>
+      </c>
+      <c r="B3184">
+        <v>251</v>
+      </c>
+      <c r="C3184" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3184">
+        <v>35</v>
+      </c>
+      <c r="E3184" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3184" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3184" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3185" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3185">
+        <v>57</v>
+      </c>
+      <c r="B3185">
+        <v>255</v>
+      </c>
+      <c r="C3185" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3185">
+        <v>35</v>
+      </c>
+      <c r="E3185" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3185" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3185" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3186" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3186">
+        <v>58</v>
+      </c>
+      <c r="B3186">
+        <v>258</v>
+      </c>
+      <c r="C3186" t="s">
+        <v>345</v>
+      </c>
+      <c r="D3186">
+        <v>35</v>
+      </c>
+      <c r="E3186" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3186" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3186" s="2">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="3187" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3187">
+        <v>59</v>
+      </c>
+      <c r="B3187">
+        <v>260</v>
+      </c>
+      <c r="C3187" t="s">
+        <v>351</v>
+      </c>
+      <c r="D3187">
+        <v>35</v>
+      </c>
+      <c r="E3187" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3187" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3187" s="2">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="3188" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3188">
+        <v>60</v>
+      </c>
+      <c r="B3188">
+        <v>261</v>
+      </c>
+      <c r="C3188" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3188">
+        <v>35</v>
+      </c>
+      <c r="E3188" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3188" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3188" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3189" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3189">
+        <v>61</v>
+      </c>
+      <c r="B3189">
+        <v>263</v>
+      </c>
+      <c r="C3189" t="s">
+        <v>359</v>
+      </c>
+      <c r="D3189">
+        <v>35</v>
+      </c>
+      <c r="E3189" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3189" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3189" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3190" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3190">
+        <v>62</v>
+      </c>
+      <c r="B3190">
+        <v>264</v>
+      </c>
+      <c r="C3190" t="s">
+        <v>360</v>
+      </c>
+      <c r="D3190">
+        <v>35</v>
+      </c>
+      <c r="E3190" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3190" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3190" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3191" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3191">
+        <v>63</v>
+      </c>
+      <c r="B3191">
+        <v>265</v>
+      </c>
+      <c r="C3191" t="s">
+        <v>409</v>
+      </c>
+      <c r="D3191">
+        <v>35</v>
+      </c>
+      <c r="E3191" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3191" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3191" s="2">
+        <v>107.14</v>
+      </c>
+    </row>
+    <row r="3192" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3192">
+        <v>64</v>
+      </c>
+      <c r="B3192">
+        <v>269</v>
+      </c>
+      <c r="C3192" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3192">
+        <v>35</v>
+      </c>
+      <c r="E3192" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3192" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3192" s="2">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="3193" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3193">
+        <v>65</v>
+      </c>
+      <c r="B3193">
+        <v>301</v>
+      </c>
+      <c r="C3193" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3193">
+        <v>35</v>
+      </c>
+      <c r="E3193" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3193" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G3193" s="2">
+        <v>309.375</v>
+      </c>
+    </row>
+    <row r="3194" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3194">
+        <v>66</v>
+      </c>
+      <c r="B3194">
+        <v>302</v>
+      </c>
+      <c r="C3194" t="s">
+        <v>363</v>
+      </c>
+      <c r="D3194">
+        <v>35</v>
+      </c>
+      <c r="E3194" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3194" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G3194" s="2">
+        <v>378.125</v>
+      </c>
+    </row>
+    <row r="3195" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3195">
+        <v>67</v>
+      </c>
+      <c r="B3195">
+        <v>273</v>
+      </c>
+      <c r="C3195" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3195">
+        <v>35</v>
+      </c>
+      <c r="E3195" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3195" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3195" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3196" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3196">
+        <v>68</v>
+      </c>
+      <c r="B3196">
+        <v>274</v>
+      </c>
+      <c r="C3196" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3196">
+        <v>35</v>
+      </c>
+      <c r="E3196" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3196" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3196" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3197" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3197">
+        <v>69</v>
+      </c>
+      <c r="B3197">
+        <v>275</v>
+      </c>
+      <c r="C3197" t="s">
+        <v>417</v>
+      </c>
+      <c r="D3197">
+        <v>35</v>
+      </c>
+      <c r="E3197" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3197" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3197" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3198" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3198">
+        <v>70</v>
+      </c>
+      <c r="B3198">
+        <v>277</v>
+      </c>
+      <c r="C3198" t="s">
+        <v>387</v>
+      </c>
+      <c r="D3198">
+        <v>35</v>
+      </c>
+      <c r="E3198" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3198" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G3198" s="2">
+        <v>218.75</v>
+      </c>
+    </row>
+    <row r="3199" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3199">
+        <v>71</v>
+      </c>
+      <c r="B3199">
+        <v>278</v>
+      </c>
+      <c r="C3199" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3199">
+        <v>35</v>
+      </c>
+      <c r="E3199" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3199" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3199" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3200" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3200">
+        <v>72</v>
+      </c>
+      <c r="B3200">
+        <v>279</v>
+      </c>
+      <c r="C3200" t="s">
+        <v>418</v>
+      </c>
+      <c r="D3200">
+        <v>35</v>
+      </c>
+      <c r="E3200" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3200" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3200" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3201" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3201">
+        <v>73</v>
+      </c>
+      <c r="B3201">
+        <v>281</v>
+      </c>
+      <c r="C3201" t="s">
+        <v>419</v>
+      </c>
+      <c r="D3201">
+        <v>35</v>
+      </c>
+      <c r="E3201" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3201" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3201" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3202" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3202">
+        <v>74</v>
+      </c>
+      <c r="B3202">
+        <v>282</v>
+      </c>
+      <c r="C3202" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3202">
+        <v>35</v>
+      </c>
+      <c r="E3202" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3202" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3202" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3203" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3203">
+        <v>75</v>
+      </c>
+      <c r="B3203">
+        <v>283</v>
+      </c>
+      <c r="C3203" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3203">
+        <v>35</v>
+      </c>
+      <c r="E3203" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3203" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G3203" s="2">
+        <v>309.375</v>
+      </c>
+    </row>
+    <row r="3204" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3204">
+        <v>76</v>
+      </c>
+      <c r="B3204">
+        <v>284</v>
+      </c>
+      <c r="C3204" t="s">
+        <v>399</v>
+      </c>
+      <c r="D3204">
+        <v>35</v>
+      </c>
+      <c r="E3204" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3204" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3204" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3205" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3205">
+        <v>77</v>
+      </c>
+      <c r="B3205">
+        <v>286</v>
+      </c>
+      <c r="C3205" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3205">
+        <v>35</v>
+      </c>
+      <c r="E3205" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3205" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G3205" s="2">
+        <v>240.625</v>
+      </c>
+    </row>
+    <row r="3206" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3206">
+        <v>78</v>
+      </c>
+      <c r="B3206">
+        <v>287</v>
+      </c>
+      <c r="C3206" t="s">
+        <v>421</v>
+      </c>
+      <c r="D3206">
+        <v>35</v>
+      </c>
+      <c r="E3206" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3206" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3206" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3207" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3207">
+        <v>79</v>
+      </c>
+      <c r="B3207">
+        <v>288</v>
+      </c>
+      <c r="C3207" t="s">
+        <v>422</v>
+      </c>
+      <c r="D3207">
+        <v>35</v>
+      </c>
+      <c r="E3207" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3207" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3207" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3208" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3208">
+        <v>80</v>
+      </c>
+      <c r="B3208">
+        <v>289</v>
+      </c>
+      <c r="C3208" t="s">
+        <v>423</v>
+      </c>
+      <c r="D3208">
+        <v>35</v>
+      </c>
+      <c r="E3208" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3208" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G3208" s="2">
+        <v>309.375</v>
+      </c>
+    </row>
+    <row r="3209" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3209">
+        <v>81</v>
+      </c>
+      <c r="B3209">
+        <v>291</v>
+      </c>
+      <c r="C3209" t="s">
+        <v>424</v>
+      </c>
+      <c r="D3209">
+        <v>35</v>
+      </c>
+      <c r="E3209" t="s">
+        <v>403</v>
+      </c>
+      <c r="F3209" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3209" s="2">
+        <v>137.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
corr hrs y prod
</commit_message>
<xml_diff>
--- a/datasets/horas_extras_2024.xlsx
+++ b/datasets/horas_extras_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{021253FD-1A91-4B4B-995F-5B98AE6D2B87}"/>
+  <xr:revisionPtr revIDLastSave="125" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F81BA433-E8C5-45D9-B65A-715E83F5B8A7}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
   </bookViews>
@@ -1738,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C5034C-9333-43F5-A544-30F944CBFAC1}">
   <dimension ref="A1:G3598"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3437" workbookViewId="0">
-      <selection activeCell="F3451" sqref="F3451"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Hrs Extras Sem 46
</commit_message>
<xml_diff>
--- a/datasets/horas_extras_2024.xlsx
+++ b/datasets/horas_extras_2024.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/275e1cc0366b6475/Documentos/Vori Vost/Pruebas-Boton/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="153" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18CE9735-E8A5-49D4-BEFD-A1F451911D4D}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{1A004CC6-3AB4-446C-BD2B-0C06F8A450D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3751547A-01EF-42E1-89DA-C29F261181C3}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8D2FABD6-4747-4576-90FC-0D93F347ACDD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8536" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8767" uniqueCount="473">
   <si>
     <t>José Guadalupe de Jesús Venegas Acosta</t>
   </si>
@@ -1444,6 +1444,18 @@
   <si>
     <t>LUIS ANGEL  AYALA AYALA</t>
   </si>
+  <si>
+    <t>JUAN LUIS LUNA AVILA</t>
+  </si>
+  <si>
+    <t>CRISTOFER LLAIR FRAGA</t>
+  </si>
+  <si>
+    <t>MARVIN MARTÍN LOPEZ MUÑOZ</t>
+  </si>
+  <si>
+    <t>ESAU GUIJOSA</t>
+  </si>
 </sst>
 </file>
 
@@ -1533,8 +1545,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G3827" totalsRowShown="0">
-  <autoFilter ref="A1:G3827" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}" name="Tabla1" displayName="Tabla1" ref="A1:G4058" totalsRowShown="0">
+  <autoFilter ref="A1:G4058" xr:uid="{CFB3B8A5-3C81-4841-BC07-B3CB2FEB34F2}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{933A802B-1DFA-4F50-A708-F8B071DB7BC5}" name="no"/>
     <tableColumn id="2" xr3:uid="{6D6E4B13-9BB4-4B8D-9AB2-9B4BC34C4362}" name="id"/>
@@ -1865,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65C5034C-9333-43F5-A544-30F944CBFAC1}">
-  <dimension ref="A1:G3827"/>
+  <dimension ref="A1:G4058"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3694" workbookViewId="0">
-      <selection activeCell="D3827" sqref="D3827"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4037" workbookViewId="0">
+      <selection activeCell="E4046" sqref="E4046"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -88520,6 +88532,4626 @@
         <v>206.25</v>
       </c>
     </row>
+    <row r="3828" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3828">
+        <v>1</v>
+      </c>
+      <c r="B3828">
+        <v>101</v>
+      </c>
+      <c r="C3828" t="s">
+        <v>427</v>
+      </c>
+      <c r="D3828">
+        <v>44</v>
+      </c>
+      <c r="F3828" s="1">
+        <v>15.5</v>
+      </c>
+      <c r="G3828" s="4">
+        <v>2421.875</v>
+      </c>
+    </row>
+    <row r="3829" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3829">
+        <v>2</v>
+      </c>
+      <c r="B3829">
+        <v>103</v>
+      </c>
+      <c r="C3829" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3829">
+        <v>44</v>
+      </c>
+      <c r="F3829" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3829" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3830" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3830">
+        <v>3</v>
+      </c>
+      <c r="B3830">
+        <v>104</v>
+      </c>
+      <c r="C3830" t="s">
+        <v>429</v>
+      </c>
+      <c r="D3830">
+        <v>44</v>
+      </c>
+      <c r="F3830" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3830" s="4">
+        <v>129.46</v>
+      </c>
+    </row>
+    <row r="3831" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3831">
+        <v>4</v>
+      </c>
+      <c r="B3831">
+        <v>106</v>
+      </c>
+      <c r="C3831" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3831">
+        <v>44</v>
+      </c>
+      <c r="F3831" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="G3831" s="4">
+        <v>482.13</v>
+      </c>
+    </row>
+    <row r="3832" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3832">
+        <v>5</v>
+      </c>
+      <c r="B3832">
+        <v>107</v>
+      </c>
+      <c r="C3832" t="s">
+        <v>430</v>
+      </c>
+      <c r="D3832">
+        <v>44</v>
+      </c>
+      <c r="F3832" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3832" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3833" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3833">
+        <v>6</v>
+      </c>
+      <c r="B3833">
+        <v>108</v>
+      </c>
+      <c r="C3833" t="s">
+        <v>431</v>
+      </c>
+      <c r="D3833">
+        <v>44</v>
+      </c>
+      <c r="F3833" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3833" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3834" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3834">
+        <v>7</v>
+      </c>
+      <c r="B3834">
+        <v>109</v>
+      </c>
+      <c r="C3834" t="s">
+        <v>432</v>
+      </c>
+      <c r="D3834">
+        <v>44</v>
+      </c>
+      <c r="F3834" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="G3834" s="4">
+        <v>1017.83</v>
+      </c>
+    </row>
+    <row r="3835" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3835">
+        <v>8</v>
+      </c>
+      <c r="B3835">
+        <v>110</v>
+      </c>
+      <c r="C3835" t="s">
+        <v>433</v>
+      </c>
+      <c r="D3835">
+        <v>44</v>
+      </c>
+      <c r="F3835" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3835" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3836" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3836">
+        <v>9</v>
+      </c>
+      <c r="B3836">
+        <v>111</v>
+      </c>
+      <c r="C3836" t="s">
+        <v>434</v>
+      </c>
+      <c r="D3836">
+        <v>44</v>
+      </c>
+      <c r="F3836" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3836" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3837" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3837">
+        <v>10</v>
+      </c>
+      <c r="B3837">
+        <v>113</v>
+      </c>
+      <c r="C3837" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3837">
+        <v>44</v>
+      </c>
+      <c r="F3837" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G3837" s="4">
+        <v>283.47500000000002</v>
+      </c>
+    </row>
+    <row r="3838" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3838">
+        <v>11</v>
+      </c>
+      <c r="B3838">
+        <v>114</v>
+      </c>
+      <c r="C3838" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3838">
+        <v>44</v>
+      </c>
+      <c r="F3838" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3838" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3839" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3839">
+        <v>12</v>
+      </c>
+      <c r="B3839">
+        <v>117</v>
+      </c>
+      <c r="C3839" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3839">
+        <v>44</v>
+      </c>
+      <c r="F3839" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3839" s="4">
+        <v>424.09999999999997</v>
+      </c>
+    </row>
+    <row r="3840" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3840">
+        <v>13</v>
+      </c>
+      <c r="B3840">
+        <v>119</v>
+      </c>
+      <c r="C3840" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3840">
+        <v>44</v>
+      </c>
+      <c r="F3840" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3840" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3841" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3841">
+        <v>14</v>
+      </c>
+      <c r="B3841">
+        <v>125</v>
+      </c>
+      <c r="C3841" t="s">
+        <v>437</v>
+      </c>
+      <c r="D3841">
+        <v>44</v>
+      </c>
+      <c r="F3841" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3841" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3842" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3842">
+        <v>15</v>
+      </c>
+      <c r="B3842">
+        <v>126</v>
+      </c>
+      <c r="C3842" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3842">
+        <v>44</v>
+      </c>
+      <c r="F3842" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3842" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3843" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3843">
+        <v>16</v>
+      </c>
+      <c r="B3843">
+        <v>129</v>
+      </c>
+      <c r="C3843" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3843">
+        <v>44</v>
+      </c>
+      <c r="F3843" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3843" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3844" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3844">
+        <v>17</v>
+      </c>
+      <c r="B3844">
+        <v>131</v>
+      </c>
+      <c r="C3844" t="s">
+        <v>438</v>
+      </c>
+      <c r="D3844">
+        <v>44</v>
+      </c>
+      <c r="F3844" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3844" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3845" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3845">
+        <v>18</v>
+      </c>
+      <c r="B3845">
+        <v>133</v>
+      </c>
+      <c r="C3845" t="s">
+        <v>439</v>
+      </c>
+      <c r="D3845">
+        <v>44</v>
+      </c>
+      <c r="F3845" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3845" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3846" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3846">
+        <v>19</v>
+      </c>
+      <c r="B3846">
+        <v>136</v>
+      </c>
+      <c r="C3846" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3846">
+        <v>44</v>
+      </c>
+      <c r="F3846" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3846" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3847" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3847">
+        <v>20</v>
+      </c>
+      <c r="B3847">
+        <v>141</v>
+      </c>
+      <c r="C3847" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3847">
+        <v>44</v>
+      </c>
+      <c r="F3847" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3847" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3848" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3848">
+        <v>21</v>
+      </c>
+      <c r="B3848">
+        <v>145</v>
+      </c>
+      <c r="C3848" t="s">
+        <v>440</v>
+      </c>
+      <c r="D3848">
+        <v>44</v>
+      </c>
+      <c r="F3848" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3848" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3849" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3849">
+        <v>22</v>
+      </c>
+      <c r="B3849">
+        <v>147</v>
+      </c>
+      <c r="C3849" t="s">
+        <v>441</v>
+      </c>
+      <c r="D3849">
+        <v>44</v>
+      </c>
+      <c r="F3849" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3849" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3850" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3850">
+        <v>23</v>
+      </c>
+      <c r="B3850">
+        <v>149</v>
+      </c>
+      <c r="C3850" t="s">
+        <v>442</v>
+      </c>
+      <c r="D3850">
+        <v>44</v>
+      </c>
+      <c r="F3850" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3850" s="4">
+        <v>142.86000000000001</v>
+      </c>
+    </row>
+    <row r="3851" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3851">
+        <v>24</v>
+      </c>
+      <c r="B3851">
+        <v>150</v>
+      </c>
+      <c r="C3851" t="s">
+        <v>443</v>
+      </c>
+      <c r="D3851">
+        <v>44</v>
+      </c>
+      <c r="F3851" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3851" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3852" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3852">
+        <v>25</v>
+      </c>
+      <c r="B3852">
+        <v>151</v>
+      </c>
+      <c r="C3852" t="s">
+        <v>444</v>
+      </c>
+      <c r="D3852">
+        <v>44</v>
+      </c>
+      <c r="F3852" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3852" s="4">
+        <v>206.25</v>
+      </c>
+    </row>
+    <row r="3853" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3853">
+        <v>26</v>
+      </c>
+      <c r="B3853">
+        <v>154</v>
+      </c>
+      <c r="C3853" t="s">
+        <v>445</v>
+      </c>
+      <c r="D3853">
+        <v>44</v>
+      </c>
+      <c r="F3853" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3853" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3854" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3854">
+        <v>27</v>
+      </c>
+      <c r="B3854">
+        <v>160</v>
+      </c>
+      <c r="C3854" t="s">
+        <v>446</v>
+      </c>
+      <c r="D3854">
+        <v>44</v>
+      </c>
+      <c r="F3854" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3854" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3855" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3855">
+        <v>28</v>
+      </c>
+      <c r="B3855">
+        <v>162</v>
+      </c>
+      <c r="C3855" t="s">
+        <v>447</v>
+      </c>
+      <c r="D3855">
+        <v>44</v>
+      </c>
+      <c r="F3855" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G3855" s="4">
+        <v>271.88</v>
+      </c>
+    </row>
+    <row r="3856" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3856">
+        <v>29</v>
+      </c>
+      <c r="B3856">
+        <v>164</v>
+      </c>
+      <c r="C3856" t="s">
+        <v>448</v>
+      </c>
+      <c r="D3856">
+        <v>44</v>
+      </c>
+      <c r="F3856" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3856" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3857" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3857">
+        <v>30</v>
+      </c>
+      <c r="B3857">
+        <v>165</v>
+      </c>
+      <c r="C3857" t="s">
+        <v>449</v>
+      </c>
+      <c r="D3857">
+        <v>44</v>
+      </c>
+      <c r="F3857" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3857" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3858" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3858">
+        <v>31</v>
+      </c>
+      <c r="B3858">
+        <v>167</v>
+      </c>
+      <c r="C3858" t="s">
+        <v>450</v>
+      </c>
+      <c r="D3858">
+        <v>44</v>
+      </c>
+      <c r="F3858" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3858" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3859" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3859">
+        <v>32</v>
+      </c>
+      <c r="B3859">
+        <v>175</v>
+      </c>
+      <c r="C3859" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3859">
+        <v>44</v>
+      </c>
+      <c r="F3859" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3859" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3860" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3860">
+        <v>33</v>
+      </c>
+      <c r="B3860">
+        <v>181</v>
+      </c>
+      <c r="C3860" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3860">
+        <v>44</v>
+      </c>
+      <c r="F3860" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3860" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3861" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3861">
+        <v>34</v>
+      </c>
+      <c r="B3861">
+        <v>186</v>
+      </c>
+      <c r="C3861" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3861">
+        <v>44</v>
+      </c>
+      <c r="F3861" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3861" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3862" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3862">
+        <v>35</v>
+      </c>
+      <c r="B3862">
+        <v>192</v>
+      </c>
+      <c r="C3862" t="s">
+        <v>425</v>
+      </c>
+      <c r="D3862">
+        <v>44</v>
+      </c>
+      <c r="F3862" s="1">
+        <v>22.5</v>
+      </c>
+      <c r="G3862" s="4">
+        <v>1687.5</v>
+      </c>
+    </row>
+    <row r="3863" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3863">
+        <v>36</v>
+      </c>
+      <c r="B3863">
+        <v>194</v>
+      </c>
+      <c r="C3863" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3863">
+        <v>44</v>
+      </c>
+      <c r="F3863" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3863" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3864" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3864">
+        <v>37</v>
+      </c>
+      <c r="B3864">
+        <v>200</v>
+      </c>
+      <c r="C3864" t="s">
+        <v>451</v>
+      </c>
+      <c r="D3864">
+        <v>44</v>
+      </c>
+      <c r="F3864" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3864" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3865" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3865">
+        <v>38</v>
+      </c>
+      <c r="B3865">
+        <v>203</v>
+      </c>
+      <c r="C3865" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3865">
+        <v>44</v>
+      </c>
+      <c r="F3865" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="G3865" s="4">
+        <v>240.625</v>
+      </c>
+    </row>
+    <row r="3866" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3866">
+        <v>39</v>
+      </c>
+      <c r="B3866">
+        <v>205</v>
+      </c>
+      <c r="C3866" t="s">
+        <v>452</v>
+      </c>
+      <c r="D3866">
+        <v>44</v>
+      </c>
+      <c r="F3866" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3866" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3867" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3867">
+        <v>40</v>
+      </c>
+      <c r="B3867">
+        <v>209</v>
+      </c>
+      <c r="C3867" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3867">
+        <v>44</v>
+      </c>
+      <c r="F3867" s="1">
+        <v>7</v>
+      </c>
+      <c r="G3867" s="4">
+        <v>481.25</v>
+      </c>
+    </row>
+    <row r="3868" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3868">
+        <v>41</v>
+      </c>
+      <c r="B3868">
+        <v>212</v>
+      </c>
+      <c r="C3868" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3868">
+        <v>44</v>
+      </c>
+      <c r="F3868" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3868" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3869" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3869">
+        <v>42</v>
+      </c>
+      <c r="B3869">
+        <v>214</v>
+      </c>
+      <c r="C3869" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3869">
+        <v>44</v>
+      </c>
+      <c r="F3869" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3869" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3870" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3870">
+        <v>43</v>
+      </c>
+      <c r="B3870">
+        <v>217</v>
+      </c>
+      <c r="C3870" t="s">
+        <v>453</v>
+      </c>
+      <c r="D3870">
+        <v>44</v>
+      </c>
+      <c r="F3870" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3870" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3871" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3871">
+        <v>44</v>
+      </c>
+      <c r="B3871">
+        <v>222</v>
+      </c>
+      <c r="C3871" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3871">
+        <v>44</v>
+      </c>
+      <c r="F3871" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="G3871" s="4">
+        <v>622.80000000000007</v>
+      </c>
+    </row>
+    <row r="3872" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3872">
+        <v>45</v>
+      </c>
+      <c r="B3872">
+        <v>223</v>
+      </c>
+      <c r="C3872" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3872">
+        <v>44</v>
+      </c>
+      <c r="F3872" s="1">
+        <v>21</v>
+      </c>
+      <c r="G3872" s="4">
+        <v>1631.2800000000002</v>
+      </c>
+    </row>
+    <row r="3873" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3873">
+        <v>46</v>
+      </c>
+      <c r="B3873">
+        <v>228</v>
+      </c>
+      <c r="C3873" t="s">
+        <v>455</v>
+      </c>
+      <c r="D3873">
+        <v>44</v>
+      </c>
+      <c r="F3873" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3873" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3874" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3874">
+        <v>47</v>
+      </c>
+      <c r="B3874">
+        <v>234</v>
+      </c>
+      <c r="C3874" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3874">
+        <v>44</v>
+      </c>
+      <c r="F3874" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3874" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3875" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3875">
+        <v>48</v>
+      </c>
+      <c r="B3875">
+        <v>237</v>
+      </c>
+      <c r="C3875" t="s">
+        <v>456</v>
+      </c>
+      <c r="D3875">
+        <v>44</v>
+      </c>
+      <c r="F3875" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3875" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3876" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3876">
+        <v>49</v>
+      </c>
+      <c r="B3876">
+        <v>241</v>
+      </c>
+      <c r="C3876" t="s">
+        <v>457</v>
+      </c>
+      <c r="D3876">
+        <v>44</v>
+      </c>
+      <c r="F3876" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3876" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3877" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3877">
+        <v>50</v>
+      </c>
+      <c r="B3877">
+        <v>251</v>
+      </c>
+      <c r="C3877" t="s">
+        <v>458</v>
+      </c>
+      <c r="D3877">
+        <v>44</v>
+      </c>
+      <c r="F3877" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3877" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3878" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3878">
+        <v>51</v>
+      </c>
+      <c r="B3878">
+        <v>255</v>
+      </c>
+      <c r="C3878" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3878">
+        <v>44</v>
+      </c>
+      <c r="F3878" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3878" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3879" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3879">
+        <v>52</v>
+      </c>
+      <c r="B3879">
+        <v>260</v>
+      </c>
+      <c r="C3879" t="s">
+        <v>460</v>
+      </c>
+      <c r="D3879">
+        <v>44</v>
+      </c>
+      <c r="F3879" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3879" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3880" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3880">
+        <v>53</v>
+      </c>
+      <c r="B3880">
+        <v>261</v>
+      </c>
+      <c r="C3880" t="s">
+        <v>461</v>
+      </c>
+      <c r="D3880">
+        <v>44</v>
+      </c>
+      <c r="F3880" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3880" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3881" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3881">
+        <v>54</v>
+      </c>
+      <c r="B3881">
+        <v>263</v>
+      </c>
+      <c r="C3881" t="s">
+        <v>462</v>
+      </c>
+      <c r="D3881">
+        <v>44</v>
+      </c>
+      <c r="F3881" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3881" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3882" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3882">
+        <v>55</v>
+      </c>
+      <c r="B3882">
+        <v>264</v>
+      </c>
+      <c r="C3882" t="s">
+        <v>360</v>
+      </c>
+      <c r="D3882">
+        <v>44</v>
+      </c>
+      <c r="F3882" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3882" s="4">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3883" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3883">
+        <v>56</v>
+      </c>
+      <c r="B3883">
+        <v>265</v>
+      </c>
+      <c r="C3883" t="s">
+        <v>463</v>
+      </c>
+      <c r="D3883">
+        <v>44</v>
+      </c>
+      <c r="F3883" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3883" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3884" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3884">
+        <v>57</v>
+      </c>
+      <c r="B3884">
+        <v>269</v>
+      </c>
+      <c r="C3884" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3884">
+        <v>44</v>
+      </c>
+      <c r="F3884" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3884" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3885" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3885">
+        <v>58</v>
+      </c>
+      <c r="B3885">
+        <v>273</v>
+      </c>
+      <c r="C3885" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3885">
+        <v>44</v>
+      </c>
+      <c r="F3885" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3885" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3886" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3886">
+        <v>59</v>
+      </c>
+      <c r="B3886">
+        <v>274</v>
+      </c>
+      <c r="C3886" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3886">
+        <v>44</v>
+      </c>
+      <c r="F3886" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3886" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3887" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3887">
+        <v>60</v>
+      </c>
+      <c r="B3887">
+        <v>275</v>
+      </c>
+      <c r="C3887" t="s">
+        <v>385</v>
+      </c>
+      <c r="D3887">
+        <v>44</v>
+      </c>
+      <c r="F3887" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3887" s="4">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3888" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3888">
+        <v>61</v>
+      </c>
+      <c r="B3888">
+        <v>277</v>
+      </c>
+      <c r="C3888" t="s">
+        <v>387</v>
+      </c>
+      <c r="D3888">
+        <v>44</v>
+      </c>
+      <c r="F3888" s="1">
+        <v>14</v>
+      </c>
+      <c r="G3888" s="4">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="3889" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3889">
+        <v>62</v>
+      </c>
+      <c r="B3889">
+        <v>278</v>
+      </c>
+      <c r="C3889" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3889">
+        <v>44</v>
+      </c>
+      <c r="F3889" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3889" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3890" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3890">
+        <v>63</v>
+      </c>
+      <c r="B3890">
+        <v>279</v>
+      </c>
+      <c r="C3890" t="s">
+        <v>389</v>
+      </c>
+      <c r="D3890">
+        <v>44</v>
+      </c>
+      <c r="F3890" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3890" s="4">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="3891" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3891">
+        <v>64</v>
+      </c>
+      <c r="B3891">
+        <v>281</v>
+      </c>
+      <c r="C3891" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3891">
+        <v>44</v>
+      </c>
+      <c r="F3891" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3891" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3892" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3892">
+        <v>65</v>
+      </c>
+      <c r="B3892">
+        <v>282</v>
+      </c>
+      <c r="C3892" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3892">
+        <v>44</v>
+      </c>
+      <c r="F3892" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3892" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3893" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3893">
+        <v>66</v>
+      </c>
+      <c r="B3893">
+        <v>283</v>
+      </c>
+      <c r="C3893" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3893">
+        <v>44</v>
+      </c>
+      <c r="F3893" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3893" s="4">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3894" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3894">
+        <v>67</v>
+      </c>
+      <c r="B3894">
+        <v>284</v>
+      </c>
+      <c r="C3894" t="s">
+        <v>465</v>
+      </c>
+      <c r="D3894">
+        <v>44</v>
+      </c>
+      <c r="F3894" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3894" s="4">
+        <v>343.75</v>
+      </c>
+    </row>
+    <row r="3895" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3895">
+        <v>68</v>
+      </c>
+      <c r="B3895">
+        <v>286</v>
+      </c>
+      <c r="C3895" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3895">
+        <v>44</v>
+      </c>
+      <c r="F3895" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3895" s="4">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3896" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3896">
+        <v>69</v>
+      </c>
+      <c r="B3896">
+        <v>288</v>
+      </c>
+      <c r="C3896" t="s">
+        <v>466</v>
+      </c>
+      <c r="D3896">
+        <v>44</v>
+      </c>
+      <c r="F3896" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3896" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3897" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3897">
+        <v>70</v>
+      </c>
+      <c r="B3897">
+        <v>289</v>
+      </c>
+      <c r="C3897" t="s">
+        <v>423</v>
+      </c>
+      <c r="D3897">
+        <v>44</v>
+      </c>
+      <c r="F3897" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3897" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3898" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3898">
+        <v>71</v>
+      </c>
+      <c r="B3898">
+        <v>291</v>
+      </c>
+      <c r="C3898" t="s">
+        <v>424</v>
+      </c>
+      <c r="D3898">
+        <v>44</v>
+      </c>
+      <c r="F3898" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3898" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3899" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3899">
+        <v>72</v>
+      </c>
+      <c r="B3899">
+        <v>293</v>
+      </c>
+      <c r="C3899" t="s">
+        <v>426</v>
+      </c>
+      <c r="D3899">
+        <v>44</v>
+      </c>
+      <c r="F3899" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3899" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3900" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3900">
+        <v>73</v>
+      </c>
+      <c r="B3900">
+        <v>294</v>
+      </c>
+      <c r="C3900" t="s">
+        <v>467</v>
+      </c>
+      <c r="D3900">
+        <v>44</v>
+      </c>
+      <c r="F3900" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3900" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3901" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3901">
+        <v>74</v>
+      </c>
+      <c r="B3901">
+        <v>295</v>
+      </c>
+      <c r="C3901" t="s">
+        <v>468</v>
+      </c>
+      <c r="D3901">
+        <v>44</v>
+      </c>
+      <c r="F3901" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3901" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3902" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3902">
+        <v>75</v>
+      </c>
+      <c r="B3902">
+        <v>301</v>
+      </c>
+      <c r="C3902" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3902">
+        <v>44</v>
+      </c>
+      <c r="F3902" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3902" s="4">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3903" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3903">
+        <v>76</v>
+      </c>
+      <c r="B3903">
+        <v>302</v>
+      </c>
+      <c r="C3903" t="s">
+        <v>363</v>
+      </c>
+      <c r="D3903">
+        <v>44</v>
+      </c>
+      <c r="F3903" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3903" s="4">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="3904" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3904">
+        <v>1</v>
+      </c>
+      <c r="B3904">
+        <v>101</v>
+      </c>
+      <c r="C3904" t="s">
+        <v>427</v>
+      </c>
+      <c r="D3904">
+        <v>45</v>
+      </c>
+      <c r="F3904" s="1">
+        <v>18</v>
+      </c>
+      <c r="G3904" s="4">
+        <v>2812.5</v>
+      </c>
+    </row>
+    <row r="3905" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3905">
+        <v>2</v>
+      </c>
+      <c r="B3905">
+        <v>103</v>
+      </c>
+      <c r="C3905" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3905">
+        <v>45</v>
+      </c>
+      <c r="F3905" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3905" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3906" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3906">
+        <v>3</v>
+      </c>
+      <c r="B3906">
+        <v>104</v>
+      </c>
+      <c r="C3906" t="s">
+        <v>429</v>
+      </c>
+      <c r="D3906">
+        <v>45</v>
+      </c>
+      <c r="F3906" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3906" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3907" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3907">
+        <v>4</v>
+      </c>
+      <c r="B3907">
+        <v>106</v>
+      </c>
+      <c r="C3907" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3907">
+        <v>45</v>
+      </c>
+      <c r="F3907" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3907" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3908" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3908">
+        <v>5</v>
+      </c>
+      <c r="B3908">
+        <v>107</v>
+      </c>
+      <c r="C3908" t="s">
+        <v>430</v>
+      </c>
+      <c r="D3908">
+        <v>45</v>
+      </c>
+      <c r="F3908" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3908" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3909" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3909">
+        <v>6</v>
+      </c>
+      <c r="B3909">
+        <v>108</v>
+      </c>
+      <c r="C3909" t="s">
+        <v>431</v>
+      </c>
+      <c r="D3909">
+        <v>45</v>
+      </c>
+      <c r="F3909" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3909" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3910" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3910">
+        <v>7</v>
+      </c>
+      <c r="B3910">
+        <v>109</v>
+      </c>
+      <c r="C3910" t="s">
+        <v>432</v>
+      </c>
+      <c r="D3910">
+        <v>45</v>
+      </c>
+      <c r="F3910" s="1">
+        <v>11</v>
+      </c>
+      <c r="G3910" s="4">
+        <v>1178.54</v>
+      </c>
+    </row>
+    <row r="3911" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3911">
+        <v>8</v>
+      </c>
+      <c r="B3911">
+        <v>110</v>
+      </c>
+      <c r="C3911" t="s">
+        <v>433</v>
+      </c>
+      <c r="D3911">
+        <v>45</v>
+      </c>
+      <c r="F3911" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3911" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3912" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3912">
+        <v>9</v>
+      </c>
+      <c r="B3912">
+        <v>111</v>
+      </c>
+      <c r="C3912" t="s">
+        <v>434</v>
+      </c>
+      <c r="D3912">
+        <v>45</v>
+      </c>
+      <c r="F3912" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3912" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3913" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3913">
+        <v>10</v>
+      </c>
+      <c r="B3913">
+        <v>113</v>
+      </c>
+      <c r="C3913" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3913">
+        <v>45</v>
+      </c>
+      <c r="F3913" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3913" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3914" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3914">
+        <v>11</v>
+      </c>
+      <c r="B3914">
+        <v>114</v>
+      </c>
+      <c r="C3914" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3914">
+        <v>45</v>
+      </c>
+      <c r="F3914" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3914" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3915" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3915">
+        <v>12</v>
+      </c>
+      <c r="B3915">
+        <v>117</v>
+      </c>
+      <c r="C3915" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3915">
+        <v>45</v>
+      </c>
+      <c r="F3915" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3915" s="4">
+        <v>254.45999999999998</v>
+      </c>
+    </row>
+    <row r="3916" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3916">
+        <v>13</v>
+      </c>
+      <c r="B3916">
+        <v>119</v>
+      </c>
+      <c r="C3916" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3916">
+        <v>45</v>
+      </c>
+      <c r="F3916" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3916" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3917" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3917">
+        <v>14</v>
+      </c>
+      <c r="B3917">
+        <v>125</v>
+      </c>
+      <c r="C3917" t="s">
+        <v>437</v>
+      </c>
+      <c r="D3917">
+        <v>45</v>
+      </c>
+      <c r="F3917" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3917" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3918" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3918">
+        <v>15</v>
+      </c>
+      <c r="B3918">
+        <v>126</v>
+      </c>
+      <c r="C3918" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3918">
+        <v>45</v>
+      </c>
+      <c r="F3918" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3918" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3919" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3919">
+        <v>16</v>
+      </c>
+      <c r="B3919">
+        <v>129</v>
+      </c>
+      <c r="C3919" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3919">
+        <v>45</v>
+      </c>
+      <c r="F3919" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3919" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3920" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3920">
+        <v>17</v>
+      </c>
+      <c r="B3920">
+        <v>131</v>
+      </c>
+      <c r="C3920" t="s">
+        <v>438</v>
+      </c>
+      <c r="D3920">
+        <v>45</v>
+      </c>
+      <c r="F3920" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3920" s="4">
+        <v>167.86</v>
+      </c>
+    </row>
+    <row r="3921" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3921">
+        <v>18</v>
+      </c>
+      <c r="B3921">
+        <v>133</v>
+      </c>
+      <c r="C3921" t="s">
+        <v>439</v>
+      </c>
+      <c r="D3921">
+        <v>45</v>
+      </c>
+      <c r="F3921" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3921" s="4">
+        <v>194.64</v>
+      </c>
+    </row>
+    <row r="3922" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3922">
+        <v>19</v>
+      </c>
+      <c r="B3922">
+        <v>136</v>
+      </c>
+      <c r="C3922" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3922">
+        <v>45</v>
+      </c>
+      <c r="F3922" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3922" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3923" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3923">
+        <v>20</v>
+      </c>
+      <c r="B3923">
+        <v>141</v>
+      </c>
+      <c r="C3923" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3923">
+        <v>45</v>
+      </c>
+      <c r="F3923" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3923" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3924" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3924">
+        <v>21</v>
+      </c>
+      <c r="B3924">
+        <v>145</v>
+      </c>
+      <c r="C3924" t="s">
+        <v>440</v>
+      </c>
+      <c r="D3924">
+        <v>45</v>
+      </c>
+      <c r="F3924" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3924" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3925" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3925">
+        <v>22</v>
+      </c>
+      <c r="B3925">
+        <v>147</v>
+      </c>
+      <c r="C3925" t="s">
+        <v>441</v>
+      </c>
+      <c r="D3925">
+        <v>45</v>
+      </c>
+      <c r="F3925" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3925" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3926" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3926">
+        <v>23</v>
+      </c>
+      <c r="B3926">
+        <v>149</v>
+      </c>
+      <c r="C3926" t="s">
+        <v>442</v>
+      </c>
+      <c r="D3926">
+        <v>45</v>
+      </c>
+      <c r="F3926" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3926" s="4">
+        <v>142.86000000000001</v>
+      </c>
+    </row>
+    <row r="3927" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3927">
+        <v>24</v>
+      </c>
+      <c r="B3927">
+        <v>150</v>
+      </c>
+      <c r="C3927" t="s">
+        <v>443</v>
+      </c>
+      <c r="D3927">
+        <v>45</v>
+      </c>
+      <c r="F3927" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3927" s="4">
+        <v>227.67000000000002</v>
+      </c>
+    </row>
+    <row r="3928" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3928">
+        <v>25</v>
+      </c>
+      <c r="B3928">
+        <v>151</v>
+      </c>
+      <c r="C3928" t="s">
+        <v>444</v>
+      </c>
+      <c r="D3928">
+        <v>45</v>
+      </c>
+      <c r="F3928" s="1">
+        <v>2</v>
+      </c>
+      <c r="G3928" s="4">
+        <v>137.5</v>
+      </c>
+    </row>
+    <row r="3929" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3929">
+        <v>26</v>
+      </c>
+      <c r="B3929">
+        <v>154</v>
+      </c>
+      <c r="C3929" t="s">
+        <v>445</v>
+      </c>
+      <c r="D3929">
+        <v>45</v>
+      </c>
+      <c r="F3929" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3929" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3930" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3930">
+        <v>27</v>
+      </c>
+      <c r="B3930">
+        <v>160</v>
+      </c>
+      <c r="C3930" t="s">
+        <v>446</v>
+      </c>
+      <c r="D3930">
+        <v>45</v>
+      </c>
+      <c r="F3930" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3930" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3931" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3931">
+        <v>28</v>
+      </c>
+      <c r="B3931">
+        <v>162</v>
+      </c>
+      <c r="C3931" t="s">
+        <v>447</v>
+      </c>
+      <c r="D3931">
+        <v>45</v>
+      </c>
+      <c r="F3931" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3931" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3932" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3932">
+        <v>29</v>
+      </c>
+      <c r="B3932">
+        <v>164</v>
+      </c>
+      <c r="C3932" t="s">
+        <v>448</v>
+      </c>
+      <c r="D3932">
+        <v>45</v>
+      </c>
+      <c r="F3932" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3932" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3933" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3933">
+        <v>30</v>
+      </c>
+      <c r="B3933">
+        <v>165</v>
+      </c>
+      <c r="C3933" t="s">
+        <v>449</v>
+      </c>
+      <c r="D3933">
+        <v>45</v>
+      </c>
+      <c r="F3933" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3933" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3934" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3934">
+        <v>31</v>
+      </c>
+      <c r="B3934">
+        <v>167</v>
+      </c>
+      <c r="C3934" t="s">
+        <v>450</v>
+      </c>
+      <c r="D3934">
+        <v>45</v>
+      </c>
+      <c r="F3934" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3934" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3935" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3935">
+        <v>32</v>
+      </c>
+      <c r="B3935">
+        <v>175</v>
+      </c>
+      <c r="C3935" t="s">
+        <v>195</v>
+      </c>
+      <c r="D3935">
+        <v>45</v>
+      </c>
+      <c r="F3935" s="1">
+        <v>5</v>
+      </c>
+      <c r="G3935" s="4">
+        <v>370.55</v>
+      </c>
+    </row>
+    <row r="3936" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3936">
+        <v>33</v>
+      </c>
+      <c r="B3936">
+        <v>181</v>
+      </c>
+      <c r="C3936" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3936">
+        <v>45</v>
+      </c>
+      <c r="F3936" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3936" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3937" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3937">
+        <v>34</v>
+      </c>
+      <c r="B3937">
+        <v>186</v>
+      </c>
+      <c r="C3937" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3937">
+        <v>45</v>
+      </c>
+      <c r="F3937" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3937" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3938" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3938">
+        <v>35</v>
+      </c>
+      <c r="B3938">
+        <v>192</v>
+      </c>
+      <c r="C3938" t="s">
+        <v>425</v>
+      </c>
+      <c r="D3938">
+        <v>45</v>
+      </c>
+      <c r="F3938" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="G3938" s="4">
+        <v>562.5</v>
+      </c>
+    </row>
+    <row r="3939" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3939">
+        <v>36</v>
+      </c>
+      <c r="B3939">
+        <v>194</v>
+      </c>
+      <c r="C3939" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3939">
+        <v>45</v>
+      </c>
+      <c r="F3939" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3939" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3940" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3940">
+        <v>37</v>
+      </c>
+      <c r="B3940">
+        <v>200</v>
+      </c>
+      <c r="C3940" t="s">
+        <v>451</v>
+      </c>
+      <c r="D3940">
+        <v>45</v>
+      </c>
+      <c r="F3940" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3940" s="4">
+        <v>233.04000000000002</v>
+      </c>
+    </row>
+    <row r="3941" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3941">
+        <v>38</v>
+      </c>
+      <c r="B3941">
+        <v>203</v>
+      </c>
+      <c r="C3941" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3941">
+        <v>45</v>
+      </c>
+      <c r="F3941" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3941" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3942" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3942">
+        <v>39</v>
+      </c>
+      <c r="B3942">
+        <v>205</v>
+      </c>
+      <c r="C3942" t="s">
+        <v>452</v>
+      </c>
+      <c r="D3942">
+        <v>45</v>
+      </c>
+      <c r="F3942" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3942" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3943" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3943">
+        <v>40</v>
+      </c>
+      <c r="B3943">
+        <v>209</v>
+      </c>
+      <c r="C3943" t="s">
+        <v>238</v>
+      </c>
+      <c r="D3943">
+        <v>45</v>
+      </c>
+      <c r="F3943" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3943" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3944" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3944">
+        <v>41</v>
+      </c>
+      <c r="B3944">
+        <v>212</v>
+      </c>
+      <c r="C3944" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3944">
+        <v>45</v>
+      </c>
+      <c r="F3944" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3944" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3945" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3945">
+        <v>42</v>
+      </c>
+      <c r="B3945">
+        <v>214</v>
+      </c>
+      <c r="C3945" t="s">
+        <v>247</v>
+      </c>
+      <c r="D3945">
+        <v>45</v>
+      </c>
+      <c r="F3945" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3945" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3946" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3946">
+        <v>43</v>
+      </c>
+      <c r="B3946">
+        <v>217</v>
+      </c>
+      <c r="C3946" t="s">
+        <v>453</v>
+      </c>
+      <c r="D3946">
+        <v>45</v>
+      </c>
+      <c r="F3946" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3946" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3947" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3947">
+        <v>44</v>
+      </c>
+      <c r="B3947">
+        <v>222</v>
+      </c>
+      <c r="C3947" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3947">
+        <v>45</v>
+      </c>
+      <c r="F3947" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3947" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3948" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3948">
+        <v>45</v>
+      </c>
+      <c r="B3948">
+        <v>223</v>
+      </c>
+      <c r="C3948" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3948">
+        <v>45</v>
+      </c>
+      <c r="F3948" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="G3948" s="4">
+        <v>660.28000000000009</v>
+      </c>
+    </row>
+    <row r="3949" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3949">
+        <v>46</v>
+      </c>
+      <c r="B3949">
+        <v>228</v>
+      </c>
+      <c r="C3949" t="s">
+        <v>455</v>
+      </c>
+      <c r="D3949">
+        <v>45</v>
+      </c>
+      <c r="F3949" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3949" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3950" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3950">
+        <v>47</v>
+      </c>
+      <c r="B3950">
+        <v>234</v>
+      </c>
+      <c r="C3950" t="s">
+        <v>277</v>
+      </c>
+      <c r="D3950">
+        <v>45</v>
+      </c>
+      <c r="F3950" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3950" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3951" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3951">
+        <v>48</v>
+      </c>
+      <c r="B3951">
+        <v>237</v>
+      </c>
+      <c r="C3951" t="s">
+        <v>456</v>
+      </c>
+      <c r="D3951">
+        <v>45</v>
+      </c>
+      <c r="F3951" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3951" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3952" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3952">
+        <v>49</v>
+      </c>
+      <c r="B3952">
+        <v>241</v>
+      </c>
+      <c r="C3952" t="s">
+        <v>457</v>
+      </c>
+      <c r="D3952">
+        <v>45</v>
+      </c>
+      <c r="F3952" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3952" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3953" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3953">
+        <v>50</v>
+      </c>
+      <c r="B3953">
+        <v>251</v>
+      </c>
+      <c r="C3953" t="s">
+        <v>458</v>
+      </c>
+      <c r="D3953">
+        <v>45</v>
+      </c>
+      <c r="F3953" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="G3953" s="4">
+        <v>103.125</v>
+      </c>
+    </row>
+    <row r="3954" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3954">
+        <v>51</v>
+      </c>
+      <c r="B3954">
+        <v>255</v>
+      </c>
+      <c r="C3954" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3954">
+        <v>45</v>
+      </c>
+      <c r="F3954" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3954" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3955" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3955">
+        <v>52</v>
+      </c>
+      <c r="B3955">
+        <v>260</v>
+      </c>
+      <c r="C3955" t="s">
+        <v>460</v>
+      </c>
+      <c r="D3955">
+        <v>45</v>
+      </c>
+      <c r="F3955" s="1">
+        <v>4</v>
+      </c>
+      <c r="G3955" s="4">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3956" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3956">
+        <v>53</v>
+      </c>
+      <c r="B3956">
+        <v>261</v>
+      </c>
+      <c r="C3956" t="s">
+        <v>461</v>
+      </c>
+      <c r="D3956">
+        <v>45</v>
+      </c>
+      <c r="F3956" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3956" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3957" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3957">
+        <v>54</v>
+      </c>
+      <c r="B3957">
+        <v>263</v>
+      </c>
+      <c r="C3957" t="s">
+        <v>462</v>
+      </c>
+      <c r="D3957">
+        <v>45</v>
+      </c>
+      <c r="F3957" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3957" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3958" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3958">
+        <v>55</v>
+      </c>
+      <c r="B3958">
+        <v>264</v>
+      </c>
+      <c r="C3958" t="s">
+        <v>360</v>
+      </c>
+      <c r="D3958">
+        <v>45</v>
+      </c>
+      <c r="F3958" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3958" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3959" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3959">
+        <v>56</v>
+      </c>
+      <c r="B3959">
+        <v>265</v>
+      </c>
+      <c r="C3959" t="s">
+        <v>463</v>
+      </c>
+      <c r="D3959">
+        <v>45</v>
+      </c>
+      <c r="F3959" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3959" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3960" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3960">
+        <v>57</v>
+      </c>
+      <c r="B3960">
+        <v>269</v>
+      </c>
+      <c r="C3960" t="s">
+        <v>374</v>
+      </c>
+      <c r="D3960">
+        <v>45</v>
+      </c>
+      <c r="F3960" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3960" s="4">
+        <v>206.25</v>
+      </c>
+    </row>
+    <row r="3961" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3961">
+        <v>58</v>
+      </c>
+      <c r="B3961">
+        <v>273</v>
+      </c>
+      <c r="C3961" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3961">
+        <v>45</v>
+      </c>
+      <c r="F3961" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3961" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3962" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3962">
+        <v>59</v>
+      </c>
+      <c r="B3962">
+        <v>274</v>
+      </c>
+      <c r="C3962" t="s">
+        <v>383</v>
+      </c>
+      <c r="D3962">
+        <v>45</v>
+      </c>
+      <c r="F3962" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3962" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3963" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3963">
+        <v>60</v>
+      </c>
+      <c r="B3963">
+        <v>275</v>
+      </c>
+      <c r="C3963" t="s">
+        <v>385</v>
+      </c>
+      <c r="D3963">
+        <v>45</v>
+      </c>
+      <c r="F3963" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3963" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3964" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3964">
+        <v>61</v>
+      </c>
+      <c r="B3964">
+        <v>277</v>
+      </c>
+      <c r="C3964" t="s">
+        <v>387</v>
+      </c>
+      <c r="D3964">
+        <v>45</v>
+      </c>
+      <c r="F3964" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3964" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3965" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3965">
+        <v>62</v>
+      </c>
+      <c r="B3965">
+        <v>278</v>
+      </c>
+      <c r="C3965" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3965">
+        <v>45</v>
+      </c>
+      <c r="F3965" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3965" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3966" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3966">
+        <v>63</v>
+      </c>
+      <c r="B3966">
+        <v>279</v>
+      </c>
+      <c r="C3966" t="s">
+        <v>389</v>
+      </c>
+      <c r="D3966">
+        <v>45</v>
+      </c>
+      <c r="F3966" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="G3966" s="4">
+        <v>653.125</v>
+      </c>
+    </row>
+    <row r="3967" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3967">
+        <v>64</v>
+      </c>
+      <c r="B3967">
+        <v>281</v>
+      </c>
+      <c r="C3967" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3967">
+        <v>45</v>
+      </c>
+      <c r="F3967" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3967" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3968" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3968">
+        <v>65</v>
+      </c>
+      <c r="B3968">
+        <v>282</v>
+      </c>
+      <c r="C3968" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3968">
+        <v>45</v>
+      </c>
+      <c r="F3968" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3968" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3969" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3969">
+        <v>66</v>
+      </c>
+      <c r="B3969">
+        <v>283</v>
+      </c>
+      <c r="C3969" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3969">
+        <v>45</v>
+      </c>
+      <c r="F3969" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3969" s="4">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="3970" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3970">
+        <v>67</v>
+      </c>
+      <c r="B3970">
+        <v>284</v>
+      </c>
+      <c r="C3970" t="s">
+        <v>465</v>
+      </c>
+      <c r="D3970">
+        <v>45</v>
+      </c>
+      <c r="F3970" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3970" s="4">
+        <v>687.5</v>
+      </c>
+    </row>
+    <row r="3971" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3971">
+        <v>68</v>
+      </c>
+      <c r="B3971">
+        <v>286</v>
+      </c>
+      <c r="C3971" t="s">
+        <v>420</v>
+      </c>
+      <c r="D3971">
+        <v>45</v>
+      </c>
+      <c r="F3971" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3971" s="4">
+        <v>206.25</v>
+      </c>
+    </row>
+    <row r="3972" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3972">
+        <v>69</v>
+      </c>
+      <c r="B3972">
+        <v>288</v>
+      </c>
+      <c r="C3972" t="s">
+        <v>466</v>
+      </c>
+      <c r="D3972">
+        <v>45</v>
+      </c>
+      <c r="F3972" s="1">
+        <v>3</v>
+      </c>
+      <c r="G3972" s="4">
+        <v>206.25</v>
+      </c>
+    </row>
+    <row r="3973" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3973">
+        <v>70</v>
+      </c>
+      <c r="B3973">
+        <v>289</v>
+      </c>
+      <c r="C3973" t="s">
+        <v>423</v>
+      </c>
+      <c r="D3973">
+        <v>45</v>
+      </c>
+      <c r="F3973" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G3973" s="4">
+        <v>171.875</v>
+      </c>
+    </row>
+    <row r="3974" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3974">
+        <v>71</v>
+      </c>
+      <c r="B3974">
+        <v>291</v>
+      </c>
+      <c r="C3974" t="s">
+        <v>424</v>
+      </c>
+      <c r="D3974">
+        <v>45</v>
+      </c>
+      <c r="F3974" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3974" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3975" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3975">
+        <v>72</v>
+      </c>
+      <c r="B3975">
+        <v>293</v>
+      </c>
+      <c r="C3975" t="s">
+        <v>426</v>
+      </c>
+      <c r="D3975">
+        <v>45</v>
+      </c>
+      <c r="F3975" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3975" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3976" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3976">
+        <v>73</v>
+      </c>
+      <c r="B3976">
+        <v>294</v>
+      </c>
+      <c r="C3976" t="s">
+        <v>467</v>
+      </c>
+      <c r="D3976">
+        <v>45</v>
+      </c>
+      <c r="F3976" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3976" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3977" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3977">
+        <v>74</v>
+      </c>
+      <c r="B3977">
+        <v>295</v>
+      </c>
+      <c r="C3977" t="s">
+        <v>468</v>
+      </c>
+      <c r="D3977">
+        <v>45</v>
+      </c>
+      <c r="F3977" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3977" s="4">
+        <v>68.75</v>
+      </c>
+    </row>
+    <row r="3978" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3978">
+        <v>75</v>
+      </c>
+      <c r="B3978">
+        <v>296</v>
+      </c>
+      <c r="C3978" t="s">
+        <v>469</v>
+      </c>
+      <c r="D3978">
+        <v>45</v>
+      </c>
+      <c r="F3978" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3978" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3979" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3979">
+        <v>76</v>
+      </c>
+      <c r="B3979">
+        <v>301</v>
+      </c>
+      <c r="C3979" t="s">
+        <v>362</v>
+      </c>
+      <c r="D3979">
+        <v>45</v>
+      </c>
+      <c r="F3979" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3979" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3980" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3980">
+        <v>77</v>
+      </c>
+      <c r="B3980">
+        <v>302</v>
+      </c>
+      <c r="C3980" t="s">
+        <v>363</v>
+      </c>
+      <c r="D3980">
+        <v>45</v>
+      </c>
+      <c r="F3980" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="G3980" s="4">
+        <v>515.625</v>
+      </c>
+    </row>
+    <row r="3981" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3981">
+        <v>1</v>
+      </c>
+      <c r="B3981">
+        <v>101</v>
+      </c>
+      <c r="C3981" t="s">
+        <v>427</v>
+      </c>
+      <c r="D3981">
+        <v>46</v>
+      </c>
+      <c r="F3981" s="1">
+        <v>16</v>
+      </c>
+      <c r="G3981" s="4">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="3982" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3982">
+        <v>2</v>
+      </c>
+      <c r="B3982">
+        <v>103</v>
+      </c>
+      <c r="C3982" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3982">
+        <v>46</v>
+      </c>
+      <c r="F3982" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3982" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3983" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3983">
+        <v>3</v>
+      </c>
+      <c r="B3983">
+        <v>104</v>
+      </c>
+      <c r="C3983" t="s">
+        <v>429</v>
+      </c>
+      <c r="D3983">
+        <v>46</v>
+      </c>
+      <c r="F3983" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G3983" s="4">
+        <v>712.03000000000009</v>
+      </c>
+    </row>
+    <row r="3984" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3984">
+        <v>4</v>
+      </c>
+      <c r="B3984">
+        <v>106</v>
+      </c>
+      <c r="C3984" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3984">
+        <v>46</v>
+      </c>
+      <c r="F3984" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3984" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3985" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3985">
+        <v>5</v>
+      </c>
+      <c r="B3985">
+        <v>107</v>
+      </c>
+      <c r="C3985" t="s">
+        <v>430</v>
+      </c>
+      <c r="D3985">
+        <v>46</v>
+      </c>
+      <c r="F3985" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3985" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3986" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3986">
+        <v>6</v>
+      </c>
+      <c r="B3986">
+        <v>108</v>
+      </c>
+      <c r="C3986" t="s">
+        <v>431</v>
+      </c>
+      <c r="D3986">
+        <v>46</v>
+      </c>
+      <c r="F3986" s="1">
+        <v>12</v>
+      </c>
+      <c r="G3986" s="4">
+        <v>1285.68</v>
+      </c>
+    </row>
+    <row r="3987" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3987">
+        <v>7</v>
+      </c>
+      <c r="B3987">
+        <v>109</v>
+      </c>
+      <c r="C3987" t="s">
+        <v>432</v>
+      </c>
+      <c r="D3987">
+        <v>46</v>
+      </c>
+      <c r="F3987" s="1">
+        <v>9</v>
+      </c>
+      <c r="G3987" s="4">
+        <v>964.26</v>
+      </c>
+    </row>
+    <row r="3988" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3988">
+        <v>8</v>
+      </c>
+      <c r="B3988">
+        <v>110</v>
+      </c>
+      <c r="C3988" t="s">
+        <v>433</v>
+      </c>
+      <c r="D3988">
+        <v>46</v>
+      </c>
+      <c r="F3988" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3988" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3989" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3989">
+        <v>9</v>
+      </c>
+      <c r="B3989">
+        <v>111</v>
+      </c>
+      <c r="C3989" t="s">
+        <v>434</v>
+      </c>
+      <c r="D3989">
+        <v>46</v>
+      </c>
+      <c r="F3989" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3989" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3990" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3990">
+        <v>10</v>
+      </c>
+      <c r="B3990">
+        <v>113</v>
+      </c>
+      <c r="C3990" t="s">
+        <v>435</v>
+      </c>
+      <c r="D3990">
+        <v>46</v>
+      </c>
+      <c r="F3990" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="G3990" s="4">
+        <v>623.64499999999998</v>
+      </c>
+    </row>
+    <row r="3991" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3991">
+        <v>11</v>
+      </c>
+      <c r="B3991">
+        <v>114</v>
+      </c>
+      <c r="C3991" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3991">
+        <v>46</v>
+      </c>
+      <c r="F3991" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3991" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3992" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3992">
+        <v>12</v>
+      </c>
+      <c r="B3992">
+        <v>117</v>
+      </c>
+      <c r="C3992" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3992">
+        <v>46</v>
+      </c>
+      <c r="F3992" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="G3992" s="4">
+        <v>212.04999999999998</v>
+      </c>
+    </row>
+    <row r="3993" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3993">
+        <v>13</v>
+      </c>
+      <c r="B3993">
+        <v>119</v>
+      </c>
+      <c r="C3993" t="s">
+        <v>436</v>
+      </c>
+      <c r="D3993">
+        <v>46</v>
+      </c>
+      <c r="F3993" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3993" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3994" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3994">
+        <v>14</v>
+      </c>
+      <c r="B3994">
+        <v>125</v>
+      </c>
+      <c r="C3994" t="s">
+        <v>437</v>
+      </c>
+      <c r="D3994">
+        <v>46</v>
+      </c>
+      <c r="F3994" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3994" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3995" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3995">
+        <v>15</v>
+      </c>
+      <c r="B3995">
+        <v>126</v>
+      </c>
+      <c r="C3995" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3995">
+        <v>46</v>
+      </c>
+      <c r="F3995" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3995" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3996" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3996">
+        <v>16</v>
+      </c>
+      <c r="B3996">
+        <v>129</v>
+      </c>
+      <c r="C3996" t="s">
+        <v>132</v>
+      </c>
+      <c r="D3996">
+        <v>46</v>
+      </c>
+      <c r="F3996" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3996" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3997" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3997">
+        <v>17</v>
+      </c>
+      <c r="B3997">
+        <v>131</v>
+      </c>
+      <c r="C3997" t="s">
+        <v>438</v>
+      </c>
+      <c r="D3997">
+        <v>46</v>
+      </c>
+      <c r="F3997" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3997" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3998" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3998">
+        <v>18</v>
+      </c>
+      <c r="B3998">
+        <v>133</v>
+      </c>
+      <c r="C3998" t="s">
+        <v>439</v>
+      </c>
+      <c r="D3998">
+        <v>46</v>
+      </c>
+      <c r="F3998" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3998" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3999" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3999">
+        <v>19</v>
+      </c>
+      <c r="B3999">
+        <v>136</v>
+      </c>
+      <c r="C3999" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3999">
+        <v>46</v>
+      </c>
+      <c r="F3999" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3999" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4000" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4000">
+        <v>20</v>
+      </c>
+      <c r="B4000">
+        <v>141</v>
+      </c>
+      <c r="C4000" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4000">
+        <v>46</v>
+      </c>
+      <c r="F4000" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4000" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4001" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4001">
+        <v>21</v>
+      </c>
+      <c r="B4001">
+        <v>145</v>
+      </c>
+      <c r="C4001" t="s">
+        <v>440</v>
+      </c>
+      <c r="D4001">
+        <v>46</v>
+      </c>
+      <c r="F4001" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4001" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4002" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4002">
+        <v>22</v>
+      </c>
+      <c r="B4002">
+        <v>147</v>
+      </c>
+      <c r="C4002" t="s">
+        <v>441</v>
+      </c>
+      <c r="D4002">
+        <v>46</v>
+      </c>
+      <c r="F4002" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4002" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4003" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4003">
+        <v>23</v>
+      </c>
+      <c r="B4003">
+        <v>149</v>
+      </c>
+      <c r="C4003" t="s">
+        <v>442</v>
+      </c>
+      <c r="D4003">
+        <v>46</v>
+      </c>
+      <c r="F4003" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4003" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4004" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4004">
+        <v>24</v>
+      </c>
+      <c r="B4004">
+        <v>150</v>
+      </c>
+      <c r="C4004" t="s">
+        <v>443</v>
+      </c>
+      <c r="D4004">
+        <v>46</v>
+      </c>
+      <c r="F4004" s="1">
+        <v>7</v>
+      </c>
+      <c r="G4004" s="4">
+        <v>531.23</v>
+      </c>
+    </row>
+    <row r="4005" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4005">
+        <v>25</v>
+      </c>
+      <c r="B4005">
+        <v>151</v>
+      </c>
+      <c r="C4005" t="s">
+        <v>444</v>
+      </c>
+      <c r="D4005">
+        <v>46</v>
+      </c>
+      <c r="F4005" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4005" s="4">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4006" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4006">
+        <v>26</v>
+      </c>
+      <c r="B4006">
+        <v>154</v>
+      </c>
+      <c r="C4006" t="s">
+        <v>445</v>
+      </c>
+      <c r="D4006">
+        <v>46</v>
+      </c>
+      <c r="F4006" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4006" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4007" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4007">
+        <v>27</v>
+      </c>
+      <c r="B4007">
+        <v>160</v>
+      </c>
+      <c r="C4007" t="s">
+        <v>446</v>
+      </c>
+      <c r="D4007">
+        <v>46</v>
+      </c>
+      <c r="F4007" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4007" s="4">
+        <v>75.89</v>
+      </c>
+    </row>
+    <row r="4008" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4008">
+        <v>28</v>
+      </c>
+      <c r="B4008">
+        <v>162</v>
+      </c>
+      <c r="C4008" t="s">
+        <v>447</v>
+      </c>
+      <c r="D4008">
+        <v>46</v>
+      </c>
+      <c r="F4008" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4008" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4009" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4009">
+        <v>29</v>
+      </c>
+      <c r="B4009">
+        <v>164</v>
+      </c>
+      <c r="C4009" t="s">
+        <v>448</v>
+      </c>
+      <c r="D4009">
+        <v>46</v>
+      </c>
+      <c r="F4009" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4009" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4010" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4010">
+        <v>30</v>
+      </c>
+      <c r="B4010">
+        <v>165</v>
+      </c>
+      <c r="C4010" t="s">
+        <v>449</v>
+      </c>
+      <c r="D4010">
+        <v>46</v>
+      </c>
+      <c r="F4010" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4010" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4011" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4011">
+        <v>31</v>
+      </c>
+      <c r="B4011">
+        <v>167</v>
+      </c>
+      <c r="C4011" t="s">
+        <v>450</v>
+      </c>
+      <c r="D4011">
+        <v>46</v>
+      </c>
+      <c r="F4011" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4011" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4012" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4012">
+        <v>32</v>
+      </c>
+      <c r="B4012">
+        <v>175</v>
+      </c>
+      <c r="C4012" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4012">
+        <v>46</v>
+      </c>
+      <c r="F4012" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4012" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4013" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4013">
+        <v>33</v>
+      </c>
+      <c r="B4013">
+        <v>181</v>
+      </c>
+      <c r="C4013" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4013">
+        <v>46</v>
+      </c>
+      <c r="F4013" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4013" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4014" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4014">
+        <v>34</v>
+      </c>
+      <c r="B4014">
+        <v>186</v>
+      </c>
+      <c r="C4014" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4014">
+        <v>46</v>
+      </c>
+      <c r="F4014" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4014" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4015" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4015">
+        <v>35</v>
+      </c>
+      <c r="B4015">
+        <v>192</v>
+      </c>
+      <c r="C4015" t="s">
+        <v>425</v>
+      </c>
+      <c r="D4015">
+        <v>46</v>
+      </c>
+      <c r="F4015" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="G4015" s="4">
+        <v>862.5</v>
+      </c>
+    </row>
+    <row r="4016" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4016">
+        <v>36</v>
+      </c>
+      <c r="B4016">
+        <v>194</v>
+      </c>
+      <c r="C4016" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4016">
+        <v>46</v>
+      </c>
+      <c r="F4016" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4016" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4017" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4017">
+        <v>37</v>
+      </c>
+      <c r="B4017">
+        <v>200</v>
+      </c>
+      <c r="C4017" t="s">
+        <v>451</v>
+      </c>
+      <c r="D4017">
+        <v>46</v>
+      </c>
+      <c r="F4017" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4017" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4018" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4018">
+        <v>38</v>
+      </c>
+      <c r="B4018">
+        <v>203</v>
+      </c>
+      <c r="C4018" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4018">
+        <v>46</v>
+      </c>
+      <c r="F4018" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4018" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4019" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4019">
+        <v>39</v>
+      </c>
+      <c r="B4019">
+        <v>205</v>
+      </c>
+      <c r="C4019" t="s">
+        <v>452</v>
+      </c>
+      <c r="D4019">
+        <v>46</v>
+      </c>
+      <c r="F4019" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4019" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4020" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4020">
+        <v>40</v>
+      </c>
+      <c r="B4020">
+        <v>209</v>
+      </c>
+      <c r="C4020" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4020">
+        <v>46</v>
+      </c>
+      <c r="F4020" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4020" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4021" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4021">
+        <v>41</v>
+      </c>
+      <c r="B4021">
+        <v>212</v>
+      </c>
+      <c r="C4021" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4021">
+        <v>46</v>
+      </c>
+      <c r="F4021" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4021" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4022" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4022">
+        <v>42</v>
+      </c>
+      <c r="B4022">
+        <v>214</v>
+      </c>
+      <c r="C4022" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4022">
+        <v>46</v>
+      </c>
+      <c r="F4022" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4022" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4023" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4023">
+        <v>43</v>
+      </c>
+      <c r="B4023">
+        <v>217</v>
+      </c>
+      <c r="C4023" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4023">
+        <v>46</v>
+      </c>
+      <c r="F4023" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4023" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4024" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4024">
+        <v>44</v>
+      </c>
+      <c r="B4024">
+        <v>222</v>
+      </c>
+      <c r="C4024" t="s">
+        <v>260</v>
+      </c>
+      <c r="D4024">
+        <v>46</v>
+      </c>
+      <c r="F4024" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4024" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4025" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4025">
+        <v>45</v>
+      </c>
+      <c r="B4025">
+        <v>223</v>
+      </c>
+      <c r="C4025" t="s">
+        <v>454</v>
+      </c>
+      <c r="D4025">
+        <v>46</v>
+      </c>
+      <c r="F4025" s="1">
+        <v>10</v>
+      </c>
+      <c r="G4025" s="4">
+        <v>776.80000000000007</v>
+      </c>
+    </row>
+    <row r="4026" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4026">
+        <v>46</v>
+      </c>
+      <c r="B4026">
+        <v>228</v>
+      </c>
+      <c r="C4026" t="s">
+        <v>455</v>
+      </c>
+      <c r="D4026">
+        <v>46</v>
+      </c>
+      <c r="F4026" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4026" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4027" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4027">
+        <v>47</v>
+      </c>
+      <c r="B4027">
+        <v>234</v>
+      </c>
+      <c r="C4027" t="s">
+        <v>277</v>
+      </c>
+      <c r="D4027">
+        <v>46</v>
+      </c>
+      <c r="F4027" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4027" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4028" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4028">
+        <v>48</v>
+      </c>
+      <c r="B4028">
+        <v>237</v>
+      </c>
+      <c r="C4028" t="s">
+        <v>456</v>
+      </c>
+      <c r="D4028">
+        <v>46</v>
+      </c>
+      <c r="F4028" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4028" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4029" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4029">
+        <v>49</v>
+      </c>
+      <c r="B4029">
+        <v>241</v>
+      </c>
+      <c r="C4029" t="s">
+        <v>457</v>
+      </c>
+      <c r="D4029">
+        <v>46</v>
+      </c>
+      <c r="F4029" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4029" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4030" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4030">
+        <v>50</v>
+      </c>
+      <c r="B4030">
+        <v>251</v>
+      </c>
+      <c r="C4030" t="s">
+        <v>458</v>
+      </c>
+      <c r="D4030">
+        <v>46</v>
+      </c>
+      <c r="F4030" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4030" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4031" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4031">
+        <v>51</v>
+      </c>
+      <c r="B4031">
+        <v>255</v>
+      </c>
+      <c r="C4031" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4031">
+        <v>46</v>
+      </c>
+      <c r="F4031" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4031" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4032" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4032">
+        <v>52</v>
+      </c>
+      <c r="B4032">
+        <v>260</v>
+      </c>
+      <c r="C4032" t="s">
+        <v>460</v>
+      </c>
+      <c r="D4032">
+        <v>46</v>
+      </c>
+      <c r="F4032" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4032" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4033" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4033">
+        <v>53</v>
+      </c>
+      <c r="B4033">
+        <v>261</v>
+      </c>
+      <c r="C4033" t="s">
+        <v>461</v>
+      </c>
+      <c r="D4033">
+        <v>46</v>
+      </c>
+      <c r="F4033" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4033" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4034" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4034">
+        <v>54</v>
+      </c>
+      <c r="B4034">
+        <v>263</v>
+      </c>
+      <c r="C4034" t="s">
+        <v>462</v>
+      </c>
+      <c r="D4034">
+        <v>46</v>
+      </c>
+      <c r="F4034" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4034" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4035" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4035">
+        <v>55</v>
+      </c>
+      <c r="B4035">
+        <v>264</v>
+      </c>
+      <c r="C4035" t="s">
+        <v>360</v>
+      </c>
+      <c r="D4035">
+        <v>46</v>
+      </c>
+      <c r="F4035" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4035" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4036" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4036">
+        <v>56</v>
+      </c>
+      <c r="B4036">
+        <v>265</v>
+      </c>
+      <c r="C4036" t="s">
+        <v>463</v>
+      </c>
+      <c r="D4036">
+        <v>46</v>
+      </c>
+      <c r="F4036" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4036" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4037" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4037">
+        <v>57</v>
+      </c>
+      <c r="B4037">
+        <v>269</v>
+      </c>
+      <c r="C4037" t="s">
+        <v>374</v>
+      </c>
+      <c r="D4037">
+        <v>46</v>
+      </c>
+      <c r="F4037" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4037" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4038" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4038">
+        <v>58</v>
+      </c>
+      <c r="B4038">
+        <v>273</v>
+      </c>
+      <c r="C4038" t="s">
+        <v>382</v>
+      </c>
+      <c r="D4038">
+        <v>46</v>
+      </c>
+      <c r="F4038" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4038" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4039" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4039">
+        <v>59</v>
+      </c>
+      <c r="B4039">
+        <v>274</v>
+      </c>
+      <c r="C4039" t="s">
+        <v>383</v>
+      </c>
+      <c r="D4039">
+        <v>46</v>
+      </c>
+      <c r="F4039" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4039" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4040" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4040">
+        <v>60</v>
+      </c>
+      <c r="B4040">
+        <v>275</v>
+      </c>
+      <c r="C4040" t="s">
+        <v>385</v>
+      </c>
+      <c r="D4040">
+        <v>46</v>
+      </c>
+      <c r="F4040" s="1">
+        <v>3</v>
+      </c>
+      <c r="G4040" s="4">
+        <v>206.25</v>
+      </c>
+    </row>
+    <row r="4041" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4041">
+        <v>61</v>
+      </c>
+      <c r="B4041">
+        <v>277</v>
+      </c>
+      <c r="C4041" t="s">
+        <v>387</v>
+      </c>
+      <c r="D4041">
+        <v>46</v>
+      </c>
+      <c r="F4041" s="1">
+        <v>11</v>
+      </c>
+      <c r="G4041" s="4">
+        <v>962.5</v>
+      </c>
+    </row>
+    <row r="4042" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4042">
+        <v>62</v>
+      </c>
+      <c r="B4042">
+        <v>278</v>
+      </c>
+      <c r="C4042" t="s">
+        <v>388</v>
+      </c>
+      <c r="D4042">
+        <v>46</v>
+      </c>
+      <c r="F4042" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4042" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4043" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4043">
+        <v>63</v>
+      </c>
+      <c r="B4043">
+        <v>279</v>
+      </c>
+      <c r="C4043" t="s">
+        <v>389</v>
+      </c>
+      <c r="D4043">
+        <v>46</v>
+      </c>
+      <c r="F4043" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4043" s="4">
+        <v>343.75</v>
+      </c>
+    </row>
+    <row r="4044" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4044">
+        <v>64</v>
+      </c>
+      <c r="B4044">
+        <v>281</v>
+      </c>
+      <c r="C4044" t="s">
+        <v>396</v>
+      </c>
+      <c r="D4044">
+        <v>46</v>
+      </c>
+      <c r="F4044" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4044" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4045" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4045">
+        <v>65</v>
+      </c>
+      <c r="B4045">
+        <v>282</v>
+      </c>
+      <c r="C4045" t="s">
+        <v>464</v>
+      </c>
+      <c r="D4045">
+        <v>46</v>
+      </c>
+      <c r="F4045" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4045" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4046" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4046">
+        <v>66</v>
+      </c>
+      <c r="B4046">
+        <v>283</v>
+      </c>
+      <c r="C4046" t="s">
+        <v>398</v>
+      </c>
+      <c r="D4046">
+        <v>46</v>
+      </c>
+      <c r="F4046" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4046" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4047" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4047">
+        <v>67</v>
+      </c>
+      <c r="B4047">
+        <v>284</v>
+      </c>
+      <c r="C4047" t="s">
+        <v>465</v>
+      </c>
+      <c r="D4047">
+        <v>46</v>
+      </c>
+      <c r="F4047" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="G4047" s="4">
+        <v>653.125</v>
+      </c>
+    </row>
+    <row r="4048" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4048">
+        <v>68</v>
+      </c>
+      <c r="B4048">
+        <v>286</v>
+      </c>
+      <c r="C4048" t="s">
+        <v>420</v>
+      </c>
+      <c r="D4048">
+        <v>46</v>
+      </c>
+      <c r="F4048" s="1">
+        <v>5</v>
+      </c>
+      <c r="G4048" s="4">
+        <v>343.75</v>
+      </c>
+    </row>
+    <row r="4049" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4049">
+        <v>69</v>
+      </c>
+      <c r="B4049">
+        <v>288</v>
+      </c>
+      <c r="C4049" t="s">
+        <v>466</v>
+      </c>
+      <c r="D4049">
+        <v>46</v>
+      </c>
+      <c r="F4049" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4049" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4050" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4050">
+        <v>70</v>
+      </c>
+      <c r="B4050">
+        <v>289</v>
+      </c>
+      <c r="C4050" t="s">
+        <v>423</v>
+      </c>
+      <c r="D4050">
+        <v>46</v>
+      </c>
+      <c r="F4050" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4050" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4051" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4051">
+        <v>71</v>
+      </c>
+      <c r="B4051">
+        <v>291</v>
+      </c>
+      <c r="C4051" t="s">
+        <v>424</v>
+      </c>
+      <c r="D4051">
+        <v>46</v>
+      </c>
+      <c r="F4051" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4051" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4052" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4052">
+        <v>72</v>
+      </c>
+      <c r="B4052">
+        <v>293</v>
+      </c>
+      <c r="C4052" t="s">
+        <v>426</v>
+      </c>
+      <c r="D4052">
+        <v>46</v>
+      </c>
+      <c r="F4052" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4052" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4053" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4053">
+        <v>73</v>
+      </c>
+      <c r="B4053">
+        <v>295</v>
+      </c>
+      <c r="C4053" t="s">
+        <v>468</v>
+      </c>
+      <c r="D4053">
+        <v>46</v>
+      </c>
+      <c r="F4053" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4053" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4054" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4054">
+        <v>74</v>
+      </c>
+      <c r="B4054">
+        <v>296</v>
+      </c>
+      <c r="C4054" t="s">
+        <v>469</v>
+      </c>
+      <c r="D4054">
+        <v>46</v>
+      </c>
+      <c r="F4054" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4054" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4055" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4055">
+        <v>75</v>
+      </c>
+      <c r="B4055">
+        <v>302</v>
+      </c>
+      <c r="C4055" t="s">
+        <v>363</v>
+      </c>
+      <c r="D4055">
+        <v>46</v>
+      </c>
+      <c r="F4055" s="1">
+        <v>8</v>
+      </c>
+      <c r="G4055" s="4">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="4056" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4056">
+        <v>76</v>
+      </c>
+      <c r="B4056">
+        <v>297</v>
+      </c>
+      <c r="C4056" t="s">
+        <v>470</v>
+      </c>
+      <c r="D4056">
+        <v>46</v>
+      </c>
+      <c r="F4056" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4056" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4057" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4057">
+        <v>77</v>
+      </c>
+      <c r="B4057">
+        <v>298</v>
+      </c>
+      <c r="C4057" t="s">
+        <v>471</v>
+      </c>
+      <c r="D4057">
+        <v>46</v>
+      </c>
+      <c r="F4057" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4057" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4058" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4058">
+        <v>78</v>
+      </c>
+      <c r="B4058">
+        <v>299</v>
+      </c>
+      <c r="C4058" t="s">
+        <v>472</v>
+      </c>
+      <c r="D4058">
+        <v>46</v>
+      </c>
+      <c r="F4058" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4058" s="4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>